<commit_message>
Updated metadata field extraction notes, added start of FGDC
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="0" windowWidth="34580" windowHeight="27080" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="0" windowWidth="34580" windowHeight="27080" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="EML" sheetId="3" r:id="rId3"/>
+    <sheet name="FGDC" sheetId="4" r:id="rId4"/>
+    <sheet name="Dryad" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="208">
   <si>
     <t>Notes</t>
   </si>
@@ -581,18 +583,6 @@
     <t>tmp_D1_Schema</t>
   </si>
   <si>
-    <t>FGDC_path</t>
-  </si>
-  <si>
-    <t>FGDC_ref</t>
-  </si>
-  <si>
-    <t>EML_path</t>
-  </si>
-  <si>
-    <t>EML_ref</t>
-  </si>
-  <si>
     <t>http://knb.ecoinformatics.org/software/eml/eml-2.1.0/eml-resource.html#abstract</t>
   </si>
   <si>
@@ -627,12 +617,6 @@
   </si>
   <si>
     <t>http://knb.ecoinformatics.org/software/eml/eml-2.1.0/eml-coverage.html#northBoundingCoordinate</t>
-  </si>
-  <si>
-    <t>http://knb.ecoinformatics.org/software/eml/eml-2.1.0/eml-coverage.html#southBoundingCoordinate</t>
-  </si>
-  <si>
-    <t>http://knb.ecoinformatics.org/software/eml/eml-2.1.0/eml-coverage.html#westBoundingCoordinate</t>
   </si>
   <si>
     <t>All descriptive text, concatenated</t>
@@ -782,7 +766,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -848,6 +832,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -857,7 +853,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="77">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -892,6 +888,12 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -920,6 +922,12 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="6" builtinId="20"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,25 +1259,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2:F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="6" max="7" width="28.6640625" customWidth="1"/>
-    <col min="8" max="11" width="42.33203125" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" customWidth="1"/>
+    <col min="6" max="7" width="42.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>183</v>
       </c>
@@ -1277,37 +1284,25 @@
         <v>184</v>
       </c>
       <c r="C1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
         <v>185</v>
       </c>
       <c r="E1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" t="s">
-        <v>189</v>
-      </c>
-      <c r="J1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K1" t="s">
-        <v>192</v>
-      </c>
-      <c r="L1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1320,17 +1315,8 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1341,7 +1327,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1354,14 +1340,8 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" t="s">
-        <v>198</v>
-      </c>
-      <c r="I4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1374,14 +1354,8 @@
       <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" t="s">
-        <v>197</v>
-      </c>
-      <c r="I5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1394,20 +1368,11 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
       <c r="H6" t="s">
-        <v>193</v>
-      </c>
-      <c r="I6" t="s">
-        <v>195</v>
-      </c>
-      <c r="L6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1421,7 +1386,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1429,7 +1394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1443,7 +1408,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1457,7 +1422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1465,18 +1430,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="F12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1484,18 +1446,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="L14" t="s">
+      <c r="H14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1508,11 +1470,11 @@
       <c r="D15" t="s">
         <v>179</v>
       </c>
-      <c r="L15" t="s">
+      <c r="H15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1526,18 +1488,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="L17" t="s">
+      <c r="H17" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1548,7 +1510,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1559,7 +1521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
@@ -1569,25 +1531,22 @@
       <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="L20" t="s">
+      <c r="H20" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="H21" t="s">
-        <v>154</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="F21" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1595,7 +1554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:8">
       <c r="A23" s="5" t="s">
         <v>32</v>
       </c>
@@ -1605,31 +1564,19 @@
       <c r="E23" t="s">
         <v>6</v>
       </c>
-      <c r="F23" t="s">
-        <v>34</v>
-      </c>
       <c r="H23" t="s">
-        <v>167</v>
-      </c>
-      <c r="I23" t="s">
-        <v>200</v>
-      </c>
-      <c r="L23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
       </c>
-      <c r="F24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -1640,7 +1587,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
@@ -1650,20 +1597,11 @@
       <c r="E26" t="s">
         <v>6</v>
       </c>
-      <c r="F26" t="s">
-        <v>39</v>
-      </c>
       <c r="H26" t="s">
-        <v>194</v>
-      </c>
-      <c r="I26" t="s">
-        <v>195</v>
-      </c>
-      <c r="L26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
@@ -1671,7 +1609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
@@ -1679,18 +1617,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>43</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="F29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="5" t="s">
         <v>44</v>
       </c>
@@ -1698,18 +1633,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
       </c>
-      <c r="F31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -1717,21 +1649,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>47</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
       </c>
-      <c r="F33" t="s">
-        <v>125</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="H33" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:8">
       <c r="A34" s="5" t="s">
         <v>48</v>
       </c>
@@ -1741,22 +1670,19 @@
       <c r="D34" t="s">
         <v>50</v>
       </c>
-      <c r="F34" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="L35" t="s">
+      <c r="H35" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -1764,7 +1690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:8">
       <c r="A37" s="5" t="s">
         <v>52</v>
       </c>
@@ -1772,16 +1698,10 @@
         <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>126</v>
-      </c>
-      <c r="H37" t="s">
-        <v>158</v>
-      </c>
-      <c r="J37" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -1789,18 +1709,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>54</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
       </c>
-      <c r="L39" t="s">
+      <c r="H39" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:8">
       <c r="A40" s="5" t="s">
         <v>55</v>
       </c>
@@ -1811,19 +1731,13 @@
         <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>56</v>
+        <v>161</v>
       </c>
       <c r="H40" t="s">
-        <v>162</v>
-      </c>
-      <c r="J40" t="s">
-        <v>161</v>
-      </c>
-      <c r="L40" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -1831,7 +1745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
         <v>58</v>
       </c>
@@ -1839,18 +1753,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
       </c>
-      <c r="L43" t="s">
+      <c r="H43" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
         <v>60</v>
       </c>
@@ -1858,7 +1772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
         <v>61</v>
       </c>
@@ -1866,7 +1780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -1874,29 +1788,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>63</v>
       </c>
       <c r="B47" t="s">
         <v>2</v>
       </c>
-      <c r="L47" t="s">
+      <c r="H47" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>64</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
-      <c r="L48" t="s">
+      <c r="H48" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:8">
       <c r="A49" s="5" t="s">
         <v>65</v>
       </c>
@@ -1906,20 +1820,11 @@
       <c r="E49" t="s">
         <v>6</v>
       </c>
-      <c r="F49" t="s">
-        <v>66</v>
-      </c>
       <c r="H49" t="s">
-        <v>166</v>
-      </c>
-      <c r="I49" t="s">
-        <v>201</v>
-      </c>
-      <c r="L49" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -1930,7 +1835,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -1941,7 +1846,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>70</v>
       </c>
@@ -1952,7 +1857,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>71</v>
       </c>
@@ -1963,18 +1868,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>72</v>
       </c>
       <c r="B54" t="s">
         <v>2</v>
       </c>
-      <c r="F54" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="2" t="s">
         <v>73</v>
       </c>
@@ -1982,7 +1884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -1990,27 +1892,18 @@
         <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H56" t="s">
-        <v>170</v>
-      </c>
-      <c r="J56" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>76</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
       </c>
-      <c r="F57" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -2018,7 +1911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -2026,18 +1919,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>79</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
       </c>
-      <c r="F60" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>80</v>
       </c>
@@ -2045,7 +1935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:8">
       <c r="A62" s="2" t="s">
         <v>81</v>
       </c>
@@ -2053,21 +1943,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>82</v>
       </c>
       <c r="B63" t="s">
         <v>2</v>
       </c>
-      <c r="F63" t="s">
-        <v>138</v>
-      </c>
-      <c r="L63" t="s">
+      <c r="H63" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>83</v>
       </c>
@@ -2078,7 +1965,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -2086,21 +1973,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>85</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
       </c>
-      <c r="F66" t="s">
-        <v>130</v>
-      </c>
-      <c r="H66" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -2108,32 +1989,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>87</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
-      <c r="F68" t="s">
-        <v>88</v>
-      </c>
-      <c r="H68" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>89</v>
       </c>
       <c r="B69" t="s">
         <v>2</v>
       </c>
-      <c r="F69" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -2144,7 +2016,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
         <v>91</v>
       </c>
@@ -2152,7 +2024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
         <v>92</v>
       </c>
@@ -2160,18 +2032,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>93</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
       </c>
-      <c r="F73" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>94</v>
       </c>
@@ -2179,18 +2048,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>95</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
       </c>
-      <c r="F75" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>96</v>
       </c>
@@ -2198,7 +2064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
         <v>97</v>
       </c>
@@ -2209,7 +2075,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>99</v>
       </c>
@@ -2217,18 +2083,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>101</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
       </c>
-      <c r="F79" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>102</v>
       </c>
@@ -2236,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:8">
       <c r="A81" s="5" t="s">
         <v>103</v>
       </c>
@@ -2246,20 +2109,11 @@
       <c r="E81" t="s">
         <v>6</v>
       </c>
-      <c r="F81" t="s">
-        <v>104</v>
-      </c>
       <c r="H81" t="s">
-        <v>168</v>
-      </c>
-      <c r="I81" t="s">
-        <v>202</v>
-      </c>
-      <c r="L81" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:8">
       <c r="A82" s="2" t="s">
         <v>106</v>
       </c>
@@ -2267,7 +2121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:8">
       <c r="A83" s="1" t="s">
         <v>107</v>
       </c>
@@ -2277,22 +2131,16 @@
       <c r="D83" t="s">
         <v>107</v>
       </c>
-      <c r="F83" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12">
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>108</v>
       </c>
       <c r="B84" t="s">
         <v>5</v>
       </c>
-      <c r="F84" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12">
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -2300,7 +2148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -2310,14 +2158,8 @@
       <c r="E86" t="s">
         <v>6</v>
       </c>
-      <c r="F86" t="s">
-        <v>204</v>
-      </c>
-      <c r="H86" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12">
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="5" t="s">
         <v>110</v>
       </c>
@@ -2328,19 +2170,10 @@
         <v>6</v>
       </c>
       <c r="F87" t="s">
-        <v>118</v>
-      </c>
-      <c r="H87" t="s">
-        <v>173</v>
-      </c>
-      <c r="I87" t="s">
-        <v>205</v>
-      </c>
-      <c r="J87" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>111</v>
       </c>
@@ -2348,7 +2181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>112</v>
       </c>
@@ -2356,18 +2189,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>113</v>
       </c>
       <c r="B90" t="s">
         <v>5</v>
       </c>
-      <c r="F90" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12">
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>114</v>
       </c>
@@ -2375,18 +2205,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>115</v>
       </c>
       <c r="B92" t="s">
         <v>10</v>
       </c>
-      <c r="L92" t="s">
+      <c r="H92" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>116</v>
       </c>
@@ -2394,16 +2224,10 @@
         <v>5</v>
       </c>
       <c r="F93" t="s">
-        <v>121</v>
-      </c>
-      <c r="H93" t="s">
-        <v>176</v>
-      </c>
-      <c r="J93" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:8">
       <c r="A94" s="5" t="s">
         <v>117</v>
       </c>
@@ -2413,20 +2237,11 @@
       <c r="E94" t="s">
         <v>6</v>
       </c>
-      <c r="F94" t="s">
-        <v>119</v>
-      </c>
       <c r="H94" t="s">
-        <v>169</v>
-      </c>
-      <c r="I94" t="s">
-        <v>203</v>
-      </c>
-      <c r="L94" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:8">
       <c r="A95" s="4" t="s">
         <v>144</v>
       </c>
@@ -2434,7 +2249,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:8">
       <c r="A96" s="4" t="s">
         <v>145</v>
       </c>
@@ -2545,7 +2360,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2555,10 +2372,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C1" t="s">
         <v>180</v>
@@ -3200,7 +3017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A107"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3212,16 +3031,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3229,10 +3048,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3245,10 +3064,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3256,10 +3075,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3267,10 +3086,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3364,7 +3183,7 @@
         <v>167</v>
       </c>
       <c r="C23" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3382,10 +3201,10 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C26" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3512,7 +3331,7 @@
         <v>166</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -3712,7 +3531,7 @@
         <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -3723,7 +3542,7 @@
         <v>173</v>
       </c>
       <c r="C87" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -3829,6 +3648,1261 @@
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D107"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="75.83203125" customWidth="1"/>
+    <col min="3" max="3" width="97.5" customWidth="1"/>
+    <col min="4" max="4" width="75.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>85</v>
+      </c>
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>107</v>
+      </c>
+      <c r="B83" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>108</v>
+      </c>
+      <c r="B84" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="97.6640625" customWidth="1"/>
+    <col min="3" max="3" width="97.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing a problem introduced with changes to the schema spreadsheet
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="51380" yWindow="-180" windowWidth="40020" windowHeight="20340" tabRatio="500"/>
+    <workbookView xWindow="51720" yWindow="1120" windowWidth="34520" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="271">
   <si>
     <t>Notes</t>
   </si>
@@ -573,9 +573,6 @@
     <t>//mets:METS/ mets:dmdSec/ mets:mdWrap/ mets:xmlData/ dim:dim/ dim:field[@element='title']/text()</t>
   </si>
   <si>
-    <t>Indexer.java</t>
-  </si>
-  <si>
     <t>//dataset/distribution/online/url/text()</t>
   </si>
   <si>
@@ -759,9 +756,6 @@
     <t>Time stamps for when D1 replicas were verified as complete</t>
   </si>
   <si>
-    <t>A multivalued field that indicates which resource maps this object appears in</t>
-  </si>
-  <si>
     <t>Multivalued field that lists the subjects that have read permission on the object</t>
   </si>
   <si>
@@ -789,9 +783,6 @@
     <t>update Hg, was "blockedMemberNode"</t>
   </si>
   <si>
-    <t>indexer.java, set this as a copy field</t>
-  </si>
-  <si>
     <t>copyfield from id</t>
   </si>
   <si>
@@ -859,6 +850,27 @@
   </si>
   <si>
     <t>copyfield from topic</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>copyfield from dateuploaded</t>
+  </si>
+  <si>
+    <t>Using "id" in SOLR since mercury is dependent on this</t>
+  </si>
+  <si>
+    <t>This is set by originMemberNode</t>
+  </si>
+  <si>
+    <t>Remove this - it is a duplicate of datemodified</t>
+  </si>
+  <si>
+    <t>A multivalued field that indicates which resource maps this object appears in. Set by the resource map sub-processor</t>
   </si>
 </sst>
 </file>
@@ -1764,13 +1776,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1784,22 +1796,22 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" t="s">
         <v>178</v>
       </c>
-      <c r="B1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D1" t="s">
-        <v>179</v>
-      </c>
       <c r="E1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" t="s">
         <v>199</v>
-      </c>
-      <c r="F1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1" t="s">
-        <v>200</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -1838,11 +1850,8 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>139</v>
-      </c>
       <c r="I3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1865,7 +1874,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1937,7 +1946,7 @@
         <v>139</v>
       </c>
       <c r="H7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2007,6 +2016,9 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
+      <c r="E11" t="s">
+        <v>141</v>
+      </c>
       <c r="I11">
         <v>0</v>
       </c>
@@ -2019,10 +2031,13 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>141</v>
       </c>
       <c r="I12" t="s">
         <v>6</v>
@@ -2038,6 +2053,9 @@
       <c r="D13" t="s">
         <v>2</v>
       </c>
+      <c r="E13" t="s">
+        <v>141</v>
+      </c>
       <c r="I13" t="s">
         <v>6</v>
       </c>
@@ -2067,7 +2085,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -2076,7 +2094,7 @@
         <v>139</v>
       </c>
       <c r="H15" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="I15" t="s">
         <v>6</v>
@@ -2084,13 +2102,10 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>205</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -2098,33 +2113,33 @@
       <c r="E16" t="s">
         <v>139</v>
       </c>
-      <c r="H16" t="s">
-        <v>245</v>
-      </c>
-      <c r="I16" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" t="s">
+        <v>242</v>
+      </c>
+      <c r="I17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" t="s">
-        <v>246</v>
-      </c>
-      <c r="I17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -2133,27 +2148,24 @@
         <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>223</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
+        <v>243</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="1" t="s">
-        <v>211</v>
+      <c r="A19" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>211</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2161,158 +2173,185 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
       </c>
+      <c r="E20" t="s">
+        <v>264</v>
+      </c>
       <c r="H20" t="s">
-        <v>248</v>
-      </c>
-      <c r="I20" t="s">
-        <v>6</v>
+        <v>244</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" t="s">
-        <v>28</v>
+      <c r="A21" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>150</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
+      <c r="E21" t="s">
+        <v>264</v>
+      </c>
+      <c r="H21" t="s">
+        <v>245</v>
+      </c>
       <c r="I21" t="s">
         <v>6</v>
       </c>
-      <c r="J21" t="s">
-        <v>224</v>
-      </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="1" t="s">
-        <v>29</v>
+      <c r="A22" t="s">
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" t="s">
-        <v>259</v>
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>141</v>
       </c>
       <c r="I22" t="s">
         <v>6</v>
+      </c>
+      <c r="J22" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>265</v>
+      </c>
+      <c r="H23" t="s">
+        <v>256</v>
+      </c>
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>31</v>
       </c>
-      <c r="F23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="E24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" t="s">
         <v>33</v>
       </c>
-      <c r="I23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" t="s">
+      <c r="I24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
         <v>2</v>
       </c>
-      <c r="I24">
+      <c r="E25" t="s">
+        <v>141</v>
+      </c>
+      <c r="I25">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="B26" t="s">
         <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
-      <c r="F26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
         <v>38</v>
       </c>
-      <c r="I26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
+      <c r="I27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28" t="s">
-        <v>249</v>
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>141</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2320,13 +2359,19 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H29" t="s">
+        <v>246</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2334,21 +2379,24 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
-      </c>
-      <c r="I30" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>141</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -2356,19 +2404,25 @@
       <c r="D31" t="s">
         <v>2</v>
       </c>
-      <c r="I31">
-        <v>0</v>
+      <c r="E31" t="s">
+        <v>141</v>
+      </c>
+      <c r="I31" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>141</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2376,7 +2430,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -2384,243 +2438,291 @@
       <c r="D33" t="s">
         <v>5</v>
       </c>
-      <c r="H33" t="s">
-        <v>153</v>
+      <c r="E33" t="s">
+        <v>141</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="1" t="s">
-        <v>46</v>
+      <c r="A34" t="s">
+        <v>45</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
-      </c>
-      <c r="C34" t="s">
-        <v>48</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
-      <c r="I34" t="s">
-        <v>6</v>
-      </c>
-      <c r="J34" t="s">
-        <v>226</v>
+      <c r="E34" t="s">
+        <v>141</v>
+      </c>
+      <c r="H34" t="s">
+        <v>153</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
+      <c r="E35" t="s">
+        <v>139</v>
+      </c>
       <c r="H35" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="I35" t="s">
         <v>6</v>
       </c>
+      <c r="J35" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" t="s">
-        <v>49</v>
+      <c r="A36" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>265</v>
+      </c>
+      <c r="H36" t="s">
+        <v>247</v>
+      </c>
+      <c r="I36" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>141</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
         <v>50</v>
       </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
         <v>5</v>
       </c>
-      <c r="I37" t="s">
-        <v>6</v>
-      </c>
-      <c r="J37" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="1" t="s">
+      <c r="E38" t="s">
+        <v>141</v>
+      </c>
+      <c r="I38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
         <v>2</v>
       </c>
-      <c r="I38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" t="s">
+      <c r="E39" t="s">
+        <v>265</v>
+      </c>
+      <c r="I39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
         <v>52</v>
       </c>
-      <c r="B39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>5</v>
-      </c>
-      <c r="H39" t="s">
-        <v>156</v>
-      </c>
-      <c r="I39" t="s">
-        <v>6</v>
-      </c>
-      <c r="J39" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B40" t="s">
         <v>6</v>
-      </c>
-      <c r="C40" t="s">
-        <v>53</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
       </c>
-      <c r="F40" t="s">
-        <v>6</v>
+      <c r="E40" t="s">
+        <v>141</v>
       </c>
       <c r="H40" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="I40" t="s">
         <v>6</v>
+      </c>
+      <c r="J40" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
         <v>2</v>
       </c>
-      <c r="I41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" t="s">
+      <c r="E42" t="s">
+        <v>265</v>
+      </c>
+      <c r="I42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" t="s">
         <v>56</v>
       </c>
-      <c r="B42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
         <v>5</v>
       </c>
-      <c r="I42">
+      <c r="E43" t="s">
+        <v>141</v>
+      </c>
+      <c r="I43">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:10">
+      <c r="A44" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
         <v>10</v>
       </c>
-      <c r="H43" t="s">
+      <c r="E44" t="s">
+        <v>139</v>
+      </c>
+      <c r="H44" t="s">
         <v>159</v>
       </c>
-      <c r="I43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>5</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
+      <c r="I44" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>141</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="1" t="s">
-        <v>60</v>
+      <c r="A46" t="s">
+        <v>59</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
       </c>
-      <c r="C46" t="s">
-        <v>60</v>
-      </c>
       <c r="D46" t="s">
-        <v>5</v>
-      </c>
-      <c r="H46" t="s">
-        <v>251</v>
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>141</v>
       </c>
       <c r="I46">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" t="s">
-        <v>61</v>
+      <c r="A47" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
       </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
       <c r="D47" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>141</v>
       </c>
       <c r="H47" t="s">
-        <v>160</v>
+        <v>248</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -2628,141 +2730,168 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>141</v>
+      </c>
+      <c r="H48" t="s">
+        <v>160</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" t="s">
         <v>62</v>
       </c>
-      <c r="B48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
         <v>5</v>
       </c>
-      <c r="H48" t="s">
+      <c r="E49" t="s">
+        <v>141</v>
+      </c>
+      <c r="H49" t="s">
         <v>156</v>
       </c>
-      <c r="I48" t="s">
-        <v>6</v>
-      </c>
-      <c r="J48" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" t="s">
-        <v>31</v>
-      </c>
-      <c r="F49" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" t="s">
-        <v>161</v>
-      </c>
       <c r="I49" t="s">
         <v>6</v>
+      </c>
+      <c r="J49" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="E50" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50" t="s">
+        <v>6</v>
       </c>
       <c r="H50" t="s">
-        <v>252</v>
-      </c>
-      <c r="I50">
-        <v>0</v>
+        <v>161</v>
+      </c>
+      <c r="I50" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
       </c>
-      <c r="I51" t="s">
-        <v>6</v>
+      <c r="E51" t="s">
+        <v>139</v>
+      </c>
+      <c r="H51" t="s">
+        <v>249</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
       </c>
+      <c r="E52" t="s">
+        <v>139</v>
+      </c>
       <c r="I52" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>203</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
       </c>
+      <c r="E53" t="s">
+        <v>139</v>
+      </c>
       <c r="I53" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" t="s">
-        <v>70</v>
+      <c r="A54" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
       </c>
+      <c r="C54" t="s">
+        <v>69</v>
+      </c>
       <c r="D54" t="s">
-        <v>2</v>
-      </c>
-      <c r="I54">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>139</v>
+      </c>
+      <c r="I54" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>141</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -2770,7 +2899,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -2778,16 +2907,16 @@
       <c r="D56" t="s">
         <v>5</v>
       </c>
-      <c r="I56" t="s">
-        <v>6</v>
-      </c>
-      <c r="J56" t="s">
-        <v>229</v>
+      <c r="E56" t="s">
+        <v>141</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
@@ -2795,22 +2924,28 @@
       <c r="D57" t="s">
         <v>5</v>
       </c>
-      <c r="I57">
-        <v>0</v>
+      <c r="E57" t="s">
+        <v>141</v>
+      </c>
+      <c r="I57" t="s">
+        <v>6</v>
+      </c>
+      <c r="J57" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="1" t="s">
-        <v>75</v>
+      <c r="A58" t="s">
+        <v>74</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>2</v>
-      </c>
-      <c r="H58" t="s">
-        <v>254</v>
+        <v>5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>141</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -2818,7 +2953,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -2826,50 +2961,65 @@
       <c r="D59" t="s">
         <v>2</v>
       </c>
+      <c r="E59" t="s">
+        <v>265</v>
+      </c>
       <c r="H59" t="s">
-        <v>253</v>
-      </c>
-      <c r="I59" t="s">
-        <v>6</v>
+        <v>251</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>265</v>
+      </c>
+      <c r="H60" t="s">
+        <v>250</v>
+      </c>
+      <c r="I60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" t="s">
         <v>77</v>
       </c>
-      <c r="B60" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
         <v>5</v>
       </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B61" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" t="s">
-        <v>2</v>
+      <c r="E61" t="s">
+        <v>141</v>
       </c>
       <c r="I61">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" t="s">
-        <v>79</v>
+      <c r="A62" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E62" t="s">
+        <v>265</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -2877,58 +3027,67 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>141</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" t="s">
         <v>80</v>
       </c>
-      <c r="B63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
         <v>2</v>
       </c>
-      <c r="H63" t="s">
+      <c r="E64" t="s">
+        <v>141</v>
+      </c>
+      <c r="H64" t="s">
         <v>137</v>
       </c>
-      <c r="I63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="1" t="s">
+      <c r="I64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B64" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="6" t="s">
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="D64" t="s">
-        <v>5</v>
-      </c>
-      <c r="H64" t="s">
-        <v>256</v>
-      </c>
-      <c r="I64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" t="s">
-        <v>6</v>
       </c>
       <c r="D65" t="s">
         <v>5</v>
       </c>
+      <c r="E65" t="s">
+        <v>139</v>
+      </c>
+      <c r="H65" t="s">
+        <v>253</v>
+      </c>
       <c r="I65">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -2936,107 +3095,122 @@
       <c r="D66" t="s">
         <v>5</v>
       </c>
-      <c r="I66" t="s">
-        <v>6</v>
-      </c>
-      <c r="J66" t="s">
-        <v>230</v>
+      <c r="E66" t="s">
+        <v>141</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="1" t="s">
-        <v>84</v>
+      <c r="A67" t="s">
+        <v>83</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>2</v>
-      </c>
-      <c r="H67" t="s">
-        <v>257</v>
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>141</v>
       </c>
       <c r="I67" t="s">
         <v>6</v>
+      </c>
+      <c r="J67" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>265</v>
+      </c>
+      <c r="H68" t="s">
+        <v>254</v>
+      </c>
+      <c r="I68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B68" t="s">
-        <v>6</v>
-      </c>
-      <c r="C68" t="s">
-        <v>222</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>221</v>
+      </c>
+      <c r="D69" t="s">
         <v>10</v>
       </c>
-      <c r="H68" t="s">
-        <v>258</v>
-      </c>
-      <c r="I68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" t="s">
+      <c r="E69" t="s">
+        <v>265</v>
+      </c>
+      <c r="H69" t="s">
+        <v>255</v>
+      </c>
+      <c r="I69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" t="s">
         <v>87</v>
       </c>
-      <c r="B69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="B70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
         <v>2</v>
       </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" t="s">
-        <v>145</v>
-      </c>
-      <c r="D70" t="s">
-        <v>5</v>
-      </c>
-      <c r="H70" t="s">
-        <v>260</v>
+      <c r="E70" t="s">
+        <v>141</v>
       </c>
       <c r="I70">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="2" t="s">
-        <v>89</v>
+      <c r="A71" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>145</v>
       </c>
       <c r="D71" t="s">
         <v>5</v>
       </c>
+      <c r="E71" t="s">
+        <v>139</v>
+      </c>
+      <c r="H71" t="s">
+        <v>257</v>
+      </c>
       <c r="I71">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="1" t="s">
-        <v>90</v>
+      <c r="A72" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
-      </c>
-      <c r="C72" t="s">
-        <v>203</v>
       </c>
       <c r="D72" t="s">
         <v>5</v>
@@ -3046,59 +3220,74 @@
       </c>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" t="s">
-        <v>91</v>
+      <c r="A73" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>202</v>
       </c>
       <c r="D73" t="s">
         <v>5</v>
       </c>
+      <c r="E73" t="s">
+        <v>139</v>
+      </c>
       <c r="I73">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="1" t="s">
-        <v>92</v>
+      <c r="A74" t="s">
+        <v>91</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>2</v>
-      </c>
-      <c r="H74" t="s">
-        <v>261</v>
+        <v>5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>141</v>
       </c>
       <c r="I74">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" t="s">
-        <v>93</v>
+      <c r="A75" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E75" t="s">
+        <v>265</v>
+      </c>
+      <c r="H75" t="s">
+        <v>258</v>
       </c>
       <c r="I75">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="1" t="s">
-        <v>94</v>
+      <c r="A76" t="s">
+        <v>93</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
+        <v>141</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -3106,64 +3295,73 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
       </c>
-      <c r="C77" t="s">
-        <v>95</v>
-      </c>
       <c r="D77" t="s">
-        <v>96</v>
-      </c>
-      <c r="I77" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="E77" t="s">
+        <v>265</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>95</v>
+      </c>
+      <c r="D78" t="s">
+        <v>96</v>
+      </c>
+      <c r="E78" t="s">
+        <v>139</v>
+      </c>
+      <c r="I78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B78" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="B79" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s">
         <v>98</v>
       </c>
-      <c r="I78" t="s">
-        <v>6</v>
-      </c>
-      <c r="J78" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" t="s">
+      <c r="E79" t="s">
+        <v>265</v>
+      </c>
+      <c r="I79" t="s">
+        <v>6</v>
+      </c>
+      <c r="J79" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" t="s">
         <v>99</v>
       </c>
-      <c r="B79" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
         <v>5</v>
       </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B80" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" t="s">
-        <v>2</v>
-      </c>
-      <c r="H80" t="s">
-        <v>262</v>
+      <c r="E80" t="s">
+        <v>141</v>
       </c>
       <c r="I80">
         <v>0</v>
@@ -3171,130 +3369,148 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81" t="s">
+        <v>265</v>
+      </c>
+      <c r="H81" t="s">
+        <v>259</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B81" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="B82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" t="s">
         <v>101</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D82" t="s">
         <v>31</v>
       </c>
-      <c r="F81" t="s">
-        <v>6</v>
-      </c>
-      <c r="H81" t="s">
+      <c r="E82" t="s">
+        <v>141</v>
+      </c>
+      <c r="F82" t="s">
+        <v>6</v>
+      </c>
+      <c r="H82" t="s">
         <v>103</v>
       </c>
-      <c r="I81" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
-      <c r="A82" t="s">
+      <c r="I82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" t="s">
         <v>104</v>
       </c>
-      <c r="B82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" t="s">
-        <v>220</v>
-      </c>
-      <c r="D82" t="s">
-        <v>5</v>
-      </c>
-      <c r="I82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="A83" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="B83" t="s">
         <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>105</v>
+        <v>219</v>
       </c>
       <c r="D83" t="s">
         <v>5</v>
       </c>
-      <c r="I83" t="s">
-        <v>6</v>
+      <c r="E83" t="s">
+        <v>141</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" t="s">
-        <v>106</v>
+      <c r="A84" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="B84" t="s">
         <v>6</v>
+      </c>
+      <c r="C84" t="s">
+        <v>105</v>
       </c>
       <c r="D84" t="s">
         <v>5</v>
       </c>
-      <c r="I84">
-        <v>0</v>
+      <c r="E84" t="s">
+        <v>139</v>
+      </c>
+      <c r="I84" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="1" t="s">
-        <v>107</v>
+      <c r="A85" t="s">
+        <v>106</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>2</v>
-      </c>
-      <c r="H85" t="s">
-        <v>263</v>
+        <v>5</v>
+      </c>
+      <c r="E85" t="s">
+        <v>141</v>
       </c>
       <c r="I85">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" t="s">
-        <v>2</v>
+      <c r="A86" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
-      </c>
-      <c r="C86" t="s">
-        <v>2</v>
       </c>
       <c r="D86" t="s">
         <v>2</v>
       </c>
-      <c r="F86" t="s">
-        <v>6</v>
+      <c r="E86" t="s">
+        <v>265</v>
       </c>
       <c r="H86" t="s">
-        <v>264</v>
-      </c>
-      <c r="I86" t="s">
-        <v>6</v>
+        <v>260</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="1" t="s">
-        <v>108</v>
+      <c r="A87" t="s">
+        <v>2</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E87" t="s">
+        <v>265</v>
       </c>
       <c r="F87" t="s">
         <v>6</v>
+      </c>
+      <c r="H87" t="s">
+        <v>261</v>
       </c>
       <c r="I87" t="s">
         <v>6</v>
@@ -3302,16 +3518,22 @@
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
+      </c>
+      <c r="C88" t="s">
+        <v>108</v>
       </c>
       <c r="D88" t="s">
         <v>5</v>
       </c>
-      <c r="H88" t="s">
-        <v>265</v>
+      <c r="E88" t="s">
+        <v>141</v>
+      </c>
+      <c r="F88" t="s">
+        <v>6</v>
       </c>
       <c r="I88" t="s">
         <v>6</v>
@@ -3319,7 +3541,7 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
@@ -3327,16 +3549,19 @@
       <c r="D89" t="s">
         <v>5</v>
       </c>
+      <c r="E89" t="s">
+        <v>265</v>
+      </c>
       <c r="H89" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="I89" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:10">
-      <c r="A90" t="s">
-        <v>111</v>
+      <c r="A90" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="B90" t="s">
         <v>6</v>
@@ -3344,22 +3569,28 @@
       <c r="D90" t="s">
         <v>5</v>
       </c>
-      <c r="I90">
-        <v>0</v>
+      <c r="E90" t="s">
+        <v>265</v>
+      </c>
+      <c r="H90" t="s">
+        <v>262</v>
+      </c>
+      <c r="I90" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:10">
-      <c r="A91" s="1" t="s">
-        <v>112</v>
+      <c r="A91" t="s">
+        <v>111</v>
       </c>
       <c r="B91" t="s">
         <v>6</v>
       </c>
       <c r="D91" t="s">
-        <v>2</v>
-      </c>
-      <c r="H91" t="s">
-        <v>266</v>
+        <v>5</v>
+      </c>
+      <c r="E91" t="s">
+        <v>141</v>
       </c>
       <c r="I91">
         <v>0</v>
@@ -3367,157 +3598,225 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" t="s">
+        <v>2</v>
+      </c>
+      <c r="E92" t="s">
+        <v>265</v>
+      </c>
+      <c r="H92" t="s">
+        <v>263</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B92" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92" t="s">
-        <v>177</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" t="s">
+        <v>176</v>
+      </c>
+      <c r="D93" t="s">
         <v>10</v>
       </c>
-      <c r="H92" t="s">
-        <v>171</v>
-      </c>
-      <c r="I92" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="A93" t="s">
+      <c r="E93" t="s">
+        <v>265</v>
+      </c>
+      <c r="H93" t="s">
+        <v>266</v>
+      </c>
+      <c r="I93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" t="s">
         <v>114</v>
       </c>
-      <c r="B93" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" t="s">
         <v>5</v>
       </c>
-      <c r="I93" t="s">
-        <v>6</v>
-      </c>
-      <c r="J93" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
-      <c r="A94" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B94" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" t="s">
-        <v>115</v>
-      </c>
-      <c r="D94" t="s">
-        <v>31</v>
-      </c>
-      <c r="F94" t="s">
-        <v>6</v>
-      </c>
-      <c r="H94" t="s">
-        <v>118</v>
+      <c r="E94" t="s">
+        <v>141</v>
       </c>
       <c r="I94" t="s">
         <v>6</v>
+      </c>
+      <c r="J94" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="1" t="s">
-        <v>206</v>
+        <v>115</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
+        <v>115</v>
+      </c>
+      <c r="D95" t="s">
+        <v>31</v>
+      </c>
+      <c r="E95" t="s">
+        <v>141</v>
+      </c>
+      <c r="F95" t="s">
+        <v>6</v>
       </c>
       <c r="H95" t="s">
-        <v>240</v>
+        <v>118</v>
+      </c>
+      <c r="I95" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="E96" t="s">
+        <v>139</v>
       </c>
       <c r="H96" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
+      </c>
+      <c r="E97" t="s">
+        <v>139</v>
       </c>
       <c r="H97" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
+      </c>
+      <c r="E98" t="s">
+        <v>139</v>
       </c>
       <c r="H98" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
+      </c>
+      <c r="E99" t="s">
+        <v>139</v>
       </c>
       <c r="H99" t="s">
-        <v>241</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
+      </c>
+      <c r="E100" t="s">
+        <v>139</v>
       </c>
       <c r="H100" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
+      </c>
+      <c r="E101" t="s">
+        <v>139</v>
+      </c>
+      <c r="H101" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
+      </c>
+      <c r="E102" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
+      </c>
+      <c r="E103" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H104" t="s">
-        <v>235</v>
+        <v>214</v>
+      </c>
+      <c r="E104" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" t="s">
-        <v>219</v>
+      <c r="A105" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E105" t="s">
+        <v>139</v>
       </c>
       <c r="H105" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>217</v>
+        <v>218</v>
+      </c>
+      <c r="E106" t="s">
+        <v>141</v>
       </c>
       <c r="H106" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>218</v>
+        <v>216</v>
+      </c>
+      <c r="E107" t="s">
+        <v>141</v>
       </c>
       <c r="H107" t="s">
-        <v>238</v>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>217</v>
+      </c>
+      <c r="E108" t="s">
+        <v>141</v>
+      </c>
+      <c r="H108" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3551,16 +3850,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" t="s">
         <v>197</v>
       </c>
-      <c r="B1" t="s">
-        <v>198</v>
-      </c>
       <c r="C1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" t="s">
         <v>175</v>
-      </c>
-      <c r="D1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3674,7 +3973,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3824,7 +4123,7 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -4210,16 +4509,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
         <v>192</v>
       </c>
-      <c r="B1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>193</v>
-      </c>
-      <c r="D1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4227,10 +4526,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4243,10 +4542,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" t="s">
         <v>186</v>
-      </c>
-      <c r="C4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4254,10 +4553,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4265,10 +4564,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4362,7 +4661,7 @@
         <v>163</v>
       </c>
       <c r="C23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4380,10 +4679,10 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
         <v>182</v>
-      </c>
-      <c r="C26" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -4510,7 +4809,7 @@
         <v>162</v>
       </c>
       <c r="C49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -4710,7 +5009,7 @@
         <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -4721,7 +5020,7 @@
         <v>169</v>
       </c>
       <c r="C87" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -4754,7 +5053,7 @@
         <v>114</v>
       </c>
       <c r="B93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -4859,16 +5158,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
         <v>192</v>
       </c>
-      <c r="B1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>193</v>
-      </c>
-      <c r="D1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5377,7 +5676,7 @@
         <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -5525,16 +5824,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
         <v>192</v>
       </c>
-      <c r="B1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>193</v>
-      </c>
-      <c r="D1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6012,7 +6311,7 @@
         <v>114</v>
       </c>
       <c r="B93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:2">

</xml_diff>

<commit_message>
Updating again, fixed this time...
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -882,7 +882,7 @@
     <t>inHG</t>
   </si>
   <si>
-    <t>Populated_0.5.1</t>
+    <t>Populated_0_5_1</t>
   </si>
 </sst>
 </file>
@@ -1791,10 +1791,10 @@
   <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H59" sqref="H59"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Numerous minor edits to CN REST service descriptions. See change log for a complete list of updates
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60180" yWindow="320" windowWidth="26980" windowHeight="20420" tabRatio="500"/>
+    <workbookView xWindow="1140" yWindow="720" windowWidth="26980" windowHeight="20420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="262">
   <si>
     <t>Notes</t>
   </si>
@@ -808,9 +808,6 @@
     <t>updateHg, was previously dateSysMetadataModified</t>
   </si>
   <si>
-    <t>DateHandler.java, should make this a date for proper searching</t>
-  </si>
-  <si>
     <t>update Hg, previously describedBy</t>
   </si>
   <si>
@@ -911,6 +908,21 @@
   </si>
   <si>
     <t>Should contain a URL for downloading the object</t>
+  </si>
+  <si>
+    <t>distinct-values(//creator/organizationName)</t>
+  </si>
+  <si>
+    <t>Need to combine these values outside of Xpath</t>
+  </si>
+  <si>
+    <t>Properly formatted should be like "LAST, FIRST INITIAL.; LAST, FIRST INITIAL.;…"</t>
+  </si>
+  <si>
+    <t>Constructed from begindate and enddate, but not sure on what happens when more than a single decade is covered</t>
+  </si>
+  <si>
+    <t>DateHandler.java, should make this a date for proper searching. Note that in Mercury, this value is based on the end date if available, otherwise the begin date, otherwise "unknown"</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1023,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="273">
+  <cellStyleXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1046,6 +1058,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1293,7 +1307,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="273">
+  <cellStyles count="275">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1433,6 +1447,7 @@
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1566,6 +1581,7 @@
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1898,10 +1914,10 @@
   <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1919,13 +1935,13 @@
         <v>164</v>
       </c>
       <c r="B1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E1" t="s">
         <v>165</v>
@@ -1943,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2006,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -2156,11 +2172,11 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>255</v>
+      <c r="B12" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -2216,8 +2232,8 @@
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>255</v>
+      <c r="B15" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -2232,7 +2248,7 @@
         <v>133</v>
       </c>
       <c r="I15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J15" t="s">
         <v>6</v>
@@ -2280,7 +2296,7 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -2289,7 +2305,7 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
-        <v>223</v>
+        <v>261</v>
       </c>
       <c r="J18" t="s">
         <v>6</v>
@@ -2326,10 +2342,10 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -2349,10 +2365,10 @@
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J21" t="s">
         <v>6</v>
@@ -2392,10 +2408,10 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J23" t="s">
         <v>6</v>
@@ -2515,7 +2531,7 @@
         <v>135</v>
       </c>
       <c r="I29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -2626,7 +2642,7 @@
         <v>133</v>
       </c>
       <c r="I35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J35" t="s">
         <v>6</v>
@@ -2643,10 +2659,10 @@
         <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J36" t="s">
         <v>6</v>
@@ -2700,7 +2716,7 @@
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J39" t="s">
         <v>6</v>
@@ -2720,7 +2736,7 @@
         <v>135</v>
       </c>
       <c r="I40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J40" t="s">
         <v>6</v>
@@ -2730,8 +2746,8 @@
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B41" t="s">
-        <v>255</v>
+      <c r="B41" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -2766,7 +2782,7 @@
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J42" t="s">
         <v>6</v>
@@ -2803,7 +2819,7 @@
         <v>133</v>
       </c>
       <c r="I44" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J44" t="s">
         <v>6</v>
@@ -2860,7 +2876,7 @@
         <v>135</v>
       </c>
       <c r="I47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -2900,7 +2916,7 @@
         <v>135</v>
       </c>
       <c r="I49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J49" t="s">
         <v>6</v>
@@ -2949,7 +2965,7 @@
         <v>133</v>
       </c>
       <c r="I51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -3100,10 +3116,10 @@
         <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I59" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -3120,10 +3136,10 @@
         <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I60" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J60" t="s">
         <v>6</v>
@@ -3160,7 +3176,7 @@
         <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -3220,7 +3236,7 @@
         <v>133</v>
       </c>
       <c r="I65" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -3280,10 +3296,10 @@
         <v>2</v>
       </c>
       <c r="F68" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I68" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J68" t="s">
         <v>6</v>
@@ -3303,10 +3319,10 @@
         <v>10</v>
       </c>
       <c r="F69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J69" t="s">
         <v>6</v>
@@ -3346,7 +3362,7 @@
         <v>133</v>
       </c>
       <c r="I71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J71">
         <v>0</v>
@@ -3420,10 +3436,10 @@
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I75" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -3457,7 +3473,7 @@
         <v>2</v>
       </c>
       <c r="F77" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J77">
         <v>0</v>
@@ -3494,7 +3510,7 @@
         <v>92</v>
       </c>
       <c r="F79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I79" t="s">
         <v>221</v>
@@ -3531,10 +3547,10 @@
         <v>2</v>
       </c>
       <c r="F81" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I81" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J81">
         <v>0</v>
@@ -3634,17 +3650,17 @@
         <v>2</v>
       </c>
       <c r="F86" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I86" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J86">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C87" t="s">
@@ -3657,13 +3673,13 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G87" t="s">
         <v>6</v>
       </c>
       <c r="I87" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J87" t="s">
         <v>6</v>
@@ -3673,7 +3689,7 @@
       <c r="A88" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C88" t="s">
@@ -3706,10 +3722,10 @@
         <v>5</v>
       </c>
       <c r="F89" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I89" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J89" t="s">
         <v>6</v>
@@ -3726,10 +3742,10 @@
         <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I90" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J90" t="s">
         <v>6</v>
@@ -3766,10 +3782,10 @@
         <v>2</v>
       </c>
       <c r="F92" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I92" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J92">
         <v>0</v>
@@ -3789,17 +3805,17 @@
         <v>10</v>
       </c>
       <c r="F93" t="s">
+        <v>244</v>
+      </c>
+      <c r="I93" t="s">
         <v>245</v>
       </c>
-      <c r="I93" t="s">
-        <v>246</v>
-      </c>
       <c r="J93" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:10">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C94" t="s">
@@ -3812,7 +3828,7 @@
         <v>135</v>
       </c>
       <c r="I94" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J94" t="s">
         <v>6</v>
@@ -3882,10 +3898,10 @@
         <v>192</v>
       </c>
       <c r="F99" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I99" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3893,7 +3909,7 @@
         <v>193</v>
       </c>
       <c r="F100" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I100" t="s">
         <v>219</v>
@@ -3998,7 +4014,7 @@
   <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A108"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4049,6 +4065,9 @@
       <c r="C4" t="s">
         <v>173</v>
       </c>
+      <c r="D4" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
@@ -4101,6 +4120,12 @@
       <c r="A12" t="s">
         <v>18</v>
       </c>
+      <c r="B12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
@@ -4122,32 +4147,35 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -4155,12 +4183,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -4171,17 +4199,17 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -4192,27 +4220,27 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Updating list of search fields and the origin of content used to populate them
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="0" windowWidth="30540" windowHeight="25420" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="800" yWindow="0" windowWidth="30540" windowHeight="25420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Dryad" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$J$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$L$102</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="286">
   <si>
     <t>Notes</t>
   </si>
@@ -694,9 +694,6 @@
     <t>replica_mn</t>
   </si>
   <si>
-    <t>replica_verified</t>
-  </si>
-  <si>
     <t>resourcemap</t>
   </si>
   <si>
@@ -751,9 +748,6 @@
     <t>Looks like project name from EML</t>
   </si>
   <si>
-    <t>Time stamps for when D1 replicas were verified as complete</t>
-  </si>
-  <si>
     <t>Multivalued field that lists the subjects that have read permission on the object</t>
   </si>
   <si>
@@ -899,6 +893,108 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Multi</t>
+  </si>
+  <si>
+    <t>ValueOrigin</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.replicationPolicy` blockedMemberNode</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.checksum`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.algorithm`</t>
+  </si>
+  <si>
+    <t>Resolve REST URL created from PID</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.dateSysMetadataModified`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.dateUploaded`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.identifier`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.replicationPolicy` numberReplicas attribute</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.formatId`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.obsoletedBy`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.obsoletes`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.replicationPolicy` preferredMemberNode</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.replicationPolicy` replicationAllowed attribute</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.rightsHolder`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.size`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.submitter`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.authoritativeMemberNode`</t>
+  </si>
+  <si>
+    <t>:attr:`SystemMetadata.replica` replica/replicationMemberNode element</t>
+  </si>
+  <si>
+    <t>List of subjects (groups and individuals) that have read permission on PID, value retrieved from :attr:`SystemMetadata.accessPolicy`.</t>
+  </si>
+  <si>
+    <t>List of subjects (groups and individuals) that have write permission on PID, value retrieved from :attr:`SystemMetadata.accessPolicy`.</t>
+  </si>
+  <si>
+    <t>List of subjects (groups and individuals) that have execute permission on PID, value retrieved from :attr:`SystemMetadata.accessPolicy`.</t>
+  </si>
+  <si>
+    <t>List of subjects (groups and individuals) that have change permission on PID, value retrieved from :attr:`SystemMetadata.accessPolicy`.</t>
+  </si>
+  <si>
+    <t>Set to True if the DataONE :term:`public user` is present in the list of subjects with readPermission on PID.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>Taxonomy</t>
+  </si>
+  <si>
+    <t>contactOrganization, datasource, decade, features, fileID, fullText, gcmdKeyword, geoform, id, includes, investigator, keywords, LTERSite, manu, name, origin, originator, parameter, placeKey, presentationCat, project, purpose, sensor, site, source, term, title, topic</t>
+  </si>
+  <si>
+    <t>List of resource map PIDs that reference this PID.</t>
+  </si>
+  <si>
+    <t>A list of all objects (PIDs) referenced by a resource map. Only populated if the current object is a resource map.</t>
+  </si>
+  <si>
+    <t>Lists all PIDs that this object describes. Obtained by parsing all resource maps in which this object is referenced. Not set for data or resource map objects.</t>
+  </si>
+  <si>
+    <t>Lists all PIDs that describe this object. Obtained by parsing all resource maps in which this object is referenced.</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1083,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="402">
+  <cellStyleXfs count="410">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1390,14 +1486,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="402">
+  <cellStyles count="410">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1601,6 +1708,14 @@
     <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -2128,13 +2243,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2143,44 +2258,51 @@
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" customWidth="1"/>
     <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" customWidth="1"/>
-    <col min="9" max="9" width="42.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+    <col min="10" max="10" width="57" customWidth="1"/>
+    <col min="11" max="11" width="42.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E1" t="s">
         <v>159</v>
       </c>
       <c r="F1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1" t="s">
         <v>177</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>176</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>178</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>253</v>
+      </c>
+      <c r="K1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="L1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2194,16 +2316,19 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>278</v>
+      </c>
+      <c r="G2" t="s">
         <v>129</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2220,19 +2345,22 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" t="s">
         <v>129</v>
       </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>224</v>
-      </c>
-      <c r="J3">
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>222</v>
+      </c>
+      <c r="L3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2246,16 +2374,19 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" t="s">
         <v>129</v>
       </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2269,19 +2400,22 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
+        <v>278</v>
+      </c>
+      <c r="G5" t="s">
         <v>129</v>
       </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" t="s">
         <v>11</v>
       </c>
-      <c r="J5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>133</v>
       </c>
@@ -2295,16 +2429,22 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
+        <v>277</v>
+      </c>
+      <c r="G6" t="s">
         <v>127</v>
       </c>
-      <c r="I6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J6">
+      <c r="J6" t="s">
+        <v>254</v>
+      </c>
+      <c r="K6" t="s">
+        <v>211</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2314,11 +2454,17 @@
       <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="J7">
+      <c r="F7" t="s">
+        <v>277</v>
+      </c>
+      <c r="G7" t="s">
+        <v>129</v>
+      </c>
+      <c r="L7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -2332,13 +2478,19 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G8" t="s">
         <v>127</v>
       </c>
       <c r="J8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>255</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -2352,13 +2504,19 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
+        <v>278</v>
+      </c>
+      <c r="G9" t="s">
         <v>127</v>
       </c>
       <c r="J9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>256</v>
+      </c>
+      <c r="L9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -2369,36 +2527,45 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
+        <v>277</v>
+      </c>
+      <c r="G10" t="s">
         <v>129</v>
       </c>
-      <c r="J10">
+      <c r="K10" t="s">
+        <v>280</v>
+      </c>
+      <c r="L10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
       </c>
       <c r="F11" t="s">
+        <v>278</v>
+      </c>
+      <c r="G11" t="s">
         <v>129</v>
       </c>
-      <c r="J11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="L11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -2409,13 +2576,19 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>253</v>
+        <v>278</v>
+      </c>
+      <c r="G12" t="s">
+        <v>251</v>
       </c>
       <c r="J12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>17</v>
+      </c>
+      <c r="L12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2425,19 +2598,28 @@
       <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="I13" t="s">
+      <c r="F13" t="s">
+        <v>278</v>
+      </c>
+      <c r="G13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" t="s">
+        <v>257</v>
+      </c>
+      <c r="K13" t="s">
         <v>134</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -2448,17 +2630,23 @@
       <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G14" t="s">
         <v>127</v>
       </c>
-      <c r="I14" t="s">
-        <v>239</v>
-      </c>
       <c r="J14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>258</v>
+      </c>
+      <c r="K14" t="s">
+        <v>237</v>
+      </c>
+      <c r="L14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>157</v>
       </c>
@@ -2468,11 +2656,17 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G15" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="J15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>182</v>
       </c>
@@ -2485,22 +2679,28 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G16" t="s">
         <v>127</v>
       </c>
-      <c r="I16" t="s">
-        <v>215</v>
-      </c>
       <c r="J16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>258</v>
+      </c>
+      <c r="K16" t="s">
+        <v>213</v>
+      </c>
+      <c r="L16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2508,40 +2708,49 @@
       <c r="E17" t="s">
         <v>4</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G17" t="s">
         <v>129</v>
       </c>
-      <c r="I17" t="s">
-        <v>252</v>
-      </c>
-      <c r="J17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" t="s">
+        <v>250</v>
+      </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
-      <c r="F18" t="s">
-        <v>236</v>
-      </c>
-      <c r="I18" t="s">
-        <v>216</v>
-      </c>
-      <c r="J18">
+      <c r="F18" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G18" t="s">
+        <v>234</v>
+      </c>
+      <c r="J18" t="s">
+        <v>285</v>
+      </c>
+      <c r="K18" t="s">
+        <v>214</v>
+      </c>
+      <c r="L18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>135</v>
       </c>
@@ -2554,17 +2763,23 @@
       <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="F19" t="s">
-        <v>236</v>
-      </c>
-      <c r="I19" t="s">
-        <v>217</v>
+      <c r="F19" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G19" t="s">
+        <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>284</v>
+      </c>
+      <c r="K19" t="s">
+        <v>215</v>
+      </c>
+      <c r="L19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2577,17 +2792,20 @@
       <c r="E20" t="s">
         <v>4</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G20" t="s">
         <v>129</v>
       </c>
-      <c r="I20" t="s">
-        <v>200</v>
-      </c>
-      <c r="J20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" t="s">
+        <v>199</v>
+      </c>
+      <c r="L20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2597,17 +2815,23 @@
       <c r="E21" t="s">
         <v>2</v>
       </c>
-      <c r="F21" t="s">
-        <v>253</v>
-      </c>
-      <c r="I21" t="s">
-        <v>228</v>
-      </c>
-      <c r="J21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="F21" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G21" t="s">
+        <v>251</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" t="s">
+        <v>226</v>
+      </c>
+      <c r="L21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -2620,20 +2844,23 @@
       <c r="E22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G22" t="s">
         <v>129</v>
       </c>
-      <c r="G22" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" t="s">
         <v>27</v>
       </c>
-      <c r="J22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="L22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -2643,14 +2870,17 @@
       <c r="E23" t="s">
         <v>2</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G23" t="s">
         <v>129</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2663,20 +2893,23 @@
       <c r="E24" t="s">
         <v>9</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G24" t="s">
         <v>129</v>
       </c>
-      <c r="G24" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="H24" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" t="s">
         <v>31</v>
       </c>
-      <c r="J24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="L24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2686,14 +2919,20 @@
       <c r="E25" t="s">
         <v>4</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G25" t="s">
         <v>129</v>
       </c>
-      <c r="J25">
+      <c r="K25" t="s">
+        <v>280</v>
+      </c>
+      <c r="L25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2703,17 +2942,20 @@
       <c r="E26" t="s">
         <v>2</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G26" t="s">
         <v>129</v>
       </c>
-      <c r="I26" t="s">
-        <v>218</v>
-      </c>
-      <c r="J26">
+      <c r="K26" t="s">
+        <v>216</v>
+      </c>
+      <c r="L26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2723,14 +2965,17 @@
       <c r="E27" t="s">
         <v>4</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G27" t="s">
         <v>129</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2740,14 +2985,17 @@
       <c r="E28" t="s">
         <v>2</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G28" t="s">
         <v>129</v>
       </c>
-      <c r="J28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="L28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2757,14 +3005,17 @@
       <c r="E29" t="s">
         <v>2</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G29" t="s">
         <v>129</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2774,14 +3025,20 @@
       <c r="E30" t="s">
         <v>4</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G30" t="s">
         <v>129</v>
       </c>
-      <c r="J30">
+      <c r="K30" t="s">
+        <v>280</v>
+      </c>
+      <c r="L30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2791,17 +3048,20 @@
       <c r="E31" t="s">
         <v>4</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G31" t="s">
         <v>129</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>138</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -2814,17 +3074,23 @@
       <c r="E32" t="s">
         <v>4</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G32" t="s">
         <v>127</v>
       </c>
-      <c r="I32" t="s">
-        <v>238</v>
-      </c>
       <c r="J32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>260</v>
+      </c>
+      <c r="K32" t="s">
+        <v>236</v>
+      </c>
+      <c r="L32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
@@ -2834,17 +3100,23 @@
       <c r="E33" t="s">
         <v>4</v>
       </c>
-      <c r="F33" t="s">
-        <v>253</v>
-      </c>
-      <c r="I33" t="s">
-        <v>219</v>
+      <c r="F33" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G33" t="s">
+        <v>251</v>
       </c>
       <c r="J33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <v>39</v>
+      </c>
+      <c r="K33" t="s">
+        <v>217</v>
+      </c>
+      <c r="L33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2854,14 +3126,17 @@
       <c r="E34" t="s">
         <v>2</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G34" t="s">
         <v>129</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2871,17 +3146,20 @@
       <c r="E35" t="s">
         <v>4</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G35" t="s">
         <v>129</v>
       </c>
-      <c r="I35" t="s">
-        <v>201</v>
-      </c>
-      <c r="J35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" t="s">
+        <v>200</v>
+      </c>
+      <c r="L35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
@@ -2891,14 +3169,20 @@
       <c r="E36" t="s">
         <v>2</v>
       </c>
-      <c r="F36" t="s">
-        <v>253</v>
+      <c r="F36" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G36" t="s">
+        <v>251</v>
       </c>
       <c r="J36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>43</v>
+      </c>
+      <c r="L36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -2908,22 +3192,25 @@
       <c r="E37" t="s">
         <v>4</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G37" t="s">
         <v>129</v>
       </c>
-      <c r="I37" t="s">
-        <v>246</v>
-      </c>
-      <c r="J37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37" t="s">
+        <v>244</v>
+      </c>
+      <c r="L37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -2934,20 +3221,23 @@
       <c r="E38" t="s">
         <v>4</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G38" t="s">
         <v>129</v>
       </c>
-      <c r="G38" t="s">
-        <v>5</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="H38" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38" t="s">
         <v>128</v>
       </c>
-      <c r="J38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="L38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
@@ -2957,14 +3247,20 @@
       <c r="E39" t="s">
         <v>2</v>
       </c>
-      <c r="F39" t="s">
-        <v>253</v>
+      <c r="F39" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G39" t="s">
+        <v>251</v>
       </c>
       <c r="J39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <v>46</v>
+      </c>
+      <c r="L39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -2974,14 +3270,20 @@
       <c r="E40" t="s">
         <v>4</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G40" t="s">
         <v>129</v>
       </c>
-      <c r="J40">
+      <c r="K40" t="s">
+        <v>280</v>
+      </c>
+      <c r="L40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -2991,14 +3293,17 @@
       <c r="E41" t="s">
         <v>4</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G41" t="s">
         <v>129</v>
       </c>
-      <c r="J41">
+      <c r="L41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -3008,14 +3313,17 @@
       <c r="E42" t="s">
         <v>2</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G42" t="s">
         <v>129</v>
       </c>
-      <c r="J42">
+      <c r="L42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
@@ -3028,17 +3336,23 @@
       <c r="E43" t="s">
         <v>4</v>
       </c>
-      <c r="F43" t="s">
-        <v>253</v>
-      </c>
-      <c r="I43" t="s">
-        <v>220</v>
-      </c>
-      <c r="J43">
+      <c r="F43" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G43" t="s">
+        <v>251</v>
+      </c>
+      <c r="J43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K43" t="s">
+        <v>218</v>
+      </c>
+      <c r="L43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -3048,17 +3362,20 @@
       <c r="E44" t="s">
         <v>2</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G44" t="s">
         <v>129</v>
       </c>
-      <c r="I44" t="s">
+      <c r="K44" t="s">
         <v>143</v>
       </c>
-      <c r="J44">
+      <c r="L44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -3068,17 +3385,20 @@
       <c r="E45" t="s">
         <v>4</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G45" t="s">
         <v>129</v>
       </c>
-      <c r="I45" t="s">
-        <v>246</v>
-      </c>
-      <c r="J45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45" t="s">
+        <v>244</v>
+      </c>
+      <c r="L45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>55</v>
       </c>
@@ -3092,19 +3412,22 @@
         <v>25</v>
       </c>
       <c r="F46" t="s">
+        <v>278</v>
+      </c>
+      <c r="G46" t="s">
         <v>129</v>
       </c>
-      <c r="G46" t="s">
-        <v>5</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="H46" t="s">
+        <v>5</v>
+      </c>
+      <c r="K46" t="s">
         <v>144</v>
       </c>
-      <c r="J46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="L46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>131</v>
       </c>
@@ -3117,17 +3440,23 @@
       <c r="E47" t="s">
         <v>4</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G47" t="s">
         <v>127</v>
       </c>
-      <c r="I47" t="s">
-        <v>221</v>
-      </c>
-      <c r="J47">
+      <c r="J47" t="s">
+        <v>261</v>
+      </c>
+      <c r="K47" t="s">
+        <v>219</v>
+      </c>
+      <c r="L47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
@@ -3140,14 +3469,20 @@
       <c r="E48" t="s">
         <v>4</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G48" t="s">
         <v>127</v>
       </c>
       <c r="J48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>262</v>
+      </c>
+      <c r="L48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
         <v>181</v>
       </c>
@@ -3160,14 +3495,20 @@
       <c r="E49" t="s">
         <v>4</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G49" t="s">
         <v>127</v>
       </c>
       <c r="J49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+        <v>263</v>
+      </c>
+      <c r="L49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
         <v>59</v>
       </c>
@@ -3180,14 +3521,20 @@
       <c r="E50" t="s">
         <v>4</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G50" t="s">
         <v>127</v>
       </c>
       <c r="J50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+        <v>264</v>
+      </c>
+      <c r="L50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -3197,14 +3544,17 @@
       <c r="E51" t="s">
         <v>2</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G51" t="s">
         <v>129</v>
       </c>
-      <c r="J51">
+      <c r="L51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -3214,14 +3564,20 @@
       <c r="E52" t="s">
         <v>4</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G52" t="s">
         <v>129</v>
       </c>
-      <c r="J52">
+      <c r="K52" t="s">
+        <v>280</v>
+      </c>
+      <c r="L52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -3234,17 +3590,20 @@
       <c r="E53" t="s">
         <v>4</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G53" t="s">
         <v>129</v>
       </c>
-      <c r="I53" t="s">
-        <v>202</v>
-      </c>
-      <c r="J53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53" t="s">
+        <v>201</v>
+      </c>
+      <c r="L53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -3254,14 +3613,17 @@
       <c r="E54" t="s">
         <v>4</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G54" t="s">
         <v>129</v>
       </c>
-      <c r="J54">
+      <c r="L54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:12">
       <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
@@ -3271,17 +3633,23 @@
       <c r="E55" t="s">
         <v>2</v>
       </c>
-      <c r="F55" t="s">
-        <v>253</v>
-      </c>
-      <c r="I55" t="s">
-        <v>223</v>
-      </c>
-      <c r="J55">
+      <c r="F55" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G55" t="s">
+        <v>251</v>
+      </c>
+      <c r="J55" t="s">
+        <v>64</v>
+      </c>
+      <c r="K55" t="s">
+        <v>221</v>
+      </c>
+      <c r="L55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:12">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -3291,17 +3659,23 @@
       <c r="E56" t="s">
         <v>2</v>
       </c>
-      <c r="F56" t="s">
-        <v>253</v>
-      </c>
-      <c r="I56" t="s">
-        <v>222</v>
+      <c r="F56" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G56" t="s">
+        <v>251</v>
       </c>
       <c r="J56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>62</v>
+      </c>
+      <c r="K56" t="s">
+        <v>220</v>
+      </c>
+      <c r="L56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3314,14 +3688,17 @@
       <c r="E57" t="s">
         <v>4</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G57" t="s">
         <v>129</v>
       </c>
-      <c r="J57">
+      <c r="L57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
@@ -3331,14 +3708,20 @@
       <c r="E58" t="s">
         <v>2</v>
       </c>
-      <c r="F58" t="s">
-        <v>253</v>
-      </c>
-      <c r="J58">
+      <c r="F58" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G58" t="s">
+        <v>251</v>
+      </c>
+      <c r="J58" t="s">
+        <v>67</v>
+      </c>
+      <c r="L58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>69</v>
       </c>
@@ -3348,14 +3731,20 @@
       <c r="E59" t="s">
         <v>4</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G59" t="s">
         <v>129</v>
       </c>
-      <c r="J59">
+      <c r="K59" t="s">
+        <v>280</v>
+      </c>
+      <c r="L59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -3366,16 +3755,19 @@
         <v>2</v>
       </c>
       <c r="F60" t="s">
+        <v>277</v>
+      </c>
+      <c r="G60" t="s">
         <v>129</v>
       </c>
-      <c r="I60" t="s">
+      <c r="K60" t="s">
         <v>125</v>
       </c>
-      <c r="J60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="L60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" s="1" t="s">
         <v>132</v>
       </c>
@@ -3389,16 +3781,22 @@
         <v>4</v>
       </c>
       <c r="F61" t="s">
+        <v>277</v>
+      </c>
+      <c r="G61" t="s">
         <v>127</v>
       </c>
-      <c r="I61" t="s">
-        <v>225</v>
-      </c>
-      <c r="J61">
+      <c r="J61" t="s">
+        <v>265</v>
+      </c>
+      <c r="K61" t="s">
+        <v>223</v>
+      </c>
+      <c r="L61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -3411,14 +3809,17 @@
       <c r="E62" t="s">
         <v>4</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G62" t="s">
         <v>129</v>
       </c>
-      <c r="J62">
+      <c r="L62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>73</v>
       </c>
@@ -3431,17 +3832,20 @@
       <c r="E63" t="s">
         <v>4</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G63" t="s">
         <v>129</v>
       </c>
-      <c r="I63" t="s">
-        <v>203</v>
-      </c>
-      <c r="J63" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="K63" t="s">
+        <v>202</v>
+      </c>
+      <c r="L63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
         <v>74</v>
       </c>
@@ -3451,17 +3855,23 @@
       <c r="E64" t="s">
         <v>2</v>
       </c>
-      <c r="F64" t="s">
-        <v>253</v>
-      </c>
-      <c r="I64" t="s">
-        <v>226</v>
+      <c r="F64" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G64" t="s">
+        <v>251</v>
       </c>
       <c r="J64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>73</v>
+      </c>
+      <c r="K64" t="s">
+        <v>224</v>
+      </c>
+      <c r="L64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="1" t="s">
         <v>75</v>
       </c>
@@ -3469,22 +3879,28 @@
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E65" t="s">
         <v>9</v>
       </c>
-      <c r="F65" t="s">
-        <v>253</v>
-      </c>
-      <c r="I65" t="s">
-        <v>227</v>
+      <c r="F65" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G65" t="s">
+        <v>251</v>
       </c>
       <c r="J65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <v>198</v>
+      </c>
+      <c r="K65" t="s">
+        <v>225</v>
+      </c>
+      <c r="L65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -3494,14 +3910,17 @@
       <c r="E66" t="s">
         <v>2</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G66" t="s">
         <v>129</v>
       </c>
-      <c r="J66">
+      <c r="L66">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
         <v>130</v>
       </c>
@@ -3514,17 +3933,23 @@
       <c r="E67" t="s">
         <v>4</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G67" t="s">
         <v>127</v>
       </c>
-      <c r="I67" t="s">
-        <v>229</v>
-      </c>
-      <c r="J67">
+      <c r="J67" t="s">
+        <v>266</v>
+      </c>
+      <c r="K67" t="s">
+        <v>227</v>
+      </c>
+      <c r="L67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:12">
       <c r="A68" s="1" t="s">
         <v>78</v>
       </c>
@@ -3537,14 +3962,20 @@
       <c r="E68" t="s">
         <v>4</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G68" t="s">
         <v>127</v>
       </c>
-      <c r="J68">
+      <c r="J68" t="s">
+        <v>267</v>
+      </c>
+      <c r="L68">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -3557,14 +3988,17 @@
       <c r="E69" t="s">
         <v>4</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G69" t="s">
         <v>129</v>
       </c>
-      <c r="J69">
+      <c r="L69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
         <v>80</v>
       </c>
@@ -3574,17 +4008,23 @@
       <c r="E70" t="s">
         <v>2</v>
       </c>
-      <c r="F70" t="s">
-        <v>253</v>
-      </c>
-      <c r="I70" t="s">
-        <v>230</v>
-      </c>
-      <c r="J70">
+      <c r="F70" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G70" t="s">
+        <v>251</v>
+      </c>
+      <c r="J70" t="s">
+        <v>79</v>
+      </c>
+      <c r="K70" t="s">
+        <v>228</v>
+      </c>
+      <c r="L70">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -3594,14 +4034,17 @@
       <c r="E71" t="s">
         <v>4</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G71" t="s">
         <v>129</v>
       </c>
-      <c r="J71">
+      <c r="L71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
         <v>82</v>
       </c>
@@ -3611,14 +4054,20 @@
       <c r="E72" t="s">
         <v>2</v>
       </c>
-      <c r="F72" t="s">
-        <v>253</v>
-      </c>
-      <c r="J72">
+      <c r="F72" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G72" t="s">
+        <v>251</v>
+      </c>
+      <c r="J72" t="s">
+        <v>81</v>
+      </c>
+      <c r="L72">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:12">
       <c r="A73" s="1" t="s">
         <v>83</v>
       </c>
@@ -3631,14 +4080,20 @@
       <c r="E73" t="s">
         <v>84</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G73" t="s">
         <v>127</v>
       </c>
       <c r="J73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
+        <v>268</v>
+      </c>
+      <c r="L73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="1" t="s">
         <v>85</v>
       </c>
@@ -3648,17 +4103,23 @@
       <c r="E74" t="s">
         <v>86</v>
       </c>
-      <c r="F74" t="s">
-        <v>253</v>
-      </c>
-      <c r="I74" t="s">
-        <v>214</v>
+      <c r="F74" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G74" t="s">
+        <v>251</v>
       </c>
       <c r="J74" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
+        <v>39</v>
+      </c>
+      <c r="K74" t="s">
+        <v>212</v>
+      </c>
+      <c r="L74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -3668,14 +4129,17 @@
       <c r="E75" t="s">
         <v>4</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G75" t="s">
         <v>129</v>
       </c>
-      <c r="J75">
+      <c r="L75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:12">
       <c r="A76" s="1" t="s">
         <v>88</v>
       </c>
@@ -3685,17 +4149,23 @@
       <c r="E76" t="s">
         <v>2</v>
       </c>
-      <c r="F76" t="s">
-        <v>253</v>
-      </c>
-      <c r="I76" t="s">
-        <v>231</v>
-      </c>
-      <c r="J76">
+      <c r="F76" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G76" t="s">
+        <v>251</v>
+      </c>
+      <c r="J76" t="s">
+        <v>87</v>
+      </c>
+      <c r="K76" t="s">
+        <v>229</v>
+      </c>
+      <c r="L76">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:12">
       <c r="A77" s="1" t="s">
         <v>89</v>
       </c>
@@ -3709,19 +4179,22 @@
         <v>25</v>
       </c>
       <c r="F77" t="s">
+        <v>278</v>
+      </c>
+      <c r="G77" t="s">
         <v>129</v>
       </c>
-      <c r="G77" t="s">
-        <v>5</v>
-      </c>
-      <c r="I77" t="s">
+      <c r="H77" t="s">
+        <v>5</v>
+      </c>
+      <c r="K77" t="s">
         <v>91</v>
       </c>
-      <c r="J77" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
+      <c r="L77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>92</v>
       </c>
@@ -3729,19 +4202,25 @@
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E78" t="s">
         <v>4</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G78" t="s">
         <v>129</v>
       </c>
-      <c r="J78">
+      <c r="K78" t="s">
+        <v>280</v>
+      </c>
+      <c r="L78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:12">
       <c r="A79" s="1" t="s">
         <v>93</v>
       </c>
@@ -3754,14 +4233,20 @@
       <c r="E79" t="s">
         <v>4</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G79" t="s">
         <v>127</v>
       </c>
       <c r="J79" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+        <v>269</v>
+      </c>
+      <c r="L79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>94</v>
       </c>
@@ -3771,14 +4256,17 @@
       <c r="E80" t="s">
         <v>4</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G80" t="s">
         <v>129</v>
       </c>
-      <c r="J80">
+      <c r="L80">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:12">
       <c r="A81" s="1" t="s">
         <v>95</v>
       </c>
@@ -3788,17 +4276,23 @@
       <c r="E81" t="s">
         <v>2</v>
       </c>
-      <c r="F81" t="s">
-        <v>253</v>
-      </c>
-      <c r="I81" t="s">
-        <v>232</v>
-      </c>
-      <c r="J81">
+      <c r="F81" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G81" t="s">
+        <v>251</v>
+      </c>
+      <c r="J81" t="s">
+        <v>94</v>
+      </c>
+      <c r="K81" t="s">
+        <v>230</v>
+      </c>
+      <c r="L81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:12">
       <c r="A82" s="1" t="s">
         <v>2</v>
       </c>
@@ -3811,20 +4305,26 @@
       <c r="E82" t="s">
         <v>2</v>
       </c>
-      <c r="F82" t="s">
-        <v>253</v>
+      <c r="F82" s="3" t="s">
+        <v>277</v>
       </c>
       <c r="G82" t="s">
-        <v>5</v>
-      </c>
-      <c r="I82" t="s">
-        <v>233</v>
+        <v>251</v>
+      </c>
+      <c r="H82" t="s">
+        <v>5</v>
       </c>
       <c r="J82" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+        <v>281</v>
+      </c>
+      <c r="K82" t="s">
+        <v>231</v>
+      </c>
+      <c r="L82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" s="1" t="s">
         <v>96</v>
       </c>
@@ -3840,17 +4340,20 @@
       <c r="E83" t="s">
         <v>4</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G83" t="s">
         <v>129</v>
       </c>
-      <c r="G83" t="s">
-        <v>5</v>
-      </c>
-      <c r="J83" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+      <c r="H83" t="s">
+        <v>5</v>
+      </c>
+      <c r="L83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" s="1" t="s">
         <v>97</v>
       </c>
@@ -3860,17 +4363,23 @@
       <c r="E84" t="s">
         <v>4</v>
       </c>
-      <c r="F84" t="s">
-        <v>253</v>
-      </c>
-      <c r="I84" t="s">
-        <v>234</v>
+      <c r="F84" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G84" t="s">
+        <v>251</v>
       </c>
       <c r="J84" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+        <v>96</v>
+      </c>
+      <c r="K84" t="s">
+        <v>232</v>
+      </c>
+      <c r="L84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" s="1" t="s">
         <v>98</v>
       </c>
@@ -3880,17 +4389,23 @@
       <c r="E85" t="s">
         <v>4</v>
       </c>
-      <c r="F85" t="s">
-        <v>253</v>
-      </c>
-      <c r="I85" t="s">
-        <v>234</v>
+      <c r="F85" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G85" t="s">
+        <v>251</v>
       </c>
       <c r="J85" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
+        <v>96</v>
+      </c>
+      <c r="K85" t="s">
+        <v>232</v>
+      </c>
+      <c r="L85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -3903,14 +4418,17 @@
       <c r="E86" t="s">
         <v>4</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G86" t="s">
         <v>129</v>
       </c>
-      <c r="J86">
+      <c r="L86">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:12">
       <c r="A87" s="1" t="s">
         <v>100</v>
       </c>
@@ -3920,17 +4438,23 @@
       <c r="E87" t="s">
         <v>2</v>
       </c>
-      <c r="F87" t="s">
-        <v>253</v>
-      </c>
-      <c r="I87" t="s">
-        <v>235</v>
-      </c>
-      <c r="J87">
+      <c r="F87" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G87" t="s">
+        <v>251</v>
+      </c>
+      <c r="J87" t="s">
+        <v>99</v>
+      </c>
+      <c r="K87" t="s">
+        <v>233</v>
+      </c>
+      <c r="L87">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:12">
       <c r="A88" s="1" t="s">
         <v>101</v>
       </c>
@@ -3943,17 +4467,23 @@
       <c r="E88" t="s">
         <v>9</v>
       </c>
-      <c r="F88" t="s">
-        <v>253</v>
-      </c>
-      <c r="I88" t="s">
-        <v>237</v>
+      <c r="F88" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G88" t="s">
+        <v>251</v>
       </c>
       <c r="J88" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
+        <v>157</v>
+      </c>
+      <c r="K88" t="s">
+        <v>235</v>
+      </c>
+      <c r="L88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" s="1" t="s">
         <v>102</v>
       </c>
@@ -3963,17 +4493,20 @@
       <c r="E89" t="s">
         <v>4</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G89" t="s">
         <v>129</v>
       </c>
-      <c r="I89" t="s">
-        <v>247</v>
-      </c>
-      <c r="J89" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
+      <c r="K89" t="s">
+        <v>245</v>
+      </c>
+      <c r="L89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="1" t="s">
         <v>103</v>
       </c>
@@ -3987,165 +4520,268 @@
         <v>25</v>
       </c>
       <c r="F90" t="s">
+        <v>278</v>
+      </c>
+      <c r="G90" t="s">
         <v>129</v>
       </c>
-      <c r="G90" t="s">
-        <v>5</v>
-      </c>
-      <c r="I90" t="s">
+      <c r="H90" t="s">
+        <v>5</v>
+      </c>
+      <c r="K90" t="s">
         <v>106</v>
       </c>
-      <c r="J90" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
+      <c r="L90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F91" t="s">
+      <c r="E91" t="s">
+        <v>4</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G91" t="s">
         <v>127</v>
       </c>
-      <c r="I91" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+      <c r="J91" t="s">
+        <v>270</v>
+      </c>
+      <c r="K91" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="1" t="s">
         <v>184</v>
       </c>
+      <c r="E92" t="s">
+        <v>4</v>
+      </c>
       <c r="F92" t="s">
+        <v>277</v>
+      </c>
+      <c r="G92" t="s">
         <v>127</v>
       </c>
-      <c r="I92" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
+      <c r="J92" t="s">
+        <v>271</v>
+      </c>
+      <c r="K92" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="E93" t="s">
+        <v>4</v>
+      </c>
       <c r="F93" t="s">
-        <v>127</v>
-      </c>
-      <c r="I93" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
+        <v>277</v>
+      </c>
+      <c r="G93" t="s">
+        <v>234</v>
+      </c>
+      <c r="J93" t="s">
+        <v>282</v>
+      </c>
+      <c r="K93" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F94" t="s">
-        <v>236</v>
-      </c>
-      <c r="I94" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
+      <c r="E94" t="s">
+        <v>4</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G94" t="s">
+        <v>234</v>
+      </c>
+      <c r="J94" t="s">
+        <v>283</v>
+      </c>
+      <c r="K94" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="30">
       <c r="A95" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="E95" t="s">
+        <v>4</v>
       </c>
       <c r="F95" t="s">
-        <v>236</v>
-      </c>
-      <c r="I95" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
+        <v>277</v>
+      </c>
+      <c r="G95" t="s">
+        <v>127</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="K95" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="30">
       <c r="A96" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="E96" t="s">
+        <v>4</v>
+      </c>
       <c r="F96" t="s">
+        <v>277</v>
+      </c>
+      <c r="G96" t="s">
         <v>127</v>
       </c>
-      <c r="I96" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="45">
       <c r="A97" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="E97" t="s">
+        <v>4</v>
+      </c>
       <c r="F97" t="s">
+        <v>277</v>
+      </c>
+      <c r="G97" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="J97" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="30">
       <c r="A98" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="E98" t="s">
+        <v>4</v>
+      </c>
       <c r="F98" t="s">
+        <v>277</v>
+      </c>
+      <c r="G98" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="J98" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="30">
       <c r="A99" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="E99" t="s">
+        <v>279</v>
+      </c>
       <c r="F99" t="s">
+        <v>278</v>
+      </c>
+      <c r="G99" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="1" t="s">
+      <c r="J99" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="K99" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" t="s">
+        <v>195</v>
+      </c>
+      <c r="E100" t="s">
+        <v>4</v>
+      </c>
+      <c r="F100" t="s">
+        <v>277</v>
+      </c>
+      <c r="G100" t="s">
+        <v>129</v>
+      </c>
+      <c r="K100" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" t="s">
         <v>193</v>
       </c>
-      <c r="F100" t="s">
-        <v>127</v>
-      </c>
-      <c r="I100" t="s">
+      <c r="E101" t="s">
+        <v>4</v>
+      </c>
+      <c r="F101" t="s">
+        <v>277</v>
+      </c>
+      <c r="G101" t="s">
+        <v>129</v>
+      </c>
+      <c r="K101" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
-      <c r="A101" t="s">
-        <v>196</v>
-      </c>
-      <c r="F101" t="s">
-        <v>129</v>
-      </c>
-      <c r="I101" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:11">
       <c r="A102" t="s">
         <v>194</v>
       </c>
+      <c r="E102" t="s">
+        <v>4</v>
+      </c>
       <c r="F102" t="s">
+        <v>277</v>
+      </c>
+      <c r="G102" t="s">
         <v>129</v>
       </c>
-      <c r="I102" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="K102" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>197</v>
+      </c>
+      <c r="E103" t="s">
+        <v>4</v>
       </c>
       <c r="F103" t="s">
+        <v>277</v>
+      </c>
+      <c r="G103" t="s">
         <v>129</v>
       </c>
-      <c r="I103" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>196</v>
+      </c>
+      <c r="E104" t="s">
+        <v>4</v>
       </c>
       <c r="F104" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
-      <c r="A105" t="s">
-        <v>197</v>
-      </c>
-      <c r="F105" t="s">
+        <v>277</v>
+      </c>
+      <c r="G104" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4166,10 +4802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:XFD93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4216,7 +4852,7 @@
         <v>167</v>
       </c>
       <c r="D3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4271,10 +4907,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4307,12 +4943,12 @@
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4751,7 +5387,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -4776,12 +5412,12 @@
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:1">
@@ -4790,18 +5426,13 @@
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>195</v>
+      <c r="A103" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4817,10 +5448,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:A105"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:XFD93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4936,7 +5567,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5408,7 +6039,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -5433,12 +6064,12 @@
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:1">
@@ -5447,18 +6078,13 @@
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>195</v>
+      <c r="A103" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -5474,10 +6100,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:A105"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:XFD93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5583,7 +6209,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5986,7 +6612,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -6011,12 +6637,12 @@
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:1">
@@ -6025,18 +6651,13 @@
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>195</v>
+      <c r="A103" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated mutability section in system metadata description.
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1083,7 +1083,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="410">
+  <cellStyleXfs count="411">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1485,6 +1485,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1504,7 +1505,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="410">
+  <cellStyles count="411">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1716,6 +1717,7 @@
     <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1916,7 +1918,78 @@
     <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -2246,10 +2319,10 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C96" sqref="C96"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2303,7 +2376,7 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -2329,7 +2402,7 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -2361,7 +2434,7 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
@@ -2387,7 +2460,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
@@ -2416,7 +2489,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>133</v>
       </c>
       <c r="C6" t="s">
@@ -2465,7 +2538,7 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
@@ -2491,7 +2564,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
@@ -2517,7 +2590,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
@@ -2540,7 +2613,7 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2566,7 +2639,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
@@ -2580,6 +2653,10 @@
       </c>
       <c r="G12" t="s">
         <v>251</v>
+      </c>
+      <c r="I12">
+        <f>IF(G12="C",1,0)</f>
+        <v>1</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
@@ -2615,7 +2692,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2647,7 +2724,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>157</v>
       </c>
       <c r="C15" t="s">
@@ -2667,7 +2744,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>182</v>
       </c>
       <c r="C16" t="s">
@@ -2722,7 +2799,7 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>187</v>
       </c>
       <c r="C18" t="s">
@@ -2751,7 +2828,7 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>135</v>
       </c>
       <c r="C19" t="s">
@@ -2806,7 +2883,7 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="C21" t="s">
@@ -2832,7 +2909,7 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="C22" t="s">
@@ -2881,7 +2958,7 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="C24" t="s">
@@ -3062,7 +3139,7 @@
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="C32" t="s">
@@ -3091,7 +3168,7 @@
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>40</v>
       </c>
       <c r="C33" t="s">
@@ -3160,7 +3237,7 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
       <c r="C36" t="s">
@@ -3206,7 +3283,7 @@
       </c>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3238,7 +3315,7 @@
       </c>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>48</v>
       </c>
       <c r="C39" t="s">
@@ -3324,7 +3401,7 @@
       </c>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>52</v>
       </c>
       <c r="C43" t="s">
@@ -3399,7 +3476,7 @@
       </c>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>55</v>
       </c>
       <c r="C46" t="s">
@@ -3428,7 +3505,7 @@
       </c>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>131</v>
       </c>
       <c r="C47" t="s">
@@ -3457,7 +3534,7 @@
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>57</v>
       </c>
       <c r="C48" t="s">
@@ -3483,7 +3560,7 @@
       </c>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>181</v>
       </c>
       <c r="C49" t="s">
@@ -3509,7 +3586,7 @@
       </c>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>59</v>
       </c>
       <c r="C50" t="s">
@@ -3624,7 +3701,7 @@
       </c>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>65</v>
       </c>
       <c r="C55" t="s">
@@ -3650,7 +3727,7 @@
       </c>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>66</v>
       </c>
       <c r="C56" t="s">
@@ -3699,7 +3776,7 @@
       </c>
     </row>
     <row r="58" spans="1:12">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>68</v>
       </c>
       <c r="C58" t="s">
@@ -3768,7 +3845,7 @@
       </c>
     </row>
     <row r="61" spans="1:12">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>132</v>
       </c>
       <c r="C61" t="s">
@@ -3846,7 +3923,7 @@
       </c>
     </row>
     <row r="64" spans="1:12">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>74</v>
       </c>
       <c r="C64" t="s">
@@ -3872,7 +3949,7 @@
       </c>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>75</v>
       </c>
       <c r="C65" t="s">
@@ -3921,7 +3998,7 @@
       </c>
     </row>
     <row r="67" spans="1:12">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>130</v>
       </c>
       <c r="C67" t="s">
@@ -3950,7 +4027,7 @@
       </c>
     </row>
     <row r="68" spans="1:12">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>78</v>
       </c>
       <c r="C68" t="s">
@@ -3999,7 +4076,7 @@
       </c>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>80</v>
       </c>
       <c r="C70" t="s">
@@ -4045,7 +4122,7 @@
       </c>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>82</v>
       </c>
       <c r="C72" t="s">
@@ -4068,7 +4145,7 @@
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>83</v>
       </c>
       <c r="C73" t="s">
@@ -4094,7 +4171,7 @@
       </c>
     </row>
     <row r="74" spans="1:12">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>85</v>
       </c>
       <c r="C74" t="s">
@@ -4140,7 +4217,7 @@
       </c>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>88</v>
       </c>
       <c r="C76" t="s">
@@ -4166,7 +4243,7 @@
       </c>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>89</v>
       </c>
       <c r="C77" t="s">
@@ -4221,7 +4298,7 @@
       </c>
     </row>
     <row r="79" spans="1:12">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>93</v>
       </c>
       <c r="C79" t="s">
@@ -4267,7 +4344,7 @@
       </c>
     </row>
     <row r="81" spans="1:12">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>95</v>
       </c>
       <c r="C81" t="s">
@@ -4293,7 +4370,7 @@
       </c>
     </row>
     <row r="82" spans="1:12">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>2</v>
       </c>
       <c r="C82" t="s">
@@ -4325,7 +4402,7 @@
       </c>
     </row>
     <row r="83" spans="1:12">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>96</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -4354,7 +4431,7 @@
       </c>
     </row>
     <row r="84" spans="1:12">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>97</v>
       </c>
       <c r="C84" t="s">
@@ -4380,7 +4457,7 @@
       </c>
     </row>
     <row r="85" spans="1:12">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>98</v>
       </c>
       <c r="C85" t="s">
@@ -4429,7 +4506,7 @@
       </c>
     </row>
     <row r="87" spans="1:12">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>100</v>
       </c>
       <c r="C87" t="s">
@@ -4455,7 +4532,7 @@
       </c>
     </row>
     <row r="88" spans="1:12">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>101</v>
       </c>
       <c r="C88" t="s">
@@ -4484,7 +4561,7 @@
       </c>
     </row>
     <row r="89" spans="1:12">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>102</v>
       </c>
       <c r="C89" t="s">
@@ -4507,7 +4584,7 @@
       </c>
     </row>
     <row r="90" spans="1:12">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>103</v>
       </c>
       <c r="C90" t="s">
@@ -4536,7 +4613,7 @@
       </c>
     </row>
     <row r="91" spans="1:12">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>183</v>
       </c>
       <c r="E91" t="s">
@@ -4556,7 +4633,7 @@
       </c>
     </row>
     <row r="92" spans="1:12">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>184</v>
       </c>
       <c r="E92" t="s">
@@ -4576,7 +4653,7 @@
       </c>
     </row>
     <row r="93" spans="1:12">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>185</v>
       </c>
       <c r="E93" t="s">
@@ -4596,7 +4673,7 @@
       </c>
     </row>
     <row r="94" spans="1:12">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>186</v>
       </c>
       <c r="E94" t="s">
@@ -4616,7 +4693,7 @@
       </c>
     </row>
     <row r="95" spans="1:12" ht="30">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>188</v>
       </c>
       <c r="E95" t="s">
@@ -4636,7 +4713,7 @@
       </c>
     </row>
     <row r="96" spans="1:12" ht="30">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>189</v>
       </c>
       <c r="E96" t="s">
@@ -4653,7 +4730,7 @@
       </c>
     </row>
     <row r="97" spans="1:11" ht="45">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>190</v>
       </c>
       <c r="E97" t="s">
@@ -4670,7 +4747,7 @@
       </c>
     </row>
     <row r="98" spans="1:11" ht="30">
-      <c r="A98" s="1" t="s">
+      <c r="A98" t="s">
         <v>191</v>
       </c>
       <c r="E98" t="s">
@@ -4687,7 +4764,7 @@
       </c>
     </row>
     <row r="99" spans="1:11" ht="30">
-      <c r="A99" s="1" t="s">
+      <c r="A99" t="s">
         <v>192</v>
       </c>
       <c r="E99" t="s">
@@ -4789,6 +4866,14 @@
   <sortState ref="C2:C94">
     <sortCondition ref="C2:C94"/>
   </sortState>
+  <conditionalFormatting sqref="A2:A104">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>IF(G2="C",1,0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>IF($G2="Y",1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Altering ping() response as described in discussion today.
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="0" windowWidth="30540" windowHeight="25420" tabRatio="500"/>
+    <workbookView xWindow="15840" yWindow="40" windowWidth="30540" windowHeight="25420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
-    <sheet name="EML" sheetId="3" r:id="rId2"/>
-    <sheet name="FGDC" sheetId="4" r:id="rId3"/>
-    <sheet name="Dryad" sheetId="5" r:id="rId4"/>
+    <sheet name="SystemMetadata" sheetId="6" r:id="rId2"/>
+    <sheet name="EML" sheetId="3" r:id="rId3"/>
+    <sheet name="FGDC" sheetId="4" r:id="rId4"/>
+    <sheet name="Dryad" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$L$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$N$102</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -55,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="289">
   <si>
     <t>Notes</t>
   </si>
@@ -995,6 +996,15 @@
   </si>
   <si>
     <t>Lists all PIDs that describe this object. Obtained by parsing all resource maps in which this object is referenced.</t>
+  </si>
+  <si>
+    <t>HGConfirmed</t>
+  </si>
+  <si>
+    <t>ds_id</t>
+  </si>
+  <si>
+    <t>D1Sys</t>
   </si>
 </sst>
 </file>
@@ -1918,7 +1928,7 @@
     <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1951,41 +1961,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2316,2562 +2296,2712 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:N105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" customWidth="1"/>
-    <col min="10" max="10" width="57" customWidth="1"/>
-    <col min="11" max="11" width="42.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+    <col min="12" max="12" width="57" customWidth="1"/>
+    <col min="13" max="13" width="42.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>158</v>
       </c>
       <c r="B1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" t="s">
         <v>242</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>240</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>239</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>159</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>252</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>177</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>176</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>178</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>253</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>278</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>129</v>
       </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>278</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>129</v>
       </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
         <v>222</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>277</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>129</v>
       </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>278</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>129</v>
       </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="N5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
         <v>133</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>277</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>127</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>254</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>211</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
       <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>277</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>129</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>278</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>127</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>255</v>
       </c>
-      <c r="L8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="N8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>278</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>127</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>256</v>
       </c>
-      <c r="L9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="N9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
       <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>277</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>129</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>280</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
         <v>197</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>278</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>129</v>
       </c>
-      <c r="L11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="N11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
       <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>278</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>251</v>
       </c>
-      <c r="I12">
-        <f>IF(G12="C",1,0)</f>
+      <c r="K12">
+        <f>IF(I12="C",1,0)</f>
         <v>1</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>17</v>
       </c>
-      <c r="L12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="N12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>19</v>
       </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>278</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>127</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>257</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>134</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
         <v>156</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>127</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>258</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>237</v>
       </c>
-      <c r="L14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="N14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>157</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>127</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>182</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
         <v>182</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>127</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>258</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>213</v>
       </c>
-      <c r="L16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="N16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" t="s">
         <v>243</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
       <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>129</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>250</v>
       </c>
-      <c r="L17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="N17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>187</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
         <v>187</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>234</v>
       </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
         <v>285</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>214</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>135</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
         <v>135</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>234</v>
       </c>
-      <c r="J19" t="s">
+      <c r="L19" t="s">
         <v>284</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>215</v>
       </c>
-      <c r="L19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="N19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>5</v>
       </c>
       <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>129</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>199</v>
       </c>
-      <c r="L20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="N20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
       <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>251</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>226</v>
       </c>
-      <c r="L21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="N21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
         <v>24</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>129</v>
       </c>
-      <c r="H22" t="s">
-        <v>5</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="J22" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" t="s">
         <v>27</v>
       </c>
-      <c r="L22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="N22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
       <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>129</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
         <v>29</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>129</v>
       </c>
-      <c r="H24" t="s">
-        <v>5</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="J24" t="s">
+        <v>5</v>
+      </c>
+      <c r="M24" t="s">
         <v>31</v>
       </c>
-      <c r="L24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="N24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
       <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>129</v>
       </c>
-      <c r="K25" t="s">
+      <c r="M25" t="s">
         <v>280</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
       <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>129</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>216</v>
       </c>
-      <c r="L26">
+      <c r="N26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
       <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G27" t="s">
+      <c r="I27" t="s">
         <v>129</v>
       </c>
-      <c r="L27">
+      <c r="N27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>35</v>
       </c>
-      <c r="C28" t="s">
-        <v>5</v>
+      <c r="B28" t="s">
+        <v>127</v>
       </c>
       <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>129</v>
       </c>
-      <c r="L28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="N28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>36</v>
       </c>
-      <c r="C29" t="s">
-        <v>5</v>
+      <c r="B29" t="s">
+        <v>127</v>
       </c>
       <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G29" t="s">
+      <c r="I29" t="s">
         <v>129</v>
       </c>
-      <c r="L29">
+      <c r="N29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>37</v>
       </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
       <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G30" t="s">
+      <c r="I30" t="s">
         <v>129</v>
       </c>
-      <c r="K30" t="s">
+      <c r="M30" t="s">
         <v>280</v>
       </c>
-      <c r="L30">
+      <c r="N30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
       <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G31" t="s">
+      <c r="I31" t="s">
         <v>129</v>
       </c>
-      <c r="K31" t="s">
+      <c r="M31" t="s">
         <v>138</v>
       </c>
-      <c r="L31">
+      <c r="N31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
         <v>41</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G32" t="s">
+      <c r="I32" t="s">
         <v>127</v>
       </c>
-      <c r="J32" t="s">
+      <c r="L32" t="s">
         <v>260</v>
       </c>
-      <c r="K32" t="s">
+      <c r="M32" t="s">
         <v>236</v>
       </c>
-      <c r="L32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="N32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>40</v>
       </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
       <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G33" t="s">
+      <c r="I33" t="s">
         <v>251</v>
       </c>
-      <c r="J33" t="s">
+      <c r="L33" t="s">
         <v>39</v>
       </c>
-      <c r="K33" t="s">
+      <c r="M33" t="s">
         <v>217</v>
       </c>
-      <c r="L33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="N33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>42</v>
       </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
       <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="H34" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G34" t="s">
+      <c r="I34" t="s">
         <v>129</v>
       </c>
-      <c r="L34">
+      <c r="N34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>43</v>
       </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
       <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
         <v>129</v>
       </c>
-      <c r="K35" t="s">
+      <c r="M35" t="s">
         <v>200</v>
       </c>
-      <c r="L35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="N35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>44</v>
       </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
       <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>251</v>
       </c>
-      <c r="J36" t="s">
+      <c r="L36" t="s">
         <v>43</v>
       </c>
-      <c r="L36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="N36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>45</v>
       </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
       <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G37" t="s">
+      <c r="I37" t="s">
         <v>129</v>
       </c>
-      <c r="K37" t="s">
+      <c r="M37" t="s">
         <v>244</v>
       </c>
-      <c r="L37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="N37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
         <v>46</v>
       </c>
-      <c r="E38" t="s">
+      <c r="G38" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G38" t="s">
+      <c r="I38" t="s">
         <v>129</v>
       </c>
-      <c r="H38" t="s">
-        <v>5</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="J38" t="s">
+        <v>5</v>
+      </c>
+      <c r="M38" t="s">
         <v>128</v>
       </c>
-      <c r="L38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="N38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>48</v>
       </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
       <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G39" t="s">
+      <c r="I39" t="s">
         <v>251</v>
       </c>
-      <c r="J39" t="s">
+      <c r="L39" t="s">
         <v>46</v>
       </c>
-      <c r="L39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="N39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>49</v>
       </c>
-      <c r="C40" t="s">
-        <v>5</v>
-      </c>
       <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G40" t="s">
+      <c r="I40" t="s">
         <v>129</v>
       </c>
-      <c r="K40" t="s">
+      <c r="M40" t="s">
         <v>280</v>
       </c>
-      <c r="L40">
+      <c r="N40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>50</v>
       </c>
-      <c r="C41" t="s">
-        <v>5</v>
+      <c r="B41" t="s">
+        <v>127</v>
       </c>
       <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G41" t="s">
+      <c r="I41" t="s">
         <v>129</v>
       </c>
-      <c r="L41">
+      <c r="N41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>51</v>
       </c>
-      <c r="C42" t="s">
-        <v>5</v>
-      </c>
       <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" t="s">
         <v>2</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G42" t="s">
+      <c r="I42" t="s">
         <v>129</v>
       </c>
-      <c r="L42">
+      <c r="N42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>52</v>
       </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" t="s">
         <v>52</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G43" t="s">
+      <c r="I43" t="s">
         <v>251</v>
       </c>
-      <c r="J43" t="s">
+      <c r="L43" t="s">
         <v>51</v>
       </c>
-      <c r="K43" t="s">
+      <c r="M43" t="s">
         <v>218</v>
       </c>
-      <c r="L43">
+      <c r="N43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>53</v>
       </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
       <c r="E44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" t="s">
         <v>2</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G44" t="s">
+      <c r="I44" t="s">
         <v>129</v>
       </c>
-      <c r="K44" t="s">
+      <c r="M44" t="s">
         <v>143</v>
       </c>
-      <c r="L44">
+      <c r="N44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
       <c r="E45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G45" t="s">
+      <c r="I45" t="s">
         <v>129</v>
       </c>
-      <c r="K45" t="s">
+      <c r="M45" t="s">
         <v>244</v>
       </c>
-      <c r="L45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="N45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>55</v>
       </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="B46" t="s">
+        <v>127</v>
+      </c>
+      <c r="E46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" t="s">
         <v>55</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46" t="s">
         <v>25</v>
       </c>
-      <c r="F46" t="s">
+      <c r="H46" t="s">
         <v>278</v>
       </c>
-      <c r="G46" t="s">
+      <c r="I46" t="s">
         <v>129</v>
       </c>
-      <c r="H46" t="s">
-        <v>5</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="J46" t="s">
+        <v>5</v>
+      </c>
+      <c r="M46" t="s">
         <v>144</v>
       </c>
-      <c r="L46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="N46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>131</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" t="s">
+        <v>127</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
         <v>131</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>4</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G47" t="s">
+      <c r="I47" t="s">
         <v>127</v>
       </c>
-      <c r="J47" t="s">
+      <c r="L47" t="s">
         <v>261</v>
       </c>
-      <c r="K47" t="s">
+      <c r="M47" t="s">
         <v>219</v>
       </c>
-      <c r="L47">
+      <c r="N47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
         <v>179</v>
       </c>
-      <c r="E48" t="s">
+      <c r="G48" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="H48" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G48" t="s">
+      <c r="I48" t="s">
         <v>127</v>
       </c>
-      <c r="J48" t="s">
+      <c r="L48" t="s">
         <v>262</v>
       </c>
-      <c r="L48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="N48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>181</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
+        <v>127</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
         <v>181</v>
       </c>
-      <c r="E49" t="s">
+      <c r="G49" t="s">
         <v>4</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G49" t="s">
+      <c r="I49" t="s">
         <v>127</v>
       </c>
-      <c r="J49" t="s">
+      <c r="L49" t="s">
         <v>263</v>
       </c>
-      <c r="L49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="N49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" t="s">
+        <v>127</v>
+      </c>
+      <c r="E50" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" t="s">
         <v>59</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>4</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G50" t="s">
+      <c r="I50" t="s">
         <v>127</v>
       </c>
-      <c r="J50" t="s">
+      <c r="L50" t="s">
         <v>264</v>
       </c>
-      <c r="L50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="N50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>60</v>
       </c>
-      <c r="C51" t="s">
-        <v>5</v>
+      <c r="B51" t="s">
+        <v>127</v>
       </c>
       <c r="E51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" t="s">
         <v>2</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="H51" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G51" t="s">
+      <c r="I51" t="s">
         <v>129</v>
       </c>
-      <c r="L51">
+      <c r="N51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>61</v>
       </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
       <c r="E52" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
         <v>4</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="H52" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G52" t="s">
+      <c r="I52" t="s">
         <v>129</v>
       </c>
-      <c r="K52" t="s">
+      <c r="M52" t="s">
         <v>280</v>
       </c>
-      <c r="L52">
+      <c r="N52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>62</v>
       </c>
-      <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>5</v>
       </c>
       <c r="E53" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" t="s">
         <v>4</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G53" t="s">
+      <c r="I53" t="s">
         <v>129</v>
       </c>
-      <c r="K53" t="s">
+      <c r="M53" t="s">
         <v>201</v>
       </c>
-      <c r="L53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="N53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>64</v>
       </c>
-      <c r="C54" t="s">
-        <v>5</v>
+      <c r="B54" t="s">
+        <v>127</v>
       </c>
       <c r="E54" t="s">
+        <v>5</v>
+      </c>
+      <c r="G54" t="s">
         <v>4</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="H54" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G54" t="s">
+      <c r="I54" t="s">
         <v>129</v>
       </c>
-      <c r="L54">
+      <c r="N54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>65</v>
       </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
       <c r="E55" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" t="s">
         <v>2</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="H55" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G55" t="s">
+      <c r="I55" t="s">
         <v>251</v>
       </c>
-      <c r="J55" t="s">
+      <c r="L55" t="s">
         <v>64</v>
       </c>
-      <c r="K55" t="s">
+      <c r="M55" t="s">
         <v>221</v>
       </c>
-      <c r="L55">
+      <c r="N55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>66</v>
       </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
       <c r="E56" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" t="s">
         <v>2</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="H56" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G56" t="s">
+      <c r="I56" t="s">
         <v>251</v>
       </c>
-      <c r="J56" t="s">
+      <c r="L56" t="s">
         <v>62</v>
       </c>
-      <c r="K56" t="s">
+      <c r="M56" t="s">
         <v>220</v>
       </c>
-      <c r="L56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="N56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>67</v>
       </c>
-      <c r="B57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>5</v>
       </c>
       <c r="E57" t="s">
+        <v>5</v>
+      </c>
+      <c r="G57" t="s">
         <v>4</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="H57" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G57" t="s">
+      <c r="I57" t="s">
         <v>129</v>
       </c>
-      <c r="L57">
+      <c r="N57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>68</v>
       </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
       <c r="E58" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" t="s">
         <v>2</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G58" t="s">
+      <c r="I58" t="s">
         <v>251</v>
       </c>
-      <c r="J58" t="s">
+      <c r="L58" t="s">
         <v>67</v>
       </c>
-      <c r="L58">
+      <c r="N58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>69</v>
       </c>
-      <c r="C59" t="s">
-        <v>5</v>
-      </c>
       <c r="E59" t="s">
+        <v>5</v>
+      </c>
+      <c r="G59" t="s">
         <v>4</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="H59" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G59" t="s">
+      <c r="I59" t="s">
         <v>129</v>
       </c>
-      <c r="K59" t="s">
+      <c r="M59" t="s">
         <v>280</v>
       </c>
-      <c r="L59">
+      <c r="N59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>70</v>
       </c>
-      <c r="C60" t="s">
-        <v>5</v>
+      <c r="B60" t="s">
+        <v>127</v>
       </c>
       <c r="E60" t="s">
+        <v>5</v>
+      </c>
+      <c r="G60" t="s">
         <v>2</v>
       </c>
-      <c r="F60" t="s">
+      <c r="H60" t="s">
         <v>277</v>
       </c>
-      <c r="G60" t="s">
+      <c r="I60" t="s">
         <v>129</v>
       </c>
-      <c r="K60" t="s">
+      <c r="M60" t="s">
         <v>125</v>
       </c>
-      <c r="L60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="N60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>132</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E61" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E61" t="s">
+      <c r="G61" t="s">
         <v>4</v>
       </c>
-      <c r="F61" t="s">
+      <c r="H61" t="s">
         <v>277</v>
       </c>
-      <c r="G61" t="s">
+      <c r="I61" t="s">
         <v>127</v>
       </c>
-      <c r="J61" t="s">
+      <c r="L61" t="s">
         <v>265</v>
       </c>
-      <c r="K61" t="s">
+      <c r="M61" t="s">
         <v>223</v>
       </c>
-      <c r="L61">
+      <c r="N61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" t="s">
         <v>5</v>
       </c>
       <c r="E62" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" t="s">
         <v>4</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="H62" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G62" t="s">
+      <c r="I62" t="s">
         <v>129</v>
       </c>
-      <c r="L62">
+      <c r="N62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
         <v>73</v>
       </c>
-      <c r="B63" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>5</v>
       </c>
       <c r="E63" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="H63" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G63" t="s">
+      <c r="I63" t="s">
         <v>129</v>
       </c>
-      <c r="K63" t="s">
+      <c r="M63" t="s">
         <v>202</v>
       </c>
-      <c r="L63" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="N63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
         <v>74</v>
       </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
       <c r="E64" t="s">
+        <v>5</v>
+      </c>
+      <c r="G64" t="s">
         <v>2</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="H64" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G64" t="s">
+      <c r="I64" t="s">
         <v>251</v>
       </c>
-      <c r="J64" t="s">
+      <c r="L64" t="s">
         <v>73</v>
       </c>
-      <c r="K64" t="s">
+      <c r="M64" t="s">
         <v>224</v>
       </c>
-      <c r="L64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="N64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
         <v>75</v>
       </c>
-      <c r="C65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" t="s">
         <v>198</v>
       </c>
-      <c r="E65" t="s">
+      <c r="G65" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="H65" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G65" t="s">
+      <c r="I65" t="s">
         <v>251</v>
       </c>
-      <c r="J65" t="s">
+      <c r="L65" t="s">
         <v>198</v>
       </c>
-      <c r="K65" t="s">
+      <c r="M65" t="s">
         <v>225</v>
       </c>
-      <c r="L65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="N65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
         <v>77</v>
       </c>
-      <c r="C66" t="s">
-        <v>5</v>
+      <c r="B66" t="s">
+        <v>127</v>
       </c>
       <c r="E66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G66" t="s">
         <v>2</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G66" t="s">
+      <c r="I66" t="s">
         <v>129</v>
       </c>
-      <c r="L66">
+      <c r="N66">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
         <v>130</v>
       </c>
       <c r="C67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" t="s">
+        <v>127</v>
+      </c>
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" t="s">
         <v>130</v>
       </c>
-      <c r="E67" t="s">
+      <c r="G67" t="s">
         <v>4</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="H67" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G67" t="s">
+      <c r="I67" t="s">
         <v>127</v>
       </c>
-      <c r="J67" t="s">
+      <c r="L67" t="s">
         <v>266</v>
       </c>
-      <c r="K67" t="s">
+      <c r="M67" t="s">
         <v>227</v>
       </c>
-      <c r="L67">
+      <c r="N67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:14">
       <c r="A68" t="s">
         <v>78</v>
       </c>
       <c r="C68" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" t="s">
+        <v>127</v>
+      </c>
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68" t="s">
         <v>180</v>
       </c>
-      <c r="E68" t="s">
+      <c r="G68" t="s">
         <v>4</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="H68" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G68" t="s">
+      <c r="I68" t="s">
         <v>127</v>
       </c>
-      <c r="J68" t="s">
+      <c r="L68" t="s">
         <v>267</v>
       </c>
-      <c r="L68">
+      <c r="N68">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:14">
       <c r="A69" t="s">
         <v>79</v>
       </c>
-      <c r="B69" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>5</v>
       </c>
       <c r="E69" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69" t="s">
         <v>4</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="H69" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G69" t="s">
+      <c r="I69" t="s">
         <v>129</v>
       </c>
-      <c r="L69">
+      <c r="N69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:14">
       <c r="A70" t="s">
         <v>80</v>
       </c>
-      <c r="C70" t="s">
-        <v>5</v>
-      </c>
       <c r="E70" t="s">
+        <v>5</v>
+      </c>
+      <c r="G70" t="s">
         <v>2</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="H70" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G70" t="s">
+      <c r="I70" t="s">
         <v>251</v>
       </c>
-      <c r="J70" t="s">
+      <c r="L70" t="s">
         <v>79</v>
       </c>
-      <c r="K70" t="s">
+      <c r="M70" t="s">
         <v>228</v>
       </c>
-      <c r="L70">
+      <c r="N70">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:14">
       <c r="A71" t="s">
         <v>81</v>
       </c>
-      <c r="C71" t="s">
-        <v>5</v>
-      </c>
       <c r="E71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71" t="s">
         <v>4</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="H71" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G71" t="s">
+      <c r="I71" t="s">
         <v>129</v>
       </c>
-      <c r="L71">
+      <c r="N71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:14">
       <c r="A72" t="s">
         <v>82</v>
       </c>
-      <c r="C72" t="s">
-        <v>5</v>
-      </c>
       <c r="E72" t="s">
+        <v>5</v>
+      </c>
+      <c r="G72" t="s">
         <v>2</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="H72" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G72" t="s">
+      <c r="I72" t="s">
         <v>251</v>
       </c>
-      <c r="J72" t="s">
+      <c r="L72" t="s">
         <v>81</v>
       </c>
-      <c r="L72">
+      <c r="N72">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:14">
       <c r="A73" t="s">
         <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" t="s">
+        <v>127</v>
+      </c>
+      <c r="E73" t="s">
+        <v>5</v>
+      </c>
+      <c r="F73" t="s">
         <v>83</v>
       </c>
-      <c r="E73" t="s">
+      <c r="G73" t="s">
         <v>84</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="H73" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G73" t="s">
+      <c r="I73" t="s">
         <v>127</v>
       </c>
-      <c r="J73" t="s">
+      <c r="L73" t="s">
         <v>268</v>
       </c>
-      <c r="L73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="N73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" t="s">
         <v>85</v>
       </c>
-      <c r="C74" t="s">
-        <v>5</v>
-      </c>
       <c r="E74" t="s">
+        <v>5</v>
+      </c>
+      <c r="G74" t="s">
         <v>86</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="H74" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G74" t="s">
+      <c r="I74" t="s">
         <v>251</v>
       </c>
-      <c r="J74" t="s">
+      <c r="L74" t="s">
         <v>39</v>
       </c>
-      <c r="K74" t="s">
+      <c r="M74" t="s">
         <v>212</v>
       </c>
-      <c r="L74" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="N74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
       <c r="A75" t="s">
         <v>87</v>
       </c>
-      <c r="C75" t="s">
-        <v>5</v>
-      </c>
       <c r="E75" t="s">
+        <v>5</v>
+      </c>
+      <c r="G75" t="s">
         <v>4</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="H75" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G75" t="s">
+      <c r="I75" t="s">
         <v>129</v>
       </c>
-      <c r="L75">
+      <c r="N75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:14">
       <c r="A76" t="s">
         <v>88</v>
       </c>
-      <c r="C76" t="s">
-        <v>5</v>
-      </c>
       <c r="E76" t="s">
+        <v>5</v>
+      </c>
+      <c r="G76" t="s">
         <v>2</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="H76" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G76" t="s">
+      <c r="I76" t="s">
         <v>251</v>
       </c>
-      <c r="J76" t="s">
+      <c r="L76" t="s">
         <v>87</v>
       </c>
-      <c r="K76" t="s">
+      <c r="M76" t="s">
         <v>229</v>
       </c>
-      <c r="L76">
+      <c r="N76">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:14">
       <c r="A77" t="s">
         <v>89</v>
       </c>
-      <c r="C77" t="s">
-        <v>5</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="B77" t="s">
+        <v>127</v>
+      </c>
+      <c r="E77" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" t="s">
         <v>89</v>
       </c>
-      <c r="E77" t="s">
+      <c r="G77" t="s">
         <v>25</v>
       </c>
-      <c r="F77" t="s">
+      <c r="H77" t="s">
         <v>278</v>
       </c>
-      <c r="G77" t="s">
+      <c r="I77" t="s">
         <v>129</v>
       </c>
-      <c r="H77" t="s">
-        <v>5</v>
-      </c>
-      <c r="K77" t="s">
+      <c r="J77" t="s">
+        <v>5</v>
+      </c>
+      <c r="M77" t="s">
         <v>91</v>
       </c>
-      <c r="L77" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="N77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" t="s">
         <v>92</v>
       </c>
-      <c r="C78" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" t="s">
         <v>196</v>
       </c>
-      <c r="E78" t="s">
+      <c r="G78" t="s">
         <v>4</v>
       </c>
-      <c r="F78" s="3" t="s">
+      <c r="H78" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G78" t="s">
+      <c r="I78" t="s">
         <v>129</v>
       </c>
-      <c r="K78" t="s">
+      <c r="M78" t="s">
         <v>280</v>
       </c>
-      <c r="L78">
+      <c r="N78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:14">
       <c r="A79" t="s">
         <v>93</v>
       </c>
       <c r="C79" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" t="s">
+        <v>127</v>
+      </c>
+      <c r="E79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" t="s">
         <v>93</v>
       </c>
-      <c r="E79" t="s">
+      <c r="G79" t="s">
         <v>4</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="H79" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G79" t="s">
+      <c r="I79" t="s">
         <v>127</v>
       </c>
-      <c r="J79" t="s">
+      <c r="L79" t="s">
         <v>269</v>
       </c>
-      <c r="L79" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="N79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" t="s">
         <v>94</v>
       </c>
-      <c r="C80" t="s">
-        <v>5</v>
-      </c>
       <c r="E80" t="s">
+        <v>5</v>
+      </c>
+      <c r="G80" t="s">
         <v>4</v>
       </c>
-      <c r="F80" s="3" t="s">
+      <c r="H80" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G80" t="s">
+      <c r="I80" t="s">
         <v>129</v>
       </c>
-      <c r="L80">
+      <c r="N80">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:14">
       <c r="A81" t="s">
         <v>95</v>
       </c>
-      <c r="C81" t="s">
-        <v>5</v>
-      </c>
       <c r="E81" t="s">
+        <v>5</v>
+      </c>
+      <c r="G81" t="s">
         <v>2</v>
       </c>
-      <c r="F81" s="3" t="s">
+      <c r="H81" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G81" t="s">
+      <c r="I81" t="s">
         <v>251</v>
       </c>
-      <c r="J81" t="s">
+      <c r="L81" t="s">
         <v>94</v>
       </c>
-      <c r="K81" t="s">
+      <c r="M81" t="s">
         <v>230</v>
       </c>
-      <c r="L81">
+      <c r="N81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:14">
       <c r="A82" t="s">
         <v>2</v>
       </c>
-      <c r="C82" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" t="s">
         <v>2</v>
       </c>
-      <c r="E82" t="s">
+      <c r="G82" t="s">
         <v>2</v>
       </c>
-      <c r="F82" s="3" t="s">
+      <c r="H82" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G82" t="s">
+      <c r="I82" t="s">
         <v>251</v>
       </c>
-      <c r="H82" t="s">
-        <v>5</v>
-      </c>
       <c r="J82" t="s">
+        <v>5</v>
+      </c>
+      <c r="L82" t="s">
         <v>281</v>
       </c>
-      <c r="K82" t="s">
+      <c r="M82" t="s">
         <v>231</v>
       </c>
-      <c r="L82" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12">
+      <c r="N82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
       <c r="A83" t="s">
         <v>96</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" t="s">
-        <v>5</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="B83" t="s">
+        <v>127</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" t="s">
         <v>96</v>
       </c>
-      <c r="E83" t="s">
+      <c r="G83" t="s">
         <v>4</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="H83" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G83" t="s">
+      <c r="I83" t="s">
         <v>129</v>
       </c>
-      <c r="H83" t="s">
-        <v>5</v>
-      </c>
-      <c r="L83" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="J83" t="s">
+        <v>5</v>
+      </c>
+      <c r="N83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84" t="s">
         <v>97</v>
       </c>
-      <c r="C84" t="s">
-        <v>5</v>
-      </c>
       <c r="E84" t="s">
+        <v>5</v>
+      </c>
+      <c r="G84" t="s">
         <v>4</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="H84" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G84" t="s">
+      <c r="I84" t="s">
         <v>251</v>
       </c>
-      <c r="J84" t="s">
+      <c r="L84" t="s">
         <v>96</v>
       </c>
-      <c r="K84" t="s">
+      <c r="M84" t="s">
         <v>232</v>
       </c>
-      <c r="L84" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="N84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14">
       <c r="A85" t="s">
         <v>98</v>
       </c>
-      <c r="C85" t="s">
-        <v>5</v>
-      </c>
       <c r="E85" t="s">
+        <v>5</v>
+      </c>
+      <c r="G85" t="s">
         <v>4</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="H85" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G85" t="s">
+      <c r="I85" t="s">
         <v>251</v>
       </c>
-      <c r="J85" t="s">
+      <c r="L85" t="s">
         <v>96</v>
       </c>
-      <c r="K85" t="s">
+      <c r="M85" t="s">
         <v>232</v>
       </c>
-      <c r="L85" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="N85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14">
       <c r="A86" t="s">
         <v>99</v>
       </c>
-      <c r="B86" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>5</v>
       </c>
       <c r="E86" t="s">
+        <v>5</v>
+      </c>
+      <c r="G86" t="s">
         <v>4</v>
       </c>
-      <c r="F86" s="3" t="s">
+      <c r="H86" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G86" t="s">
+      <c r="I86" t="s">
         <v>129</v>
       </c>
-      <c r="L86">
+      <c r="N86">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:14">
       <c r="A87" t="s">
         <v>100</v>
       </c>
-      <c r="C87" t="s">
-        <v>5</v>
-      </c>
       <c r="E87" t="s">
+        <v>5</v>
+      </c>
+      <c r="G87" t="s">
         <v>2</v>
       </c>
-      <c r="F87" s="3" t="s">
+      <c r="H87" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G87" t="s">
+      <c r="I87" t="s">
         <v>251</v>
       </c>
-      <c r="J87" t="s">
+      <c r="L87" t="s">
         <v>99</v>
       </c>
-      <c r="K87" t="s">
+      <c r="M87" t="s">
         <v>233</v>
       </c>
-      <c r="L87">
+      <c r="N87">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:14">
       <c r="A88" t="s">
         <v>101</v>
       </c>
-      <c r="C88" t="s">
-        <v>5</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
+        <v>5</v>
+      </c>
+      <c r="F88" t="s">
         <v>157</v>
       </c>
-      <c r="E88" t="s">
+      <c r="G88" t="s">
         <v>9</v>
       </c>
-      <c r="F88" s="3" t="s">
+      <c r="H88" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G88" t="s">
+      <c r="I88" t="s">
         <v>251</v>
       </c>
-      <c r="J88" t="s">
+      <c r="L88" t="s">
         <v>157</v>
       </c>
-      <c r="K88" t="s">
+      <c r="M88" t="s">
         <v>235</v>
       </c>
-      <c r="L88" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="N88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14">
       <c r="A89" t="s">
         <v>102</v>
       </c>
-      <c r="C89" t="s">
-        <v>5</v>
-      </c>
       <c r="E89" t="s">
+        <v>5</v>
+      </c>
+      <c r="G89" t="s">
         <v>4</v>
       </c>
-      <c r="F89" s="3" t="s">
+      <c r="H89" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G89" t="s">
+      <c r="I89" t="s">
         <v>129</v>
       </c>
-      <c r="K89" t="s">
+      <c r="M89" t="s">
         <v>245</v>
       </c>
-      <c r="L89" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="N89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" t="s">
         <v>103</v>
       </c>
-      <c r="C90" t="s">
-        <v>5</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="B90" t="s">
+        <v>127</v>
+      </c>
+      <c r="E90" t="s">
+        <v>5</v>
+      </c>
+      <c r="F90" t="s">
         <v>103</v>
       </c>
-      <c r="E90" t="s">
+      <c r="G90" t="s">
         <v>25</v>
       </c>
-      <c r="F90" t="s">
+      <c r="H90" t="s">
         <v>278</v>
       </c>
-      <c r="G90" t="s">
+      <c r="I90" t="s">
         <v>129</v>
       </c>
-      <c r="H90" t="s">
-        <v>5</v>
-      </c>
-      <c r="K90" t="s">
+      <c r="J90" t="s">
+        <v>5</v>
+      </c>
+      <c r="M90" t="s">
         <v>106</v>
       </c>
-      <c r="L90" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="N90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14">
       <c r="A91" t="s">
         <v>183</v>
       </c>
-      <c r="E91" t="s">
+      <c r="C91" t="s">
+        <v>127</v>
+      </c>
+      <c r="G91" t="s">
         <v>4</v>
       </c>
-      <c r="F91" s="3" t="s">
+      <c r="H91" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G91" t="s">
+      <c r="I91" t="s">
         <v>127</v>
       </c>
-      <c r="J91" t="s">
+      <c r="L91" t="s">
         <v>270</v>
       </c>
-      <c r="K91" t="s">
+      <c r="M91" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:14">
       <c r="A92" t="s">
         <v>184</v>
       </c>
-      <c r="E92" t="s">
+      <c r="C92" t="s">
+        <v>127</v>
+      </c>
+      <c r="G92" t="s">
         <v>4</v>
       </c>
-      <c r="F92" t="s">
+      <c r="H92" t="s">
         <v>277</v>
       </c>
-      <c r="G92" t="s">
+      <c r="I92" t="s">
         <v>127</v>
       </c>
-      <c r="J92" t="s">
+      <c r="L92" t="s">
         <v>271</v>
       </c>
-      <c r="K92" t="s">
+      <c r="M92" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:14">
       <c r="A93" t="s">
         <v>185</v>
       </c>
-      <c r="E93" t="s">
+      <c r="G93" t="s">
         <v>4</v>
       </c>
-      <c r="F93" t="s">
+      <c r="H93" t="s">
         <v>277</v>
       </c>
-      <c r="G93" t="s">
+      <c r="I93" t="s">
         <v>234</v>
       </c>
-      <c r="J93" t="s">
+      <c r="L93" t="s">
         <v>282</v>
       </c>
-      <c r="K93" t="s">
+      <c r="M93" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:14">
       <c r="A94" t="s">
         <v>186</v>
       </c>
-      <c r="E94" t="s">
+      <c r="G94" t="s">
         <v>4</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="H94" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="G94" t="s">
+      <c r="I94" t="s">
         <v>234</v>
       </c>
-      <c r="J94" t="s">
+      <c r="L94" t="s">
         <v>283</v>
       </c>
-      <c r="K94" t="s">
+      <c r="M94" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="30">
+    <row r="95" spans="1:14" ht="30">
       <c r="A95" t="s">
         <v>188</v>
       </c>
-      <c r="E95" t="s">
+      <c r="C95" t="s">
+        <v>127</v>
+      </c>
+      <c r="G95" t="s">
         <v>4</v>
       </c>
-      <c r="F95" t="s">
+      <c r="H95" t="s">
         <v>277</v>
       </c>
-      <c r="G95" t="s">
+      <c r="I95" t="s">
         <v>127</v>
       </c>
-      <c r="J95" s="4" t="s">
+      <c r="L95" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="K95" t="s">
+      <c r="M95" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="30">
+    <row r="96" spans="1:14" ht="30">
       <c r="A96" t="s">
         <v>189</v>
       </c>
-      <c r="E96" t="s">
+      <c r="C96" t="s">
+        <v>127</v>
+      </c>
+      <c r="G96" t="s">
         <v>4</v>
       </c>
-      <c r="F96" t="s">
+      <c r="H96" t="s">
         <v>277</v>
       </c>
-      <c r="G96" t="s">
+      <c r="I96" t="s">
         <v>127</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="L96" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="45">
+    <row r="97" spans="1:13" ht="45">
       <c r="A97" t="s">
         <v>190</v>
       </c>
-      <c r="E97" t="s">
+      <c r="C97" t="s">
+        <v>127</v>
+      </c>
+      <c r="G97" t="s">
         <v>4</v>
       </c>
-      <c r="F97" t="s">
+      <c r="H97" t="s">
         <v>277</v>
       </c>
-      <c r="G97" t="s">
+      <c r="I97" t="s">
         <v>127</v>
       </c>
-      <c r="J97" s="4" t="s">
+      <c r="L97" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="30">
+    <row r="98" spans="1:13" ht="30">
       <c r="A98" t="s">
         <v>191</v>
       </c>
-      <c r="E98" t="s">
+      <c r="C98" t="s">
+        <v>127</v>
+      </c>
+      <c r="G98" t="s">
         <v>4</v>
       </c>
-      <c r="F98" t="s">
+      <c r="H98" t="s">
         <v>277</v>
       </c>
-      <c r="G98" t="s">
+      <c r="I98" t="s">
         <v>127</v>
       </c>
-      <c r="J98" s="4" t="s">
+      <c r="L98" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="30">
+    <row r="99" spans="1:13" ht="30">
       <c r="A99" t="s">
         <v>192</v>
       </c>
-      <c r="E99" t="s">
+      <c r="C99" t="s">
+        <v>127</v>
+      </c>
+      <c r="G99" t="s">
         <v>279</v>
       </c>
-      <c r="F99" t="s">
+      <c r="H99" t="s">
         <v>278</v>
       </c>
-      <c r="G99" t="s">
+      <c r="I99" t="s">
         <v>127</v>
       </c>
-      <c r="J99" s="4" t="s">
+      <c r="L99" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="K99" t="s">
+      <c r="M99" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:13">
       <c r="A100" t="s">
         <v>195</v>
       </c>
-      <c r="E100" t="s">
+      <c r="G100" t="s">
         <v>4</v>
       </c>
-      <c r="F100" t="s">
+      <c r="H100" t="s">
         <v>277</v>
       </c>
-      <c r="G100" t="s">
+      <c r="I100" t="s">
         <v>129</v>
       </c>
-      <c r="K100" t="s">
+      <c r="M100" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:13">
       <c r="A101" t="s">
         <v>193</v>
       </c>
-      <c r="E101" t="s">
+      <c r="G101" t="s">
         <v>4</v>
       </c>
-      <c r="F101" t="s">
+      <c r="H101" t="s">
         <v>277</v>
       </c>
-      <c r="G101" t="s">
+      <c r="I101" t="s">
         <v>129</v>
       </c>
-      <c r="K101" t="s">
+      <c r="M101" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:13">
       <c r="A102" t="s">
         <v>194</v>
       </c>
-      <c r="E102" t="s">
+      <c r="G102" t="s">
         <v>4</v>
       </c>
-      <c r="F102" t="s">
+      <c r="H102" t="s">
         <v>277</v>
       </c>
-      <c r="G102" t="s">
+      <c r="I102" t="s">
         <v>129</v>
       </c>
-      <c r="K102" t="s">
+      <c r="M102" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:13">
       <c r="A103" t="s">
         <v>197</v>
       </c>
-      <c r="E103" t="s">
+      <c r="G103" t="s">
         <v>4</v>
       </c>
-      <c r="F103" t="s">
+      <c r="H103" t="s">
         <v>277</v>
       </c>
-      <c r="G103" t="s">
+      <c r="I103" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:13">
       <c r="A104" t="s">
         <v>196</v>
       </c>
-      <c r="E104" t="s">
+      <c r="G104" t="s">
         <v>4</v>
       </c>
-      <c r="F104" t="s">
+      <c r="H104" t="s">
         <v>277</v>
       </c>
-      <c r="G104" t="s">
+      <c r="I104" t="s">
         <v>129</v>
       </c>
     </row>
+    <row r="105" spans="1:13">
+      <c r="A105" t="s">
+        <v>287</v>
+      </c>
+      <c r="B105" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="C2:C94">
-    <sortCondition ref="C2:C94"/>
+  <sortState ref="E2:E94">
+    <sortCondition ref="E2:E94"/>
   </sortState>
-  <conditionalFormatting sqref="A2:A104">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>IF(G2="C",1,0)</formula>
+  <conditionalFormatting sqref="A2:A105">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>IF($I2="Y",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>IF($G2="Y",1,0)</formula>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>IF(I2="C",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4886,6 +5016,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D104"/>
   <sheetViews>
@@ -5531,7 +5680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D104"/>
   <sheetViews>
@@ -6183,7 +6332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D104"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated EML worksheet with current xPath information used by current index processing implementation.  noted where fields are copy field destinations and where the path present in the EML worksheet is not found in the eml field definition file.
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="0" windowWidth="30540" windowHeight="25420" tabRatio="500"/>
+    <workbookView xWindow="11540" yWindow="0" windowWidth="22000" windowHeight="20400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$N$102</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="313">
   <si>
     <t>Notes</t>
   </si>
@@ -556,9 +556,6 @@
     <t>PropertLookup_props_writer.java</t>
   </si>
   <si>
-    <t>//eml:eml/dataset/creator/individualName/surName/text()</t>
-  </si>
-  <si>
     <t>//mets:METS/ mets:dmdSec/ mets:mdWrap/ mets:xmlData/ dim:dim/ dim:field[@qualifier='author']/text()</t>
   </si>
   <si>
@@ -586,24 +583,12 @@
     <t>//dataset/coverage/geographicCoverage/boundingCoordinates/westBoundingCoordinate/text()</t>
   </si>
   <si>
-    <t>concat (//eml:eml/ dataset/ creator/ individualName/ givenName /text(),' ',//eml:eml/ dataset/ creator/ individualName/ surName /text())</t>
-  </si>
-  <si>
-    <t>//eml:eml/ dataset/ project/ title/text()</t>
-  </si>
-  <si>
-    <t>//dataset/pubDate/text()</t>
-  </si>
-  <si>
     <t>//dataset/title/text()</t>
   </si>
   <si>
     <t>//mets:METS/ mets:dmdSec/ mets:mdWrap/ mets:xmlData/ dim:dim/ dim:field[@element='title']/text()</t>
   </si>
   <si>
-    <t>//dataset/distribution/online/url/text()</t>
-  </si>
-  <si>
     <t>//mets:METS/ mets:dmdSec/ mets:mdWrap/ mets:xmlData/ dim:dim/ dim:field[@qualifier='uri']/text()</t>
   </si>
   <si>
@@ -625,15 +610,9 @@
     <t>//dataset/coverage/temporalCoverage/rangeOfDates/beginDate/calendarDate/text()</t>
   </si>
   <si>
-    <t>//dataset/coverage/temporalCoverage/rangeOfDates/endDate/calendarDate/text()"</t>
-  </si>
-  <si>
     <t>http://knb.ecoinformatics.org/software/eml/eml-2.1.0/eml-coverage.html#TemporalCoverage</t>
   </si>
   <si>
-    <t>//dataset/abstract/para/text()</t>
-  </si>
-  <si>
     <t>//dataset/creator/individualName/surName/text()</t>
   </si>
   <si>
@@ -877,9 +856,6 @@
     <t>Should contain a URL for downloading the object</t>
   </si>
   <si>
-    <t>distinct-values(//creator/organizationName)</t>
-  </si>
-  <si>
     <t>Need to combine these values outside of Xpath</t>
   </si>
   <si>
@@ -1001,6 +977,105 @@
   </si>
   <si>
     <t>D1Sys</t>
+  </si>
+  <si>
+    <t>//dataset/abstract/descendant::text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/replicationPolicy/blockedMemberNode/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/checksum/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/checksum/@algorithm</t>
+  </si>
+  <si>
+    <t>//dataset/creator/organizationName/text()</t>
+  </si>
+  <si>
+    <t>Copyfield destination</t>
+  </si>
+  <si>
+    <t>WebUrlSolrField, driven off systemMetadata/identifier/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/originMemberNode/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/dateUploaded/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/dateSysMetadataModified/text()</t>
+  </si>
+  <si>
+    <t>Derived from ORE Resource Map</t>
+  </si>
+  <si>
+    <t>//dataset/coverage/temporalCoverage/rangeOfDates/endDate/calendarDate/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/identifier/text()</t>
+  </si>
+  <si>
+    <t>RULE NOT PRESENT IN INDEX PROCESSING - //eml:eml/dataset/creator/individualName/surName/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/replicationPolicy/@numberReplicas</t>
+  </si>
+  <si>
+    <t>systemMetadata/formatId/text()</t>
+  </si>
+  <si>
+    <t>RULE NOT PRESENT IN INDEX PROCESSING - concat (//eml:eml/ dataset/ creator/ individualName/ givenName /text(),' ',//eml:eml/ dataset/ creator/ individualName/ surName /text())</t>
+  </si>
+  <si>
+    <t>systemMetadata/replicationPolicy/preferredMemberNode/text()</t>
+  </si>
+  <si>
+    <t>RULE NOT PRESENT IN INDEX PROCESSING - //eml:eml/ dataset/ project/ title/text()</t>
+  </si>
+  <si>
+    <t>RULE NOT PRESENT IN INDEX PROCESSING - //dataset/pubDate/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/replicationPolicy/@replicationAllowed</t>
+  </si>
+  <si>
+    <t>systemMetadata/rightsHolder/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/size/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/submitter/text()</t>
+  </si>
+  <si>
+    <t>All descriptive text, concatenated, Copyfield destination</t>
+  </si>
+  <si>
+    <t>WebUrlSolrField, driven off systemMetadata/identifier/text() ---- ORIGINAL VALUE FOR THIS COLUMN:  //dataset/distribution/online/url/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/authoritativeMemberNode/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/replica/replicaMemberNode/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/accessPolicy/allow[permission= 'read']/subject/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/accessPolicy/allow[permission= 'write']/subject/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/accessPolicy/allow[permission= 'execute']/subject/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/accessPolicy/allow[permission= 'changePermission']/subject/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/accessPolicy/allow[permission= 'read']/subject[text()='public']/text()</t>
   </si>
 </sst>
 </file>
@@ -2274,68 +2349,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A54" sqref="A54"/>
+      <selection pane="bottomRight" activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" customWidth="1"/>
-    <col min="6" max="6" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" customWidth="1"/>
-    <col min="12" max="12" width="57" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="73.83203125" customWidth="1"/>
     <col min="13" max="13" width="42.6640625" customWidth="1"/>
     <col min="14" max="14" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="J1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="K1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="L1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2355,7 +2434,7 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I2" t="s">
         <v>129</v>
@@ -2384,7 +2463,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I3" t="s">
         <v>129</v>
@@ -2393,7 +2472,7 @@
         <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2413,7 +2492,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I4" t="s">
         <v>129</v>
@@ -2442,7 +2521,7 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I5" t="s">
         <v>129</v>
@@ -2474,16 +2553,16 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I6" t="s">
         <v>127</v>
       </c>
       <c r="L6" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="M6" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -2500,7 +2579,7 @@
         <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I7" t="s">
         <v>129</v>
@@ -2526,13 +2605,13 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I8" t="s">
         <v>127</v>
       </c>
       <c r="L8" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="N8" t="s">
         <v>5</v>
@@ -2555,13 +2634,13 @@
         <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I9" t="s">
         <v>127</v>
       </c>
       <c r="L9" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="N9" t="s">
         <v>5</v>
@@ -2578,13 +2657,13 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I10" t="s">
         <v>129</v>
       </c>
       <c r="M10" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -2598,19 +2677,19 @@
         <v>127</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I11" t="s">
         <v>129</v>
@@ -2630,10 +2709,10 @@
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I12" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="K12">
         <f>IF(I12="C",1,0)</f>
@@ -2663,13 +2742,13 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I13" t="s">
         <v>127</v>
       </c>
       <c r="L13" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="M13" t="s">
         <v>134</v>
@@ -2689,28 +2768,28 @@
         <v>127</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G14" t="s">
         <v>4</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I14" t="s">
         <v>127</v>
       </c>
       <c r="L14" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="M14" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="N14" t="s">
         <v>5</v>
@@ -2718,7 +2797,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
         <v>127</v>
@@ -2730,18 +2809,18 @@
         <v>9</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I15" t="s">
         <v>127</v>
       </c>
       <c r="L15" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
         <v>127</v>
@@ -2750,22 +2829,22 @@
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G16" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I16" t="s">
         <v>127</v>
       </c>
       <c r="L16" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="M16" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="N16" t="s">
         <v>5</v>
@@ -2779,7 +2858,7 @@
         <v>127</v>
       </c>
       <c r="D17" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -2788,13 +2867,13 @@
         <v>4</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I17" t="s">
         <v>129</v>
       </c>
       <c r="M17" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="N17" t="s">
         <v>5</v>
@@ -2802,28 +2881,28 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
       </c>
       <c r="H18" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="I18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L18" t="s">
         <v>277</v>
       </c>
-      <c r="I18" t="s">
-        <v>234</v>
-      </c>
-      <c r="L18" t="s">
-        <v>285</v>
-      </c>
       <c r="M18" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -2843,16 +2922,16 @@
         <v>4</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I19" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="L19" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="M19" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="N19" t="s">
         <v>5</v>
@@ -2872,13 +2951,13 @@
         <v>4</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I20" t="s">
         <v>129</v>
       </c>
       <c r="M20" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="N20" t="s">
         <v>5</v>
@@ -2895,16 +2974,16 @@
         <v>2</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I21" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="M21" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="N21" t="s">
         <v>5</v>
@@ -2927,7 +3006,7 @@
         <v>25</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I22" t="s">
         <v>129</v>
@@ -2953,7 +3032,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I23" t="s">
         <v>129</v>
@@ -2979,7 +3058,7 @@
         <v>9</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I24" t="s">
         <v>129</v>
@@ -3005,13 +3084,13 @@
         <v>4</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I25" t="s">
         <v>129</v>
       </c>
       <c r="M25" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -3028,13 +3107,13 @@
         <v>2</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I26" t="s">
         <v>129</v>
       </c>
       <c r="M26" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -3051,7 +3130,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I27" t="s">
         <v>129</v>
@@ -3074,7 +3153,7 @@
         <v>2</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I28" t="s">
         <v>129</v>
@@ -3097,7 +3176,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I29" t="s">
         <v>129</v>
@@ -3117,13 +3196,13 @@
         <v>4</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I30" t="s">
         <v>129</v>
       </c>
       <c r="M30" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -3140,7 +3219,7 @@
         <v>4</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I31" t="s">
         <v>129</v>
@@ -3169,16 +3248,16 @@
         <v>4</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I32" t="s">
         <v>127</v>
       </c>
       <c r="L32" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="M32" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="N32" t="s">
         <v>5</v>
@@ -3195,16 +3274,16 @@
         <v>4</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I33" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L33" t="s">
         <v>39</v>
       </c>
       <c r="M33" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="N33" t="s">
         <v>5</v>
@@ -3221,7 +3300,7 @@
         <v>2</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
@@ -3241,13 +3320,13 @@
         <v>4</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
       </c>
       <c r="M35" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="N35" t="s">
         <v>5</v>
@@ -3264,10 +3343,10 @@
         <v>2</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I36" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L36" t="s">
         <v>43</v>
@@ -3287,13 +3366,13 @@
         <v>4</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I37" t="s">
         <v>129</v>
       </c>
       <c r="M37" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="N37" t="s">
         <v>5</v>
@@ -3304,7 +3383,7 @@
         <v>46</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E38" t="s">
         <v>5</v>
@@ -3316,7 +3395,7 @@
         <v>4</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I38" t="s">
         <v>129</v>
@@ -3342,10 +3421,10 @@
         <v>2</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I39" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L39" t="s">
         <v>46</v>
@@ -3365,13 +3444,13 @@
         <v>4</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I40" t="s">
         <v>129</v>
       </c>
       <c r="M40" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="N40">
         <v>0</v>
@@ -3391,7 +3470,7 @@
         <v>4</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
@@ -3411,7 +3490,7 @@
         <v>2</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
@@ -3434,16 +3513,16 @@
         <v>4</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I43" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L43" t="s">
         <v>51</v>
       </c>
       <c r="M43" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="N43">
         <v>0</v>
@@ -3460,13 +3539,13 @@
         <v>2</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I44" t="s">
         <v>129</v>
       </c>
       <c r="M44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -3483,13 +3562,13 @@
         <v>4</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
       </c>
       <c r="M45" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="N45" t="s">
         <v>5</v>
@@ -3512,7 +3591,7 @@
         <v>25</v>
       </c>
       <c r="H46" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
@@ -3521,7 +3600,7 @@
         <v>5</v>
       </c>
       <c r="M46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N46" t="s">
         <v>5</v>
@@ -3544,16 +3623,16 @@
         <v>4</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I47" t="s">
         <v>127</v>
       </c>
       <c r="L47" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="M47" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -3570,19 +3649,19 @@
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I48" t="s">
         <v>127</v>
       </c>
       <c r="L48" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="N48" t="s">
         <v>5</v>
@@ -3590,7 +3669,7 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C49" t="s">
         <v>127</v>
@@ -3599,19 +3678,19 @@
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I49" t="s">
         <v>127</v>
       </c>
       <c r="L49" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="N49" t="s">
         <v>5</v>
@@ -3634,13 +3713,13 @@
         <v>4</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I50" t="s">
         <v>127</v>
       </c>
       <c r="L50" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="N50" t="s">
         <v>5</v>
@@ -3660,7 +3739,7 @@
         <v>2</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I51" t="s">
         <v>129</v>
@@ -3680,13 +3759,13 @@
         <v>4</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I52" t="s">
         <v>129</v>
       </c>
       <c r="M52" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -3706,13 +3785,13 @@
         <v>4</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I53" t="s">
         <v>129</v>
       </c>
       <c r="M53" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="N53" t="s">
         <v>5</v>
@@ -3732,7 +3811,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I54" t="s">
         <v>129</v>
@@ -3752,16 +3831,16 @@
         <v>2</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I55" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L55" t="s">
         <v>64</v>
       </c>
       <c r="M55" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="N55">
         <v>0</v>
@@ -3778,16 +3857,16 @@
         <v>2</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I56" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L56" t="s">
         <v>62</v>
       </c>
       <c r="M56" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="N56" t="s">
         <v>5</v>
@@ -3807,7 +3886,7 @@
         <v>4</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I57" t="s">
         <v>129</v>
@@ -3827,10 +3906,10 @@
         <v>2</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I58" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L58" t="s">
         <v>67</v>
@@ -3850,13 +3929,13 @@
         <v>4</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I59" t="s">
         <v>129</v>
       </c>
       <c r="M59" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -3876,7 +3955,7 @@
         <v>2</v>
       </c>
       <c r="H60" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I60" t="s">
         <v>129</v>
@@ -3905,16 +3984,16 @@
         <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I61" t="s">
         <v>127</v>
       </c>
       <c r="L61" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="M61" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="N61">
         <v>0</v>
@@ -3937,7 +4016,7 @@
         <v>4</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I62" t="s">
         <v>129</v>
@@ -3960,13 +4039,13 @@
         <v>4</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I63" t="s">
         <v>129</v>
       </c>
       <c r="M63" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="N63" t="s">
         <v>5</v>
@@ -3983,16 +4062,16 @@
         <v>2</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I64" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L64" t="s">
         <v>73</v>
       </c>
       <c r="M64" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="N64" t="s">
         <v>5</v>
@@ -4009,22 +4088,22 @@
         <v>5</v>
       </c>
       <c r="F65" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G65" t="s">
         <v>9</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I65" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L65" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="M65" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="N65" t="s">
         <v>5</v>
@@ -4044,7 +4123,7 @@
         <v>2</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I66" t="s">
         <v>129</v>
@@ -4070,16 +4149,16 @@
         <v>4</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I67" t="s">
         <v>127</v>
       </c>
       <c r="L67" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="M67" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="N67">
         <v>0</v>
@@ -4096,19 +4175,19 @@
         <v>5</v>
       </c>
       <c r="F68" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G68" t="s">
         <v>4</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I68" t="s">
         <v>127</v>
       </c>
       <c r="L68" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="N68">
         <v>0</v>
@@ -4128,7 +4207,7 @@
         <v>4</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I69" t="s">
         <v>129</v>
@@ -4148,16 +4227,16 @@
         <v>2</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I70" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L70" t="s">
         <v>79</v>
       </c>
       <c r="M70" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N70">
         <v>0</v>
@@ -4174,7 +4253,7 @@
         <v>4</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I71" t="s">
         <v>129</v>
@@ -4194,10 +4273,10 @@
         <v>2</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I72" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L72" t="s">
         <v>81</v>
@@ -4223,13 +4302,13 @@
         <v>84</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I73" t="s">
         <v>127</v>
       </c>
       <c r="L73" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="N73" t="s">
         <v>5</v>
@@ -4246,16 +4325,16 @@
         <v>86</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I74" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L74" t="s">
         <v>39</v>
       </c>
       <c r="M74" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="N74" t="s">
         <v>5</v>
@@ -4272,7 +4351,7 @@
         <v>4</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I75" t="s">
         <v>129</v>
@@ -4292,16 +4371,16 @@
         <v>2</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I76" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L76" t="s">
         <v>87</v>
       </c>
       <c r="M76" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="N76">
         <v>0</v>
@@ -4324,7 +4403,7 @@
         <v>25</v>
       </c>
       <c r="H77" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I77" t="s">
         <v>129</v>
@@ -4347,19 +4426,19 @@
         <v>5</v>
       </c>
       <c r="F78" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="G78" t="s">
         <v>4</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I78" t="s">
         <v>129</v>
       </c>
       <c r="M78" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="N78">
         <v>0</v>
@@ -4382,13 +4461,13 @@
         <v>4</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I79" t="s">
         <v>127</v>
       </c>
       <c r="L79" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="N79" t="s">
         <v>5</v>
@@ -4405,7 +4484,7 @@
         <v>4</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I80" t="s">
         <v>129</v>
@@ -4425,16 +4504,16 @@
         <v>2</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I81" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L81" t="s">
         <v>94</v>
       </c>
       <c r="M81" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="N81">
         <v>0</v>
@@ -4454,19 +4533,19 @@
         <v>2</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I82" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="J82" t="s">
         <v>5</v>
       </c>
       <c r="L82" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="M82" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="N82" t="s">
         <v>5</v>
@@ -4492,7 +4571,7 @@
         <v>4</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I83" t="s">
         <v>129</v>
@@ -4515,16 +4594,16 @@
         <v>4</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I84" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L84" t="s">
         <v>96</v>
       </c>
       <c r="M84" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="N84" t="s">
         <v>5</v>
@@ -4541,16 +4620,16 @@
         <v>4</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I85" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L85" t="s">
         <v>96</v>
       </c>
       <c r="M85" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="N85" t="s">
         <v>5</v>
@@ -4570,7 +4649,7 @@
         <v>4</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I86" t="s">
         <v>129</v>
@@ -4590,16 +4669,16 @@
         <v>2</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I87" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L87" t="s">
         <v>99</v>
       </c>
       <c r="M87" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="N87">
         <v>0</v>
@@ -4613,22 +4692,22 @@
         <v>5</v>
       </c>
       <c r="F88" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G88" t="s">
         <v>9</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I88" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L88" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="M88" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="N88" t="s">
         <v>5</v>
@@ -4645,13 +4724,13 @@
         <v>4</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I89" t="s">
         <v>129</v>
       </c>
       <c r="M89" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="N89" t="s">
         <v>5</v>
@@ -4674,7 +4753,7 @@
         <v>25</v>
       </c>
       <c r="H90" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I90" t="s">
         <v>129</v>
@@ -4691,7 +4770,7 @@
     </row>
     <row r="91" spans="1:14">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C91" t="s">
         <v>127</v>
@@ -4700,21 +4779,21 @@
         <v>4</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I91" t="s">
         <v>127</v>
       </c>
       <c r="L91" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="M91" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:14">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C92" t="s">
         <v>127</v>
@@ -4723,61 +4802,61 @@
         <v>4</v>
       </c>
       <c r="H92" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I92" t="s">
         <v>127</v>
       </c>
       <c r="L92" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="M92" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G93" t="s">
         <v>4</v>
       </c>
       <c r="H93" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I93" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="L93" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="M93" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G94" t="s">
         <v>4</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I94" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="L94" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="M94" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" ht="30">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C95" t="s">
         <v>127</v>
@@ -4786,21 +4865,21 @@
         <v>4</v>
       </c>
       <c r="H95" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I95" t="s">
         <v>127</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="M95" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" ht="30">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C96" t="s">
         <v>127</v>
@@ -4809,18 +4888,18 @@
         <v>4</v>
       </c>
       <c r="H96" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I96" t="s">
         <v>127</v>
       </c>
       <c r="L96" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" ht="45">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C97" t="s">
         <v>127</v>
@@ -4829,18 +4908,18 @@
         <v>4</v>
       </c>
       <c r="H97" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I97" t="s">
         <v>127</v>
       </c>
       <c r="L97" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" ht="30">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C98" t="s">
         <v>127</v>
@@ -4849,98 +4928,98 @@
         <v>4</v>
       </c>
       <c r="H98" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I98" t="s">
         <v>127</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" ht="30">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
       <c r="A99" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C99" t="s">
         <v>127</v>
       </c>
       <c r="G99" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="H99" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I99" t="s">
         <v>127</v>
       </c>
       <c r="L99" s="4" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="M99" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G100" t="s">
         <v>4</v>
       </c>
       <c r="H100" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I100" t="s">
         <v>129</v>
       </c>
       <c r="M100" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G101" t="s">
         <v>4</v>
       </c>
       <c r="H101" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I101" t="s">
         <v>129</v>
       </c>
       <c r="M101" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G102" t="s">
         <v>4</v>
       </c>
       <c r="H102" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I102" t="s">
         <v>129</v>
       </c>
       <c r="M102" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G103" t="s">
         <v>4</v>
       </c>
       <c r="H103" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I103" t="s">
         <v>129</v>
@@ -4948,13 +5027,13 @@
     </row>
     <row r="104" spans="1:13">
       <c r="A104" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="G104" t="s">
         <v>4</v>
       </c>
       <c r="H104" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I104" t="s">
         <v>129</v>
@@ -4973,7 +5052,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4987,30 +5065,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
-    <col min="2" max="2" width="95.33203125" customWidth="1"/>
-    <col min="3" max="3" width="84.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="114.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5018,10 +5099,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>280</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5029,13 +5110,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5043,10 +5124,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5054,16 +5135,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>133</v>
       </c>
+      <c r="B6" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
@@ -5074,11 +5158,17 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>15</v>
       </c>
+      <c r="B9" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -5090,35 +5180,50 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>246</v>
+        <v>284</v>
       </c>
       <c r="D11" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>18</v>
       </c>
+      <c r="B12" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>19</v>
       </c>
+      <c r="B13" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>20</v>
       </c>
+      <c r="B14" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>175</v>
+      </c>
+      <c r="B16" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5126,18 +5231,24 @@
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>180</v>
+      </c>
+      <c r="B18" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>135</v>
       </c>
+      <c r="B19" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
@@ -5151,16 +5262,19 @@
       <c r="A21" t="s">
         <v>23</v>
       </c>
+      <c r="B21" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C22" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5173,10 +5287,10 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>291</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5218,11 +5332,17 @@
       <c r="A32" t="s">
         <v>39</v>
       </c>
+      <c r="B32" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>40</v>
       </c>
+      <c r="B33" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
@@ -5234,13 +5354,16 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>44</v>
       </c>
+      <c r="B36" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
@@ -5252,13 +5375,16 @@
         <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>48</v>
       </c>
+      <c r="B39" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
@@ -5279,6 +5405,9 @@
       <c r="A43" t="s">
         <v>52</v>
       </c>
+      <c r="B43" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
@@ -5295,21 +5424,27 @@
         <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C46" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
         <v>131</v>
       </c>
+      <c r="B47" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>57</v>
       </c>
+      <c r="B48" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
@@ -5336,7 +5471,7 @@
         <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>149</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -5348,11 +5483,17 @@
       <c r="A55" t="s">
         <v>65</v>
       </c>
+      <c r="B55" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>66</v>
       </c>
+      <c r="B56" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
@@ -5363,6 +5504,9 @@
       <c r="A58" t="s">
         <v>68</v>
       </c>
+      <c r="B58" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
@@ -5378,6 +5522,9 @@
       <c r="A61" t="s">
         <v>71</v>
       </c>
+      <c r="B61" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
@@ -5389,20 +5536,23 @@
         <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
+        <v>298</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>74</v>
       </c>
+      <c r="B64" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>151</v>
+        <v>299</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -5414,11 +5564,17 @@
       <c r="A67" t="s">
         <v>130</v>
       </c>
+      <c r="B67" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>78</v>
       </c>
+      <c r="B68" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
@@ -5429,6 +5585,9 @@
       <c r="A70" t="s">
         <v>80</v>
       </c>
+      <c r="B70" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
@@ -5439,16 +5598,25 @@
       <c r="A72" t="s">
         <v>82</v>
       </c>
+      <c r="B72" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>83</v>
       </c>
+      <c r="B73" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>85</v>
       </c>
+      <c r="B74" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
@@ -5459,13 +5627,16 @@
       <c r="A76" t="s">
         <v>88</v>
       </c>
+      <c r="B76" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>89</v>
       </c>
       <c r="B77" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -5477,6 +5648,9 @@
       <c r="A79" t="s">
         <v>93</v>
       </c>
+      <c r="B79" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
@@ -5487,13 +5661,16 @@
       <c r="A81" t="s">
         <v>95</v>
       </c>
+      <c r="B81" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>170</v>
+        <v>304</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -5501,21 +5678,27 @@
         <v>96</v>
       </c>
       <c r="B83" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C83" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>97</v>
       </c>
+      <c r="B84" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>98</v>
       </c>
+      <c r="B85" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
@@ -5526,18 +5709,24 @@
       <c r="A87" t="s">
         <v>100</v>
       </c>
+      <c r="B87" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>101</v>
       </c>
+      <c r="B88" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>102</v>
       </c>
       <c r="B89" t="s">
-        <v>154</v>
+        <v>305</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -5545,82 +5734,108 @@
         <v>103</v>
       </c>
       <c r="B90" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>176</v>
+      </c>
+      <c r="B91" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="B92" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>178</v>
+      </c>
+      <c r="B93" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>179</v>
+      </c>
+      <c r="B94" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>181</v>
+      </c>
+      <c r="B95" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>183</v>
+      </c>
+      <c r="B97" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>184</v>
+      </c>
+      <c r="B98" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>185</v>
+      </c>
+      <c r="B99" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="3" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5647,16 +5862,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5735,12 +5950,12 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5750,7 +5965,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -6145,7 +6360,7 @@
         <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -6202,77 +6417,76 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6298,16 +6512,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6377,12 +6591,12 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -6392,7 +6606,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -6483,7 +6697,7 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -6501,7 +6715,7 @@
         <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -6579,7 +6793,7 @@
         <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -6732,7 +6946,7 @@
         <v>96</v>
       </c>
       <c r="B83" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -6765,7 +6979,7 @@
         <v>102</v>
       </c>
       <c r="B89" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -6775,77 +6989,76 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added descriptions to most of the SOLR index fields.
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="0" windowWidth="22000" windowHeight="20400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5120" yWindow="1740" windowWidth="45280" windowHeight="25040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Dryad" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$N$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$O$104</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="363">
   <si>
     <t>Notes</t>
   </si>
@@ -877,72 +877,12 @@
     <t>ValueOrigin</t>
   </si>
   <si>
-    <t>:attr:`SystemMetadata.replicationPolicy` blockedMemberNode</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.checksum`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.algorithm`</t>
-  </si>
-  <si>
     <t>Resolve REST URL created from PID</t>
   </si>
   <si>
-    <t>:attr:`SystemMetadata.dateSysMetadataModified`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.dateUploaded`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.identifier`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.replicationPolicy` numberReplicas attribute</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.formatId`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.obsoletedBy`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.obsoletes`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.replicationPolicy` preferredMemberNode</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.replicationPolicy` replicationAllowed attribute</t>
-  </si>
-  <si>
     <t>:attr:`SystemMetadata.rightsHolder`</t>
   </si>
   <si>
-    <t>:attr:`SystemMetadata.size`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.submitter`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.authoritativeMemberNode`</t>
-  </si>
-  <si>
-    <t>:attr:`SystemMetadata.replica` replica/replicationMemberNode element</t>
-  </si>
-  <si>
-    <t>List of subjects (groups and individuals) that have read permission on PID, value retrieved from :attr:`SystemMetadata.accessPolicy`.</t>
-  </si>
-  <si>
-    <t>List of subjects (groups and individuals) that have write permission on PID, value retrieved from :attr:`SystemMetadata.accessPolicy`.</t>
-  </si>
-  <si>
-    <t>List of subjects (groups and individuals) that have execute permission on PID, value retrieved from :attr:`SystemMetadata.accessPolicy`.</t>
-  </si>
-  <si>
-    <t>List of subjects (groups and individuals) that have change permission on PID, value retrieved from :attr:`SystemMetadata.accessPolicy`.</t>
-  </si>
-  <si>
     <t>Set to True if the DataONE :term:`public user` is present in the list of subjects with readPermission on PID.</t>
   </si>
   <si>
@@ -1076,6 +1016,216 @@
   </si>
   <si>
     <t>systemMetadata/accessPolicy/allow[permission= 'read']/subject[text()='public']/text()</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>The full text of the abstract as provided in the science metadata document.</t>
+  </si>
+  <si>
+    <t>The LAST name(s) of the author(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principle Investigator (PI) / Author as listed in the metadata document. </t>
+  </si>
+  <si>
+    <t>The starting date of the temporal range of the content described by the metadata document.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Taxonomic class name(s)</t>
+  </si>
+  <si>
+    <t>Taxonomic family name(s)</t>
+  </si>
+  <si>
+    <t>Taxonomic genus name(s)</t>
+  </si>
+  <si>
+    <t>Taxonomic kingdom(s)</t>
+  </si>
+  <si>
+    <t>Taxonomic order name(s)</t>
+  </si>
+  <si>
+    <t>Taxonomic phylum (or division) name(s)</t>
+  </si>
+  <si>
+    <t>Taxonomic species name(s)</t>
+  </si>
+  <si>
+    <t>Taxonomic scientific name(s) at the most precise level available for the organisms of relevance to the dataset</t>
+  </si>
+  <si>
+    <t>The latest decade that is covered by the dataset, expressed in the form "1999-2009"</t>
+  </si>
+  <si>
+    <t>Eastern most longitude of the spatial extent, in decimal degrees, WGS84</t>
+  </si>
+  <si>
+    <t>Northern most latitude of the spatial extent, in decimal degrees, WGS84</t>
+  </si>
+  <si>
+    <t>Southern most latitude of the spatial extent, in decimal degrees, WGS84</t>
+  </si>
+  <si>
+    <t>Western most longitude of the spatial extent, in decimal degrees, WGS84</t>
+  </si>
+  <si>
+    <t>Name of the organization to contact for more information about the dataset</t>
+  </si>
+  <si>
+    <t>The ending date of the temporal range of the content described by the metadata document.</t>
+  </si>
+  <si>
+    <t>Full text of the metadata record, used to support full text searches</t>
+  </si>
+  <si>
+    <t>Keywords drawn from the GCMD controlled vocabulary</t>
+  </si>
+  <si>
+    <t>Name of the investigator(s) responsible for developing the dataset and associated content.</t>
+  </si>
+  <si>
+    <t>Set to "Y" for records that contain spatial information</t>
+  </si>
+  <si>
+    <t>Keywords recorded in the science metadata document. These may be controlled by the generator of the metadata or by the metadata standard of the document, but are effectively uncontrolled within the  DataONE context.</t>
+  </si>
+  <si>
+    <t>Set to "Y" if there is no bounding box information available (i.e., the east, west, north, south most coordinates)</t>
+  </si>
+  <si>
+    <t>URL for Open Geospatial Web service if available.</t>
+  </si>
+  <si>
+    <t>Title of the dataset as recorded in the science metadata.</t>
+  </si>
+  <si>
+    <t>A multi-valued field that contains the node Ids of member nodes that are blocked from holding replicas of this object.</t>
+  </si>
+  <si>
+    <t>Algorithm used for generating the object checksum</t>
+  </si>
+  <si>
+    <t>The checksum for the object</t>
+  </si>
+  <si>
+    <t>The URL that can be used to resolve the location of the object given its PID.</t>
+  </si>
+  <si>
+    <t>:attr:`Types.ReplicationPolicy.blockedMemberNode`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.checksum`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.Checksum.algorithm`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.originMemberNode`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.dateUploaded`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.dateSysMetadataModified`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.identifier`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.replicationPolicy.numberReplicas`</t>
+  </si>
+  <si>
+    <t>Requested number of replicas for the object</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.formatId`</t>
+  </si>
+  <si>
+    <t>The format identifier indicating the type of content this record refers to.</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.obsoletedBy`</t>
+  </si>
+  <si>
+    <t>If set, indicates the identifier of the object that obsoletes this one.</t>
+  </si>
+  <si>
+    <t>If set, indicates the object that this record obsoletes.</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.obsoletes`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.ReplicationPolicy.preferredMemberNode`</t>
+  </si>
+  <si>
+    <t>A list of member node identifiers that are preferred replication targets for this object.</t>
+  </si>
+  <si>
+    <t>True if this object can be replicated.</t>
+  </si>
+  <si>
+    <t>:attr:`Types.ReplicationPolicy.replicationAllowed`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The :term:`Subject` that acts as the rights holder for the object. </t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.size`</t>
+  </si>
+  <si>
+    <t>The size of the object, in bytes.</t>
+  </si>
+  <si>
+    <t>The :term:`Subject` name of the original submitter of the content to DataONE.</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.submitter`</t>
+  </si>
+  <si>
+    <t>:attr:`Types.SystemMetadata.authoritativeMemberNode`</t>
+  </si>
+  <si>
+    <t>The node Id of the authoritative Member Node for the object.</t>
+  </si>
+  <si>
+    <t>:attr:`Types.Replica.replicationMemberNode`</t>
+  </si>
+  <si>
+    <t>One or more node Ids holding copies of the object.</t>
+  </si>
+  <si>
+    <t>List of subjects (groups and individuals) that have read permission on PID.</t>
+  </si>
+  <si>
+    <t>:attr:`Types.AccessRule.subject` where permission = read</t>
+  </si>
+  <si>
+    <t>List of subjects (groups and individuals) that have write permission on PID.</t>
+  </si>
+  <si>
+    <t>List of subjects (groups and individuals) that have change permission on PID.</t>
+  </si>
+  <si>
+    <t>:attr:`Types.AccessRule.subject` where permission = changePermission</t>
+  </si>
+  <si>
+    <t>:attr:`Types.AccessRule.subject` where permission = write</t>
+  </si>
+  <si>
+    <t>The node Id of the member node that originally contributed the content.</t>
+  </si>
+  <si>
+    <t>The date and time when the object was uploaded to the Member Node.</t>
+  </si>
+  <si>
+    <t>The date and time when the object system metadata was last updated.</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1314,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="411">
+  <cellStyleXfs count="431">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1576,8 +1726,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1585,8 +1755,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="411">
+  <cellStyles count="431">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1799,6 +1972,16 @@
     <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1997,6 +2180,16 @@
     <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -2347,13 +2540,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N104"/>
+  <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A83" sqref="A83:XFD83"/>
+      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2368,20 +2561,21 @@
     <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="73.83203125" customWidth="1"/>
-    <col min="13" max="13" width="42.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="57.1640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="73.83203125" customWidth="1"/>
+    <col min="14" max="14" width="42.6640625" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C1" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="D1" t="s">
         <v>235</v>
@@ -2407,17 +2601,20 @@
       <c r="K1" t="s">
         <v>171</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="M1" t="s">
         <v>245</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15" ht="30">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2434,7 +2631,7 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I2" t="s">
         <v>129</v>
@@ -2442,11 +2639,14 @@
       <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="L2" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="30">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2463,7 +2663,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I3" t="s">
         <v>129</v>
@@ -2471,14 +2671,17 @@
       <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="M3" t="s">
+      <c r="L3" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="N3" t="s">
         <v>215</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2492,7 +2695,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I4" t="s">
         <v>129</v>
@@ -2500,11 +2703,14 @@
       <c r="J4" t="s">
         <v>5</v>
       </c>
-      <c r="N4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="L4" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="O4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="30">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2521,7 +2727,7 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I5" t="s">
         <v>129</v>
@@ -2529,14 +2735,17 @@
       <c r="J5" t="s">
         <v>5</v>
       </c>
-      <c r="M5" t="s">
+      <c r="L5" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="N5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -2553,22 +2762,25 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I6" t="s">
         <v>127</v>
       </c>
-      <c r="L6" t="s">
-        <v>246</v>
+      <c r="L6" s="4" t="s">
+        <v>322</v>
       </c>
       <c r="M6" t="s">
+        <v>326</v>
+      </c>
+      <c r="N6" t="s">
         <v>204</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2579,16 +2791,19 @@
         <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I7" t="s">
         <v>129</v>
       </c>
-      <c r="N7">
+      <c r="L7" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2605,19 +2820,22 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I8" t="s">
         <v>127</v>
       </c>
-      <c r="L8" t="s">
-        <v>247</v>
-      </c>
-      <c r="N8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="L8" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="M8" t="s">
+        <v>327</v>
+      </c>
+      <c r="O8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2634,19 +2852,22 @@
         <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I9" t="s">
         <v>127</v>
       </c>
-      <c r="L9" t="s">
-        <v>248</v>
-      </c>
-      <c r="N9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="L9" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="M9" t="s">
+        <v>328</v>
+      </c>
+      <c r="O9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2657,19 +2878,22 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I10" t="s">
         <v>129</v>
       </c>
-      <c r="M10" t="s">
-        <v>272</v>
-      </c>
-      <c r="N10">
+      <c r="L10" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="N10" t="s">
+        <v>252</v>
+      </c>
+      <c r="O10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15" ht="30">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2689,16 +2913,19 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I11" t="s">
         <v>129</v>
       </c>
-      <c r="N11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="L11" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="O11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2709,7 +2936,7 @@
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I12" t="s">
         <v>243</v>
@@ -2718,14 +2945,14 @@
         <f>IF(I12="C",1,0)</f>
         <v>1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>17</v>
       </c>
-      <c r="N12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="30">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2742,22 +2969,25 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I13" t="s">
         <v>127</v>
       </c>
-      <c r="L13" t="s">
-        <v>249</v>
+      <c r="L13" s="4" t="s">
+        <v>325</v>
       </c>
       <c r="M13" t="s">
+        <v>246</v>
+      </c>
+      <c r="N13" t="s">
         <v>134</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15" ht="30">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2780,22 +3010,25 @@
         <v>4</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I14" t="s">
         <v>127</v>
       </c>
-      <c r="L14" t="s">
-        <v>250</v>
+      <c r="L14" s="4" t="s">
+        <v>360</v>
       </c>
       <c r="M14" t="s">
+        <v>329</v>
+      </c>
+      <c r="N14" t="s">
         <v>230</v>
       </c>
-      <c r="N14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="30">
       <c r="A15" t="s">
         <v>152</v>
       </c>
@@ -2809,16 +3042,19 @@
         <v>9</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I15" t="s">
         <v>127</v>
       </c>
-      <c r="L15" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="L15" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="M15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="30">
       <c r="A16" t="s">
         <v>175</v>
       </c>
@@ -2835,22 +3071,25 @@
         <v>9</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I16" t="s">
         <v>127</v>
       </c>
-      <c r="L16" t="s">
-        <v>250</v>
+      <c r="L16" s="4" t="s">
+        <v>362</v>
       </c>
       <c r="M16" t="s">
+        <v>331</v>
+      </c>
+      <c r="N16" t="s">
         <v>206</v>
       </c>
-      <c r="N16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="30">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2867,19 +3106,22 @@
         <v>4</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I17" t="s">
         <v>129</v>
       </c>
-      <c r="M17" t="s">
+      <c r="L17" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="N17" t="s">
         <v>242</v>
       </c>
-      <c r="N17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="30">
       <c r="A18" t="s">
         <v>180</v>
       </c>
@@ -2893,22 +3135,22 @@
         <v>4</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I18" t="s">
         <v>227</v>
       </c>
-      <c r="L18" t="s">
-        <v>277</v>
-      </c>
-      <c r="M18" t="s">
+      <c r="L18" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="N18" t="s">
         <v>207</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15" ht="45">
       <c r="A19" t="s">
         <v>135</v>
       </c>
@@ -2922,22 +3164,22 @@
         <v>4</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I19" t="s">
         <v>227</v>
       </c>
-      <c r="L19" t="s">
-        <v>276</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="L19" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="N19" t="s">
         <v>208</v>
       </c>
-      <c r="N19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2951,19 +3193,22 @@
         <v>4</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I20" t="s">
         <v>129</v>
       </c>
-      <c r="M20" t="s">
+      <c r="L20" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N20" t="s">
         <v>192</v>
       </c>
-      <c r="N20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2974,22 +3219,22 @@
         <v>2</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I21" t="s">
         <v>243</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>219</v>
       </c>
-      <c r="N21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="O21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="30">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -3006,7 +3251,7 @@
         <v>25</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I22" t="s">
         <v>129</v>
@@ -3014,14 +3259,17 @@
       <c r="J22" t="s">
         <v>5</v>
       </c>
-      <c r="M22" t="s">
+      <c r="L22" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="N22" t="s">
         <v>27</v>
       </c>
-      <c r="N22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="O22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -3032,16 +3280,19 @@
         <v>2</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I23" t="s">
         <v>129</v>
       </c>
-      <c r="N23">
+      <c r="L23" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15" ht="30">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3058,7 +3309,7 @@
         <v>9</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I24" t="s">
         <v>129</v>
@@ -3066,14 +3317,17 @@
       <c r="J24" t="s">
         <v>5</v>
       </c>
-      <c r="M24" t="s">
+      <c r="L24" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="N24" t="s">
         <v>31</v>
       </c>
-      <c r="N24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="O24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -3084,19 +3338,22 @@
         <v>4</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I25" t="s">
         <v>129</v>
       </c>
-      <c r="M25" t="s">
-        <v>272</v>
-      </c>
-      <c r="N25">
+      <c r="L25" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="N25" t="s">
+        <v>252</v>
+      </c>
+      <c r="O25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -3107,19 +3364,22 @@
         <v>2</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I26" t="s">
         <v>129</v>
       </c>
-      <c r="M26" t="s">
+      <c r="L26" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N26" t="s">
         <v>209</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -3130,16 +3390,19 @@
         <v>4</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I27" t="s">
         <v>129</v>
       </c>
-      <c r="N27">
+      <c r="L27" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -3153,16 +3416,19 @@
         <v>2</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I28" t="s">
         <v>129</v>
       </c>
-      <c r="N28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="L28" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="O28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -3176,16 +3442,19 @@
         <v>2</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I29" t="s">
         <v>129</v>
       </c>
-      <c r="N29">
+      <c r="L29" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="O29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -3196,19 +3465,22 @@
         <v>4</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I30" t="s">
         <v>129</v>
       </c>
-      <c r="M30" t="s">
-        <v>272</v>
-      </c>
-      <c r="N30">
+      <c r="L30" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="N30" t="s">
+        <v>252</v>
+      </c>
+      <c r="O30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -3219,19 +3491,22 @@
         <v>4</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I31" t="s">
         <v>129</v>
       </c>
-      <c r="M31" t="s">
+      <c r="L31" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N31" t="s">
         <v>138</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3248,22 +3523,22 @@
         <v>4</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I32" t="s">
         <v>127</v>
       </c>
-      <c r="L32" t="s">
-        <v>252</v>
-      </c>
       <c r="M32" t="s">
+        <v>332</v>
+      </c>
+      <c r="N32" t="s">
         <v>229</v>
       </c>
-      <c r="N32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="O32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -3274,22 +3549,22 @@
         <v>4</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I33" t="s">
         <v>243</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>39</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>210</v>
       </c>
-      <c r="N33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="O33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -3300,16 +3575,19 @@
         <v>2</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
       </c>
-      <c r="N34">
+      <c r="L34" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:15" ht="30">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -3320,19 +3598,22 @@
         <v>4</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
       </c>
-      <c r="M35" t="s">
+      <c r="L35" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="N35" t="s">
         <v>193</v>
       </c>
-      <c r="N35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="O35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -3343,19 +3624,19 @@
         <v>2</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I36" t="s">
         <v>243</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>43</v>
       </c>
-      <c r="N36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="O36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -3366,19 +3647,22 @@
         <v>4</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I37" t="s">
         <v>129</v>
       </c>
-      <c r="M37" t="s">
+      <c r="L37" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="N37" t="s">
         <v>237</v>
       </c>
-      <c r="N37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="O37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="60">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -3395,7 +3679,7 @@
         <v>4</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I38" t="s">
         <v>129</v>
@@ -3403,14 +3687,17 @@
       <c r="J38" t="s">
         <v>5</v>
       </c>
-      <c r="M38" t="s">
+      <c r="L38" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="N38" t="s">
         <v>128</v>
       </c>
-      <c r="N38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="O38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -3421,19 +3708,19 @@
         <v>2</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I39" t="s">
         <v>243</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>46</v>
       </c>
-      <c r="N39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="O39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -3444,19 +3731,22 @@
         <v>4</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I40" t="s">
         <v>129</v>
       </c>
-      <c r="M40" t="s">
-        <v>272</v>
-      </c>
-      <c r="N40">
+      <c r="L40" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="N40" t="s">
+        <v>252</v>
+      </c>
+      <c r="O40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -3470,16 +3760,19 @@
         <v>4</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
       </c>
-      <c r="N41">
+      <c r="L41" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -3490,16 +3783,19 @@
         <v>2</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
       </c>
-      <c r="N42">
+      <c r="L42" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -3513,22 +3809,22 @@
         <v>4</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I43" t="s">
         <v>243</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>51</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>211</v>
       </c>
-      <c r="N43">
+      <c r="O43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -3539,19 +3835,22 @@
         <v>2</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I44" t="s">
         <v>129</v>
       </c>
-      <c r="M44" t="s">
+      <c r="L44" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N44" t="s">
         <v>142</v>
       </c>
-      <c r="N44">
+      <c r="O44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:15" ht="30">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -3562,19 +3861,22 @@
         <v>4</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
       </c>
-      <c r="M45" t="s">
+      <c r="L45" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="N45" t="s">
         <v>237</v>
       </c>
-      <c r="N45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="O45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="30">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3591,7 +3893,7 @@
         <v>25</v>
       </c>
       <c r="H46" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
@@ -3599,14 +3901,17 @@
       <c r="J46" t="s">
         <v>5</v>
       </c>
-      <c r="M46" t="s">
+      <c r="L46" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="N46" t="s">
         <v>143</v>
       </c>
-      <c r="N46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="O46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>131</v>
       </c>
@@ -3623,22 +3928,25 @@
         <v>4</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I47" t="s">
         <v>127</v>
       </c>
-      <c r="L47" t="s">
-        <v>253</v>
+      <c r="L47" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="M47" t="s">
+        <v>333</v>
+      </c>
+      <c r="N47" t="s">
         <v>212</v>
       </c>
-      <c r="N47">
+      <c r="O47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:15" ht="30">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -3655,19 +3963,22 @@
         <v>4</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I48" t="s">
         <v>127</v>
       </c>
-      <c r="L48" t="s">
-        <v>254</v>
-      </c>
-      <c r="N48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="L48" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="M48" t="s">
+        <v>335</v>
+      </c>
+      <c r="O48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -3684,19 +3995,22 @@
         <v>4</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I49" t="s">
         <v>127</v>
       </c>
-      <c r="L49" t="s">
-        <v>255</v>
-      </c>
-      <c r="N49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+      <c r="L49" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="M49" t="s">
+        <v>337</v>
+      </c>
+      <c r="O49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -3713,19 +4027,22 @@
         <v>4</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I50" t="s">
         <v>127</v>
       </c>
-      <c r="L50" t="s">
-        <v>256</v>
-      </c>
-      <c r="N50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="L50" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="M50" t="s">
+        <v>340</v>
+      </c>
+      <c r="O50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -3739,16 +4056,19 @@
         <v>2</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I51" t="s">
         <v>129</v>
       </c>
-      <c r="N51">
+      <c r="L51" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="O51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -3759,19 +4079,22 @@
         <v>4</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I52" t="s">
         <v>129</v>
       </c>
-      <c r="M52" t="s">
-        <v>272</v>
-      </c>
-      <c r="N52">
+      <c r="L52" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="N52" t="s">
+        <v>252</v>
+      </c>
+      <c r="O52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -3785,19 +4108,22 @@
         <v>4</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I53" t="s">
         <v>129</v>
       </c>
-      <c r="M53" t="s">
+      <c r="L53" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N53" t="s">
         <v>194</v>
       </c>
-      <c r="N53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="O53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -3811,16 +4137,19 @@
         <v>4</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I54" t="s">
         <v>129</v>
       </c>
-      <c r="N54">
+      <c r="L54" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -3831,22 +4160,22 @@
         <v>2</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I55" t="s">
         <v>243</v>
       </c>
-      <c r="L55" t="s">
+      <c r="M55" t="s">
         <v>64</v>
       </c>
-      <c r="M55" t="s">
+      <c r="N55" t="s">
         <v>214</v>
       </c>
-      <c r="N55">
+      <c r="O55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -3857,22 +4186,22 @@
         <v>2</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I56" t="s">
         <v>243</v>
       </c>
-      <c r="L56" t="s">
+      <c r="M56" t="s">
         <v>62</v>
       </c>
-      <c r="M56" t="s">
+      <c r="N56" t="s">
         <v>213</v>
       </c>
-      <c r="N56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+      <c r="O56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3886,16 +4215,19 @@
         <v>4</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I57" t="s">
         <v>129</v>
       </c>
-      <c r="N57">
+      <c r="L57" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -3906,19 +4238,19 @@
         <v>2</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I58" t="s">
         <v>243</v>
       </c>
-      <c r="L58" t="s">
+      <c r="M58" t="s">
         <v>67</v>
       </c>
-      <c r="N58">
+      <c r="O58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>69</v>
       </c>
@@ -3929,19 +4261,22 @@
         <v>4</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I59" t="s">
         <v>129</v>
       </c>
-      <c r="M59" t="s">
-        <v>272</v>
-      </c>
-      <c r="N59">
+      <c r="L59" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="N59" t="s">
+        <v>252</v>
+      </c>
+      <c r="O59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -3955,19 +4290,22 @@
         <v>2</v>
       </c>
       <c r="H60" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I60" t="s">
         <v>129</v>
       </c>
-      <c r="M60" t="s">
+      <c r="L60" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N60" t="s">
         <v>125</v>
       </c>
-      <c r="N60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+      <c r="O60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="30">
       <c r="A61" t="s">
         <v>132</v>
       </c>
@@ -3984,22 +4322,25 @@
         <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I61" t="s">
         <v>127</v>
       </c>
-      <c r="L61" t="s">
-        <v>257</v>
+      <c r="L61" s="4" t="s">
+        <v>342</v>
       </c>
       <c r="M61" t="s">
+        <v>341</v>
+      </c>
+      <c r="N61" t="s">
         <v>216</v>
       </c>
-      <c r="N61">
+      <c r="O61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -4016,16 +4357,19 @@
         <v>4</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I62" t="s">
         <v>129</v>
       </c>
-      <c r="N62">
+      <c r="L62" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>73</v>
       </c>
@@ -4039,19 +4383,22 @@
         <v>4</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I63" t="s">
         <v>129</v>
       </c>
-      <c r="M63" t="s">
+      <c r="L63" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N63" t="s">
         <v>195</v>
       </c>
-      <c r="N63" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="O63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>74</v>
       </c>
@@ -4062,22 +4409,22 @@
         <v>2</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I64" t="s">
         <v>243</v>
       </c>
-      <c r="L64" t="s">
+      <c r="M64" t="s">
         <v>73</v>
       </c>
-      <c r="M64" t="s">
+      <c r="N64" t="s">
         <v>217</v>
       </c>
-      <c r="N64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="O64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>75</v>
       </c>
@@ -4094,22 +4441,22 @@
         <v>9</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I65" t="s">
         <v>243</v>
       </c>
-      <c r="L65" t="s">
+      <c r="M65" t="s">
         <v>191</v>
       </c>
-      <c r="M65" t="s">
+      <c r="N65" t="s">
         <v>218</v>
       </c>
-      <c r="N65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="O65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -4123,16 +4470,19 @@
         <v>2</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I66" t="s">
         <v>129</v>
       </c>
-      <c r="N66">
+      <c r="L66" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O66">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -4146,25 +4496,28 @@
         <v>130</v>
       </c>
       <c r="G67" t="s">
-        <v>4</v>
+        <v>251</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I67" t="s">
         <v>127</v>
       </c>
-      <c r="L67" t="s">
-        <v>258</v>
+      <c r="L67" s="4" t="s">
+        <v>343</v>
       </c>
       <c r="M67" t="s">
+        <v>344</v>
+      </c>
+      <c r="N67" t="s">
         <v>220</v>
       </c>
-      <c r="N67">
+      <c r="O67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>78</v>
       </c>
@@ -4181,19 +4534,22 @@
         <v>4</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I68" t="s">
         <v>127</v>
       </c>
-      <c r="L68" t="s">
-        <v>259</v>
-      </c>
-      <c r="N68">
+      <c r="L68" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="M68" t="s">
+        <v>247</v>
+      </c>
+      <c r="O68">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -4207,16 +4563,19 @@
         <v>4</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I69" t="s">
         <v>129</v>
       </c>
-      <c r="N69">
+      <c r="L69" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -4227,22 +4586,22 @@
         <v>2</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I70" t="s">
         <v>243</v>
       </c>
-      <c r="L70" t="s">
+      <c r="M70" t="s">
         <v>79</v>
       </c>
-      <c r="M70" t="s">
+      <c r="N70" t="s">
         <v>221</v>
       </c>
-      <c r="N70">
+      <c r="O70">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -4253,16 +4612,19 @@
         <v>4</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I71" t="s">
         <v>129</v>
       </c>
-      <c r="N71">
+      <c r="L71" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -4273,19 +4635,19 @@
         <v>2</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I72" t="s">
         <v>243</v>
       </c>
-      <c r="L72" t="s">
+      <c r="M72" t="s">
         <v>81</v>
       </c>
-      <c r="N72">
+      <c r="O72">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>83</v>
       </c>
@@ -4302,19 +4664,22 @@
         <v>84</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I73" t="s">
         <v>127</v>
       </c>
-      <c r="L73" t="s">
-        <v>260</v>
-      </c>
-      <c r="N73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14">
+      <c r="L73" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="M73" t="s">
+        <v>346</v>
+      </c>
+      <c r="O73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -4325,22 +4690,22 @@
         <v>86</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I74" t="s">
         <v>243</v>
       </c>
-      <c r="L74" t="s">
+      <c r="M74" t="s">
         <v>39</v>
       </c>
-      <c r="M74" t="s">
+      <c r="N74" t="s">
         <v>205</v>
       </c>
-      <c r="N74" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14">
+      <c r="O74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -4351,16 +4716,19 @@
         <v>4</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I75" t="s">
         <v>129</v>
       </c>
-      <c r="N75">
+      <c r="L75" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -4371,22 +4739,22 @@
         <v>2</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I76" t="s">
         <v>243</v>
       </c>
-      <c r="L76" t="s">
+      <c r="M76" t="s">
         <v>87</v>
       </c>
-      <c r="M76" t="s">
+      <c r="N76" t="s">
         <v>222</v>
       </c>
-      <c r="N76">
+      <c r="O76">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:15" ht="30">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -4403,7 +4771,7 @@
         <v>25</v>
       </c>
       <c r="H77" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I77" t="s">
         <v>129</v>
@@ -4411,14 +4779,17 @@
       <c r="J77" t="s">
         <v>5</v>
       </c>
-      <c r="M77" t="s">
+      <c r="L77" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="N77" t="s">
         <v>91</v>
       </c>
-      <c r="N77" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14">
+      <c r="O77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>92</v>
       </c>
@@ -4432,19 +4803,22 @@
         <v>4</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I78" t="s">
         <v>129</v>
       </c>
-      <c r="M78" t="s">
-        <v>272</v>
-      </c>
-      <c r="N78">
+      <c r="L78" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="N78" t="s">
+        <v>252</v>
+      </c>
+      <c r="O78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:15" ht="30">
       <c r="A79" t="s">
         <v>93</v>
       </c>
@@ -4461,19 +4835,22 @@
         <v>4</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I79" t="s">
         <v>127</v>
       </c>
-      <c r="L79" t="s">
-        <v>261</v>
-      </c>
-      <c r="N79" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14">
+      <c r="L79" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="M79" t="s">
+        <v>349</v>
+      </c>
+      <c r="O79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>94</v>
       </c>
@@ -4484,16 +4861,19 @@
         <v>4</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I80" t="s">
         <v>129</v>
       </c>
-      <c r="N80">
+      <c r="L80" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O80">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>95</v>
       </c>
@@ -4504,22 +4884,22 @@
         <v>2</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I81" t="s">
         <v>243</v>
       </c>
-      <c r="L81" t="s">
+      <c r="M81" t="s">
         <v>94</v>
       </c>
-      <c r="M81" t="s">
+      <c r="N81" t="s">
         <v>223</v>
       </c>
-      <c r="N81">
+      <c r="O81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -4533,7 +4913,7 @@
         <v>2</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I82" t="s">
         <v>243</v>
@@ -4541,17 +4921,17 @@
       <c r="J82" t="s">
         <v>5</v>
       </c>
-      <c r="L82" t="s">
-        <v>273</v>
-      </c>
       <c r="M82" t="s">
+        <v>253</v>
+      </c>
+      <c r="N82" t="s">
         <v>224</v>
       </c>
-      <c r="N82" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14">
+      <c r="O82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -4571,7 +4951,7 @@
         <v>4</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I83" t="s">
         <v>129</v>
@@ -4579,11 +4959,14 @@
       <c r="J83" t="s">
         <v>5</v>
       </c>
-      <c r="N83" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="L83" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="O83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>97</v>
       </c>
@@ -4594,22 +4977,22 @@
         <v>4</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I84" t="s">
         <v>243</v>
       </c>
-      <c r="L84" t="s">
+      <c r="M84" t="s">
         <v>96</v>
       </c>
-      <c r="M84" t="s">
+      <c r="N84" t="s">
         <v>225</v>
       </c>
-      <c r="N84" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14">
+      <c r="O84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -4620,22 +5003,22 @@
         <v>4</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I85" t="s">
         <v>243</v>
       </c>
-      <c r="L85" t="s">
+      <c r="M85" t="s">
         <v>96</v>
       </c>
-      <c r="M85" t="s">
+      <c r="N85" t="s">
         <v>225</v>
       </c>
-      <c r="N85" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14">
+      <c r="O85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -4649,16 +5032,19 @@
         <v>4</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I86" t="s">
         <v>129</v>
       </c>
-      <c r="N86">
+      <c r="L86" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="O86">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -4669,22 +5055,22 @@
         <v>2</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I87" t="s">
         <v>243</v>
       </c>
-      <c r="L87" t="s">
+      <c r="M87" t="s">
         <v>99</v>
       </c>
-      <c r="M87" t="s">
+      <c r="N87" t="s">
         <v>226</v>
       </c>
-      <c r="N87">
+      <c r="O87">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -4698,22 +5084,22 @@
         <v>9</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I88" t="s">
         <v>243</v>
       </c>
-      <c r="L88" t="s">
+      <c r="M88" t="s">
         <v>152</v>
       </c>
-      <c r="M88" t="s">
+      <c r="N88" t="s">
         <v>228</v>
       </c>
-      <c r="N88" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14">
+      <c r="O88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -4724,19 +5110,22 @@
         <v>4</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I89" t="s">
         <v>129</v>
       </c>
-      <c r="M89" t="s">
+      <c r="L89" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N89" t="s">
         <v>238</v>
       </c>
-      <c r="N89" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14">
+      <c r="O89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="30">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -4753,7 +5142,7 @@
         <v>25</v>
       </c>
       <c r="H90" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I90" t="s">
         <v>129</v>
@@ -4761,14 +5150,17 @@
       <c r="J90" t="s">
         <v>5</v>
       </c>
-      <c r="M90" t="s">
+      <c r="L90" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="N90" t="s">
         <v>106</v>
       </c>
-      <c r="N90" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="O90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
         <v>176</v>
       </c>
@@ -4779,19 +5171,22 @@
         <v>4</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I91" t="s">
         <v>127</v>
       </c>
-      <c r="L91" t="s">
-        <v>262</v>
+      <c r="L91" s="4" t="s">
+        <v>351</v>
       </c>
       <c r="M91" t="s">
+        <v>350</v>
+      </c>
+      <c r="N91" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -4802,19 +5197,22 @@
         <v>4</v>
       </c>
       <c r="H92" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I92" t="s">
         <v>127</v>
       </c>
-      <c r="L92" t="s">
-        <v>263</v>
+      <c r="L92" s="4" t="s">
+        <v>353</v>
       </c>
       <c r="M92" t="s">
+        <v>352</v>
+      </c>
+      <c r="N92" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>178</v>
       </c>
@@ -4822,19 +5220,19 @@
         <v>4</v>
       </c>
       <c r="H93" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I93" t="s">
         <v>227</v>
       </c>
-      <c r="L93" t="s">
-        <v>274</v>
-      </c>
-      <c r="M93" t="s">
+      <c r="L93" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="N93" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:15" ht="30">
       <c r="A94" t="s">
         <v>179</v>
       </c>
@@ -4842,19 +5240,19 @@
         <v>4</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I94" t="s">
         <v>227</v>
       </c>
-      <c r="L94" t="s">
-        <v>275</v>
-      </c>
-      <c r="M94" t="s">
+      <c r="L94" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="N94" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:15" ht="30">
       <c r="A95" t="s">
         <v>181</v>
       </c>
@@ -4865,19 +5263,22 @@
         <v>4</v>
       </c>
       <c r="H95" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I95" t="s">
         <v>127</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="M95" t="s">
+        <v>354</v>
+      </c>
+      <c r="M95" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="N95" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:15" ht="30">
       <c r="A96" t="s">
         <v>182</v>
       </c>
@@ -4888,16 +5289,19 @@
         <v>4</v>
       </c>
       <c r="H96" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I96" t="s">
         <v>127</v>
       </c>
       <c r="L96" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13">
+        <v>356</v>
+      </c>
+      <c r="M96" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" t="s">
         <v>183</v>
       </c>
@@ -4908,16 +5312,14 @@
         <v>4</v>
       </c>
       <c r="H97" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I97" t="s">
         <v>127</v>
       </c>
-      <c r="L97" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="M97" s="4"/>
+    </row>
+    <row r="98" spans="1:14" ht="30">
       <c r="A98" t="s">
         <v>184</v>
       </c>
@@ -4928,16 +5330,19 @@
         <v>4</v>
       </c>
       <c r="H98" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I98" t="s">
         <v>127</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13">
+        <v>357</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="30">
       <c r="A99" t="s">
         <v>185</v>
       </c>
@@ -4945,22 +5350,23 @@
         <v>127</v>
       </c>
       <c r="G99" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="H99" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I99" t="s">
         <v>127</v>
       </c>
       <c r="L99" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="M99" t="s">
+        <v>248</v>
+      </c>
+      <c r="M99" s="4"/>
+      <c r="N99" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:14">
       <c r="A100" t="s">
         <v>188</v>
       </c>
@@ -4968,16 +5374,19 @@
         <v>4</v>
       </c>
       <c r="H100" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I100" t="s">
         <v>129</v>
       </c>
-      <c r="M100" t="s">
+      <c r="L100" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N100" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:14">
       <c r="A101" t="s">
         <v>186</v>
       </c>
@@ -4985,16 +5394,19 @@
         <v>4</v>
       </c>
       <c r="H101" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I101" t="s">
         <v>129</v>
       </c>
-      <c r="M101" t="s">
+      <c r="L101" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N101" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:14">
       <c r="A102" t="s">
         <v>187</v>
       </c>
@@ -5002,16 +5414,19 @@
         <v>4</v>
       </c>
       <c r="H102" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I102" t="s">
         <v>129</v>
       </c>
-      <c r="M102" t="s">
+      <c r="L102" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="N102" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:14">
       <c r="A103" t="s">
         <v>190</v>
       </c>
@@ -5019,13 +5434,16 @@
         <v>4</v>
       </c>
       <c r="H103" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I103" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="L103" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" ht="30">
       <c r="A104" t="s">
         <v>189</v>
       </c>
@@ -5033,10 +5451,13 @@
         <v>4</v>
       </c>
       <c r="H104" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="I104" t="s">
         <v>129</v>
+      </c>
+      <c r="L104" s="5" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -5052,6 +5473,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5065,11 +5487,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A105" sqref="A105"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5099,7 +5521,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="C2" t="s">
         <v>155</v>
@@ -5146,7 +5568,7 @@
         <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5159,7 +5581,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5167,7 +5589,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5180,7 +5602,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="D11" t="s">
         <v>239</v>
@@ -5191,7 +5613,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5199,7 +5621,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5207,7 +5629,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5215,7 +5637,7 @@
         <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5223,7 +5645,7 @@
         <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5239,7 +5661,7 @@
         <v>180</v>
       </c>
       <c r="B18" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5247,7 +5669,7 @@
         <v>135</v>
       </c>
       <c r="B19" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5263,7 +5685,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5287,7 +5709,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="C24" t="s">
         <v>157</v>
@@ -5333,7 +5755,7 @@
         <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -5341,7 +5763,7 @@
         <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -5354,7 +5776,7 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -5362,7 +5784,7 @@
         <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -5383,7 +5805,7 @@
         <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -5406,7 +5828,7 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -5435,7 +5857,7 @@
         <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -5443,7 +5865,7 @@
         <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -5471,7 +5893,7 @@
         <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -5484,7 +5906,7 @@
         <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5492,7 +5914,7 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -5505,7 +5927,7 @@
         <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -5523,7 +5945,7 @@
         <v>71</v>
       </c>
       <c r="B61" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -5536,7 +5958,7 @@
         <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -5544,7 +5966,7 @@
         <v>74</v>
       </c>
       <c r="B64" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -5552,7 +5974,7 @@
         <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -5565,7 +5987,7 @@
         <v>130</v>
       </c>
       <c r="B67" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -5573,7 +5995,7 @@
         <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -5586,7 +6008,7 @@
         <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -5599,7 +6021,7 @@
         <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -5607,7 +6029,7 @@
         <v>83</v>
       </c>
       <c r="B73" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -5615,7 +6037,7 @@
         <v>85</v>
       </c>
       <c r="B74" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -5628,7 +6050,7 @@
         <v>88</v>
       </c>
       <c r="B76" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -5649,7 +6071,7 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -5662,7 +6084,7 @@
         <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -5670,7 +6092,7 @@
         <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -5689,7 +6111,7 @@
         <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -5697,7 +6119,7 @@
         <v>98</v>
       </c>
       <c r="B85" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -5710,7 +6132,7 @@
         <v>100</v>
       </c>
       <c r="B87" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -5718,7 +6140,7 @@
         <v>101</v>
       </c>
       <c r="B88" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -5726,7 +6148,7 @@
         <v>102</v>
       </c>
       <c r="B89" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -5742,7 +6164,7 @@
         <v>176</v>
       </c>
       <c r="B91" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -5750,7 +6172,7 @@
         <v>177</v>
       </c>
       <c r="B92" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -5758,7 +6180,7 @@
         <v>178</v>
       </c>
       <c r="B93" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -5766,7 +6188,7 @@
         <v>179</v>
       </c>
       <c r="B94" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -5774,7 +6196,7 @@
         <v>181</v>
       </c>
       <c r="B95" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -5782,7 +6204,7 @@
         <v>182</v>
       </c>
       <c r="B96" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -5790,7 +6212,7 @@
         <v>183</v>
       </c>
       <c r="B97" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -5798,7 +6220,7 @@
         <v>184</v>
       </c>
       <c r="B98" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -5806,7 +6228,7 @@
         <v>185</v>
       </c>
       <c r="B99" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="1:2">

</xml_diff>

<commit_message>
Added table of all search index fields and their origin with brief descriptions.
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="1740" windowWidth="45280" windowHeight="25040" tabRatio="500"/>
+    <workbookView xWindow="4440" yWindow="3940" windowWidth="45280" windowHeight="25040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="381">
   <si>
     <t>Notes</t>
   </si>
@@ -1226,6 +1226,60 @@
   </si>
   <si>
     <t>The date and time when the object system metadata was last updated.</t>
+  </si>
+  <si>
+    <t>Copy from contactOrganization</t>
+  </si>
+  <si>
+    <t>Copy from distribution</t>
+  </si>
+  <si>
+    <t>Copy from id</t>
+  </si>
+  <si>
+    <t>Copy from investigator</t>
+  </si>
+  <si>
+    <t>Copy from keywords</t>
+  </si>
+  <si>
+    <t>Copy from manu</t>
+  </si>
+  <si>
+    <t>Copy from originator</t>
+  </si>
+  <si>
+    <t>Copy from origin</t>
+  </si>
+  <si>
+    <t>Copy from parameter</t>
+  </si>
+  <si>
+    <t>Copy from project</t>
+  </si>
+  <si>
+    <t>Copy from datePublished</t>
+  </si>
+  <si>
+    <t>Copy from sensor</t>
+  </si>
+  <si>
+    <t>Copy from site</t>
+  </si>
+  <si>
+    <t>Copy from source</t>
+  </si>
+  <si>
+    <t>Copy from term</t>
+  </si>
+  <si>
+    <t>Copy from title</t>
+  </si>
+  <si>
+    <t>Copy from topic</t>
+  </si>
+  <si>
+    <t>Copy from dateuploaded</t>
   </si>
 </sst>
 </file>
@@ -2543,10 +2597,10 @@
   <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomRight" activeCell="N88" sqref="N88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2946,7 +3000,7 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>17</v>
+        <v>363</v>
       </c>
       <c r="O12" t="s">
         <v>5</v>
@@ -3225,7 +3279,7 @@
         <v>243</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>22</v>
+        <v>364</v>
       </c>
       <c r="N21" t="s">
         <v>219</v>
@@ -3555,7 +3609,7 @@
         <v>243</v>
       </c>
       <c r="M33" t="s">
-        <v>39</v>
+        <v>365</v>
       </c>
       <c r="N33" t="s">
         <v>210</v>
@@ -3630,7 +3684,7 @@
         <v>243</v>
       </c>
       <c r="M36" t="s">
-        <v>43</v>
+        <v>366</v>
       </c>
       <c r="O36" t="s">
         <v>5</v>
@@ -3714,7 +3768,7 @@
         <v>243</v>
       </c>
       <c r="M39" t="s">
-        <v>46</v>
+        <v>367</v>
       </c>
       <c r="O39" t="s">
         <v>5</v>
@@ -3815,7 +3869,7 @@
         <v>243</v>
       </c>
       <c r="M43" t="s">
-        <v>51</v>
+        <v>368</v>
       </c>
       <c r="N43" t="s">
         <v>211</v>
@@ -4166,7 +4220,7 @@
         <v>243</v>
       </c>
       <c r="M55" t="s">
-        <v>64</v>
+        <v>369</v>
       </c>
       <c r="N55" t="s">
         <v>214</v>
@@ -4192,7 +4246,7 @@
         <v>243</v>
       </c>
       <c r="M56" t="s">
-        <v>62</v>
+        <v>370</v>
       </c>
       <c r="N56" t="s">
         <v>213</v>
@@ -4244,7 +4298,7 @@
         <v>243</v>
       </c>
       <c r="M58" t="s">
-        <v>67</v>
+        <v>371</v>
       </c>
       <c r="O58">
         <v>0</v>
@@ -4415,7 +4469,7 @@
         <v>243</v>
       </c>
       <c r="M64" t="s">
-        <v>73</v>
+        <v>372</v>
       </c>
       <c r="N64" t="s">
         <v>217</v>
@@ -4447,7 +4501,7 @@
         <v>243</v>
       </c>
       <c r="M65" t="s">
-        <v>191</v>
+        <v>373</v>
       </c>
       <c r="N65" t="s">
         <v>218</v>
@@ -4592,7 +4646,7 @@
         <v>243</v>
       </c>
       <c r="M70" t="s">
-        <v>79</v>
+        <v>374</v>
       </c>
       <c r="N70" t="s">
         <v>221</v>
@@ -4641,7 +4695,7 @@
         <v>243</v>
       </c>
       <c r="M72" t="s">
-        <v>81</v>
+        <v>375</v>
       </c>
       <c r="O72">
         <v>0</v>
@@ -4696,7 +4750,7 @@
         <v>243</v>
       </c>
       <c r="M74" t="s">
-        <v>39</v>
+        <v>365</v>
       </c>
       <c r="N74" t="s">
         <v>205</v>
@@ -4745,7 +4799,7 @@
         <v>243</v>
       </c>
       <c r="M76" t="s">
-        <v>87</v>
+        <v>376</v>
       </c>
       <c r="N76" t="s">
         <v>222</v>
@@ -4890,7 +4944,7 @@
         <v>243</v>
       </c>
       <c r="M81" t="s">
-        <v>94</v>
+        <v>377</v>
       </c>
       <c r="N81" t="s">
         <v>223</v>
@@ -4983,7 +5037,7 @@
         <v>243</v>
       </c>
       <c r="M84" t="s">
-        <v>96</v>
+        <v>378</v>
       </c>
       <c r="N84" t="s">
         <v>225</v>
@@ -5009,7 +5063,7 @@
         <v>243</v>
       </c>
       <c r="M85" t="s">
-        <v>96</v>
+        <v>378</v>
       </c>
       <c r="N85" t="s">
         <v>225</v>
@@ -5061,7 +5115,7 @@
         <v>243</v>
       </c>
       <c r="M87" t="s">
-        <v>99</v>
+        <v>379</v>
       </c>
       <c r="N87" t="s">
         <v>226</v>
@@ -5090,7 +5144,7 @@
         <v>243</v>
       </c>
       <c r="M88" t="s">
-        <v>152</v>
+        <v>380</v>
       </c>
       <c r="N88" t="s">
         <v>228</v>

</xml_diff>

<commit_message>
Working through search index documentation. Incomplete.
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="8760" windowWidth="50240" windowHeight="18880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="360">
   <si>
     <t>Notes</t>
   </si>
@@ -713,9 +713,6 @@
     <t>copyfield from project</t>
   </si>
   <si>
-    <t>set as copyfield from datePublished</t>
-  </si>
-  <si>
     <t>was replicationAllowed</t>
   </si>
   <si>
@@ -1115,54 +1112,6 @@
     <t>The date and time when the object system metadata was last updated.</t>
   </si>
   <si>
-    <t>Copy from contactOrganization</t>
-  </si>
-  <si>
-    <t>Copy from id</t>
-  </si>
-  <si>
-    <t>Copy from investigator</t>
-  </si>
-  <si>
-    <t>Copy from keywords</t>
-  </si>
-  <si>
-    <t>Copy from originator</t>
-  </si>
-  <si>
-    <t>Copy from origin</t>
-  </si>
-  <si>
-    <t>Copy from parameter</t>
-  </si>
-  <si>
-    <t>Copy from project</t>
-  </si>
-  <si>
-    <t>Copy from datePublished</t>
-  </si>
-  <si>
-    <t>Copy from sensor</t>
-  </si>
-  <si>
-    <t>Copy from site</t>
-  </si>
-  <si>
-    <t>Copy from source</t>
-  </si>
-  <si>
-    <t>Copy from term</t>
-  </si>
-  <si>
-    <t>Copy from title</t>
-  </si>
-  <si>
-    <t>Copy from topic</t>
-  </si>
-  <si>
-    <t>Copy from dateuploaded</t>
-  </si>
-  <si>
     <t>The version or edition number of the item described.</t>
   </si>
   <si>
@@ -1224,6 +1173,63 @@
   </si>
   <si>
     <t>:term:`Public User`</t>
+  </si>
+  <si>
+    <t>systemMetadata/obsoletedBy/text()</t>
+  </si>
+  <si>
+    <t>systemMetadata/obsoletes/text()</t>
+  </si>
+  <si>
+    <t>The identifier of the object being indexed.</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.id`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.investigator`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.contactOrganization`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.keywords`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.originator`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.origin`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.parameter`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.project`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.sensor`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.site`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.source`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.term`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.title`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.topic`</t>
+  </si>
+  <si>
+    <t>Copy from :attr:`~SearchMetadata.dateuploaded`</t>
+  </si>
+  <si>
+    <t>Contains the :func:`CNRead.resolve` URL for the object ONLY if the object is a science metadata object.</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1312,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="520">
+  <cellStyleXfs count="550">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1716,6 +1722,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1842,7 +1878,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="520">
+  <cellStyles count="550">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2110,6 +2146,21 @@
     <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2362,6 +2413,21 @@
     <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -2734,11 +2800,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2760,22 +2826,22 @@
         <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
         <v>148</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30">
@@ -2786,13 +2852,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
         <v>115</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -2806,13 +2872,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
         <v>115</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
         <v>184</v>
@@ -2829,13 +2895,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>115</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -2849,13 +2915,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
         <v>115</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -2872,16 +2938,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D6" t="s">
         <v>113</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G6" t="s">
         <v>175</v>
@@ -2898,16 +2964,16 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
         <v>113</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
@@ -2921,16 +2987,16 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D8" t="s">
         <v>113</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H8" t="s">
         <v>5</v>
@@ -2944,16 +3010,16 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D9" t="s">
         <v>115</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2967,13 +3033,13 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s">
         <v>115</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
@@ -2987,13 +3053,13 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>207</v>
-      </c>
-      <c r="F11" t="s">
-        <v>321</v>
+        <v>206</v>
+      </c>
+      <c r="E11" t="s">
+        <v>346</v>
       </c>
       <c r="H11" t="s">
         <v>5</v>
@@ -3007,16 +3073,16 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D12" t="s">
         <v>113</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G12" t="s">
         <v>120</v>
@@ -3033,19 +3099,19 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D13" t="s">
         <v>113</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H13" t="s">
         <v>5</v>
@@ -3059,16 +3125,16 @@
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D14" t="s">
         <v>113</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30">
@@ -3079,16 +3145,16 @@
         <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D15" t="s">
         <v>113</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G15" t="s">
         <v>177</v>
@@ -3105,16 +3171,16 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
         <v>115</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H16" t="s">
         <v>5</v>
@@ -3128,13 +3194,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G17" t="s">
         <v>178</v>
@@ -3151,13 +3217,13 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G18" t="s">
         <v>179</v>
@@ -3174,13 +3240,13 @@
         <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D19" t="s">
         <v>115</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G19" t="s">
         <v>23</v>
@@ -3197,13 +3263,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D20" t="s">
         <v>115</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -3217,13 +3283,13 @@
         <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D21" t="s">
         <v>115</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G21" t="s">
         <v>27</v>
@@ -3240,22 +3306,22 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D22" t="s">
         <v>115</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="30">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -3263,13 +3329,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D23" t="s">
         <v>115</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>256</v>
+        <v>359</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3283,13 +3349,13 @@
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D24" t="s">
         <v>115</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H24" t="s">
         <v>5</v>
@@ -3303,13 +3369,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D25" t="s">
         <v>115</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -3323,16 +3389,16 @@
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D26" t="s">
         <v>115</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -3346,13 +3412,13 @@
         <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D27" t="s">
         <v>115</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="G27" t="s">
         <v>122</v>
@@ -3369,16 +3435,19 @@
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D28" t="s">
         <v>113</v>
       </c>
+      <c r="E28" s="3" t="s">
+        <v>343</v>
+      </c>
       <c r="F28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H28" t="s">
         <v>5</v>
@@ -3392,13 +3461,13 @@
         <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D29" t="s">
-        <v>207</v>
-      </c>
-      <c r="F29" t="s">
-        <v>322</v>
+        <v>206</v>
+      </c>
+      <c r="E29" t="s">
+        <v>344</v>
       </c>
       <c r="G29" t="s">
         <v>180</v>
@@ -3415,13 +3484,13 @@
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D30" t="s">
         <v>115</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G30" t="s">
         <v>165</v>
@@ -3438,13 +3507,13 @@
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D31" t="s">
-        <v>207</v>
-      </c>
-      <c r="F31" t="s">
-        <v>323</v>
+        <v>206</v>
+      </c>
+      <c r="E31" t="s">
+        <v>345</v>
       </c>
       <c r="H31" t="s">
         <v>5</v>
@@ -3458,16 +3527,16 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D32" t="s">
         <v>115</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H32" t="s">
         <v>5</v>
@@ -3481,13 +3550,13 @@
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D33" t="s">
         <v>115</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G33" t="s">
         <v>114</v>
@@ -3504,13 +3573,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D34" t="s">
-        <v>207</v>
-      </c>
-      <c r="F34" t="s">
-        <v>324</v>
+        <v>206</v>
+      </c>
+      <c r="E34" t="s">
+        <v>347</v>
       </c>
       <c r="H34" t="s">
         <v>5</v>
@@ -3524,16 +3593,16 @@
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D35" t="s">
         <v>115</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -3547,13 +3616,13 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D36" t="s">
         <v>115</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3567,16 +3636,16 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D37" t="s">
         <v>115</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H37" t="s">
         <v>5</v>
@@ -3590,13 +3659,13 @@
         <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D38" t="s">
         <v>115</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G38" t="s">
         <v>126</v>
@@ -3613,16 +3682,16 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D39" t="s">
         <v>113</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F39" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G39" t="s">
         <v>181</v>
@@ -3639,16 +3708,16 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D40" t="s">
         <v>113</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H40" t="s">
         <v>5</v>
@@ -3662,16 +3731,16 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D41" t="s">
         <v>113</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H41" t="s">
         <v>5</v>
@@ -3685,16 +3754,16 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D42" t="s">
         <v>113</v>
       </c>
       <c r="E42" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F42" t="s">
         <v>297</v>
-      </c>
-      <c r="F42" t="s">
-        <v>298</v>
       </c>
       <c r="H42" t="s">
         <v>5</v>
@@ -3708,13 +3777,13 @@
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D43" t="s">
         <v>115</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3728,16 +3797,16 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D44" t="s">
         <v>115</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3751,13 +3820,13 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D45" t="s">
         <v>115</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="G45" t="s">
         <v>166</v>
@@ -3774,13 +3843,13 @@
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D46" t="s">
         <v>115</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3794,13 +3863,13 @@
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D47" t="s">
-        <v>207</v>
-      </c>
-      <c r="F47" t="s">
-        <v>325</v>
+        <v>206</v>
+      </c>
+      <c r="E47" t="s">
+        <v>348</v>
       </c>
       <c r="G47" t="s">
         <v>183</v>
@@ -3817,13 +3886,13 @@
         <v>2</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D48" t="s">
-        <v>207</v>
-      </c>
-      <c r="F48" t="s">
-        <v>326</v>
+        <v>206</v>
+      </c>
+      <c r="E48" t="s">
+        <v>349</v>
       </c>
       <c r="G48" t="s">
         <v>182</v>
@@ -3840,13 +3909,13 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D49" t="s">
         <v>115</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -3860,13 +3929,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D50" t="s">
-        <v>207</v>
-      </c>
-      <c r="F50" t="s">
-        <v>327</v>
+        <v>206</v>
+      </c>
+      <c r="E50" t="s">
+        <v>350</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3880,16 +3949,16 @@
         <v>4</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D51" t="s">
         <v>115</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -3903,13 +3972,13 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D52" t="s">
         <v>115</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="G52" t="s">
         <v>111</v>
@@ -3926,16 +3995,16 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D53" t="s">
         <v>113</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G53" t="s">
         <v>185</v>
@@ -3952,13 +4021,13 @@
         <v>4</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D54" t="s">
         <v>115</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3972,13 +4041,13 @@
         <v>4</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D55" t="s">
         <v>115</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="G55" t="s">
         <v>167</v>
@@ -3995,13 +4064,13 @@
         <v>2</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D56" t="s">
-        <v>207</v>
-      </c>
-      <c r="F56" t="s">
-        <v>328</v>
+        <v>206</v>
+      </c>
+      <c r="E56" t="s">
+        <v>351</v>
       </c>
       <c r="G56" t="s">
         <v>186</v>
@@ -4018,19 +4087,13 @@
         <v>9</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D57" t="s">
         <v>115</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="F57" t="s">
-        <v>329</v>
-      </c>
-      <c r="G57" t="s">
-        <v>187</v>
+        <v>339</v>
       </c>
       <c r="H57" t="s">
         <v>5</v>
@@ -4044,13 +4107,13 @@
         <v>2</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D58" t="s">
         <v>115</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4061,22 +4124,22 @@
         <v>116</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D59" t="s">
         <v>113</v>
       </c>
       <c r="E59" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F59" t="s">
         <v>301</v>
       </c>
-      <c r="F59" t="s">
-        <v>302</v>
-      </c>
       <c r="G59" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -4090,16 +4153,16 @@
         <v>4</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D60" t="s">
         <v>113</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -4113,13 +4176,13 @@
         <v>4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D61" t="s">
         <v>115</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -4133,16 +4196,16 @@
         <v>2</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D62" t="s">
-        <v>207</v>
-      </c>
-      <c r="F62" t="s">
-        <v>330</v>
+        <v>206</v>
+      </c>
+      <c r="E62" t="s">
+        <v>352</v>
       </c>
       <c r="G62" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -4156,13 +4219,13 @@
         <v>4</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D63" t="s">
         <v>115</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -4176,13 +4239,13 @@
         <v>2</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D64" t="s">
-        <v>207</v>
-      </c>
-      <c r="F64" t="s">
-        <v>331</v>
+        <v>206</v>
+      </c>
+      <c r="E64" t="s">
+        <v>353</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -4196,16 +4259,16 @@
         <v>72</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D65" t="s">
         <v>113</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F65" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H65" t="s">
         <v>5</v>
@@ -4219,13 +4282,13 @@
         <v>74</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D66" t="s">
-        <v>207</v>
-      </c>
-      <c r="F66" t="s">
-        <v>322</v>
+        <v>206</v>
+      </c>
+      <c r="E66" t="s">
+        <v>344</v>
       </c>
       <c r="G66" t="s">
         <v>176</v>
@@ -4242,13 +4305,13 @@
         <v>4</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D67" t="s">
         <v>115</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -4262,16 +4325,16 @@
         <v>2</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D68" t="s">
-        <v>207</v>
-      </c>
-      <c r="F68" t="s">
-        <v>332</v>
+        <v>206</v>
+      </c>
+      <c r="E68" t="s">
+        <v>354</v>
       </c>
       <c r="G68" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -4285,13 +4348,13 @@
         <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D69" t="s">
         <v>115</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G69" t="s">
         <v>79</v>
@@ -4308,16 +4371,16 @@
         <v>4</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D70" t="s">
         <v>115</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G70" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -4331,16 +4394,16 @@
         <v>4</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D71" t="s">
         <v>113</v>
       </c>
       <c r="E71" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="F71" t="s">
         <v>306</v>
-      </c>
-      <c r="F71" t="s">
-        <v>307</v>
       </c>
       <c r="H71" t="s">
         <v>5</v>
@@ -4354,13 +4417,13 @@
         <v>4</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D72" t="s">
         <v>115</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4374,16 +4437,16 @@
         <v>2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D73" t="s">
-        <v>207</v>
-      </c>
-      <c r="F73" t="s">
-        <v>333</v>
+        <v>206</v>
+      </c>
+      <c r="E73" t="s">
+        <v>355</v>
       </c>
       <c r="G73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -4397,16 +4460,16 @@
         <v>2</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D74" t="s">
-        <v>207</v>
-      </c>
-      <c r="F74" t="s">
-        <v>217</v>
+        <v>206</v>
+      </c>
+      <c r="E74" t="s">
+        <v>216</v>
       </c>
       <c r="G74" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H74" t="s">
         <v>5</v>
@@ -4420,13 +4483,13 @@
         <v>4</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D75" t="s">
         <v>115</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H75" t="s">
         <v>5</v>
@@ -4440,16 +4503,16 @@
         <v>4</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D76" t="s">
-        <v>207</v>
-      </c>
-      <c r="F76" t="s">
-        <v>334</v>
+        <v>206</v>
+      </c>
+      <c r="E76" t="s">
+        <v>356</v>
       </c>
       <c r="G76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H76" t="s">
         <v>5</v>
@@ -4463,16 +4526,16 @@
         <v>4</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D77" t="s">
-        <v>207</v>
-      </c>
-      <c r="F77" t="s">
-        <v>334</v>
+        <v>206</v>
+      </c>
+      <c r="E77" t="s">
+        <v>356</v>
       </c>
       <c r="G77" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H77" t="s">
         <v>5</v>
@@ -4486,13 +4549,13 @@
         <v>4</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D78" t="s">
         <v>115</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -4506,16 +4569,16 @@
         <v>2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D79" t="s">
-        <v>207</v>
-      </c>
-      <c r="F79" t="s">
-        <v>335</v>
+        <v>206</v>
+      </c>
+      <c r="E79" t="s">
+        <v>357</v>
       </c>
       <c r="G79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -4529,16 +4592,16 @@
         <v>9</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D80" t="s">
-        <v>207</v>
-      </c>
-      <c r="F80" t="s">
-        <v>336</v>
+        <v>206</v>
+      </c>
+      <c r="E80" t="s">
+        <v>358</v>
       </c>
       <c r="G80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H80" t="s">
         <v>5</v>
@@ -4552,16 +4615,16 @@
         <v>4</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D81" t="s">
         <v>115</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="G81" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H81" t="s">
         <v>5</v>
@@ -4575,13 +4638,13 @@
         <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D82" t="s">
         <v>115</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G82" t="s">
         <v>94</v>
@@ -4598,16 +4661,16 @@
         <v>4</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D83" t="s">
         <v>113</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F83" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G83" t="s">
         <v>173</v>
@@ -4621,16 +4684,16 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D84" t="s">
         <v>113</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F84" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G84" t="s">
         <v>172</v>
@@ -4644,16 +4707,16 @@
         <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D85" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="30">
@@ -4664,13 +4727,13 @@
         <v>4</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D86" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G86" t="s">
         <v>174</v>
@@ -4684,16 +4747,16 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D87" t="s">
         <v>113</v>
       </c>
       <c r="E87" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>312</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="G87" t="s">
         <v>168</v>
@@ -4707,16 +4770,16 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D88" t="s">
         <v>113</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4727,7 +4790,7 @@
         <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D89" t="s">
         <v>113</v>
@@ -4742,16 +4805,16 @@
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D90" t="s">
         <v>113</v>
       </c>
       <c r="E90" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="30">
@@ -4759,16 +4822,16 @@
         <v>160</v>
       </c>
       <c r="B91" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C91" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D91" t="s">
         <v>113</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" t="s">
@@ -4783,13 +4846,13 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D92" t="s">
         <v>115</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G92" t="s">
         <v>170</v>
@@ -4803,13 +4866,13 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D93" t="s">
         <v>115</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G93" t="s">
         <v>171</v>
@@ -4823,13 +4886,13 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D94" t="s">
         <v>115</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="30">
@@ -4840,13 +4903,13 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D95" t="s">
         <v>115</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4873,8 +4936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4892,10 +4955,10 @@
         <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -4909,13 +4972,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4926,13 +4989,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4943,13 +5006,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4960,13 +5023,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4977,13 +5040,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4994,13 +5057,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5011,13 +5074,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5028,13 +5091,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5045,13 +5108,13 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5062,13 +5125,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5079,10 +5142,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="D12" t="s">
+        <v>341</v>
       </c>
       <c r="E12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -5093,10 +5159,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="D13" t="s">
+        <v>342</v>
       </c>
       <c r="E13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5107,13 +5176,13 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -5121,16 +5190,16 @@
         <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -5141,13 +5210,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5158,13 +5227,13 @@
         <v>72</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5175,13 +5244,13 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5192,13 +5261,13 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5209,13 +5278,13 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5226,13 +5295,13 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5243,13 +5312,13 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
@@ -5260,13 +5329,13 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5274,16 +5343,16 @@
         <v>160</v>
       </c>
       <c r="B24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -5322,10 +5391,10 @@
         <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -5339,7 +5408,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -5352,7 +5421,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -5365,7 +5434,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5376,7 +5445,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5428,10 +5497,10 @@
         <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>146</v>
@@ -5448,10 +5517,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E2" t="s">
         <v>137</v>
@@ -5465,7 +5534,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
         <v>141</v>
@@ -5474,7 +5543,7 @@
         <v>142</v>
       </c>
       <c r="F3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5485,7 +5554,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>140</v>
@@ -5502,7 +5571,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
         <v>138</v>
@@ -5519,7 +5588,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5530,13 +5599,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5547,10 +5616,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5561,7 +5630,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D9" t="s">
         <v>128</v>
@@ -5578,7 +5647,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5589,10 +5658,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E11" t="s">
         <v>139</v>
@@ -5606,7 +5675,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5617,7 +5686,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5628,7 +5697,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5639,7 +5708,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -5650,7 +5719,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5661,7 +5730,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5672,10 +5741,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5686,7 +5755,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5697,7 +5766,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D20" t="s">
         <v>125</v>
@@ -5711,7 +5780,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5722,7 +5791,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5733,7 +5802,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5744,7 +5813,7 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D24" t="s">
         <v>127</v>
@@ -5761,7 +5830,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5772,7 +5841,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -5783,10 +5852,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5797,7 +5866,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -5808,7 +5877,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5819,7 +5888,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5830,7 +5899,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -5841,7 +5910,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -5852,10 +5921,10 @@
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -5866,10 +5935,10 @@
         <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -5880,7 +5949,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -5891,7 +5960,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -5902,7 +5971,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -5913,7 +5982,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -5924,7 +5993,7 @@
         <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D39" t="s">
         <v>129</v>
@@ -5938,7 +6007,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -5949,7 +6018,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -5960,7 +6029,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D42" t="s">
         <v>131</v>
@@ -5977,7 +6046,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -5988,10 +6057,10 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6002,7 +6071,7 @@
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D45" t="s">
         <v>130</v>
@@ -6016,7 +6085,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -6027,7 +6096,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -6038,7 +6107,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -6049,7 +6118,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -6087,10 +6156,10 @@
         <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -6107,7 +6176,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -6121,7 +6190,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6132,7 +6201,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6143,7 +6212,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -6157,7 +6226,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6168,7 +6237,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
         <v>96</v>
@@ -6182,7 +6251,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6193,7 +6262,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -6207,7 +6276,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s">
         <v>97</v>
@@ -6221,7 +6290,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
@@ -6235,7 +6304,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -6246,7 +6315,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D13" t="s">
         <v>98</v>
@@ -6260,7 +6329,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -6271,7 +6340,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
@@ -6285,7 +6354,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -6296,7 +6365,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D17" t="s">
         <v>99</v>
@@ -6310,7 +6379,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D18" t="s">
         <v>100</v>
@@ -6324,7 +6393,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -6335,7 +6404,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D20" t="s">
         <v>40</v>
@@ -6349,7 +6418,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -6360,10 +6429,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -6374,7 +6443,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -6385,7 +6454,7 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
@@ -6399,7 +6468,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D25" t="s">
         <v>101</v>
@@ -6413,7 +6482,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -6424,7 +6493,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D27" t="s">
         <v>52</v>
@@ -6438,7 +6507,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D28" t="s">
         <v>102</v>
@@ -6452,7 +6521,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D29" t="s">
         <v>103</v>
@@ -6466,7 +6535,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -6477,10 +6546,10 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -6491,7 +6560,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -6502,7 +6571,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D33" t="s">
         <v>104</v>
@@ -6516,7 +6585,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D34" t="s">
         <v>64</v>
@@ -6530,7 +6599,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D35" t="s">
         <v>105</v>
@@ -6544,7 +6613,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D36" t="s">
         <v>106</v>
@@ -6558,7 +6627,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D37" t="s">
         <v>108</v>
@@ -6572,7 +6641,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D38" t="s">
         <v>107</v>
@@ -6586,7 +6655,7 @@
         <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D39" t="s">
         <v>78</v>
@@ -6600,7 +6669,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -6611,7 +6680,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D41" t="s">
         <v>109</v>
@@ -6625,7 +6694,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D42" t="s">
         <v>92</v>
@@ -6639,7 +6708,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D43" t="s">
         <v>110</v>
@@ -6653,7 +6722,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D44" t="s">
         <v>95</v>
@@ -6667,7 +6736,7 @@
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D45" t="s">
         <v>93</v>
@@ -6681,7 +6750,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -6692,7 +6761,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -6703,7 +6772,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -6714,7 +6783,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -6751,10 +6820,10 @@
         <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -6771,7 +6840,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6782,7 +6851,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6793,7 +6862,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6804,7 +6873,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6815,7 +6884,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6826,7 +6895,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6837,7 +6906,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6848,7 +6917,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6859,7 +6928,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6870,7 +6939,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6881,7 +6950,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -6892,7 +6961,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -6903,7 +6972,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -6914,7 +6983,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -6925,7 +6994,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -6936,7 +7005,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -6947,7 +7016,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D18" t="s">
         <v>123</v>
@@ -6961,7 +7030,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -6972,7 +7041,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D20" t="s">
         <v>124</v>
@@ -6986,7 +7055,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -6997,7 +7066,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -7008,7 +7077,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -7019,7 +7088,7 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -7030,7 +7099,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -7041,7 +7110,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -7052,7 +7121,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D27" t="s">
         <v>123</v>
@@ -7066,7 +7135,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -7077,7 +7146,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -7088,7 +7157,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -7099,7 +7168,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -7110,7 +7179,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -7121,7 +7190,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -7132,7 +7201,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -7143,7 +7212,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -7154,7 +7223,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -7165,7 +7234,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -7176,7 +7245,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -7187,7 +7256,7 @@
         <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -7198,7 +7267,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -7209,7 +7278,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -7220,7 +7289,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D42" t="s">
         <v>132</v>
@@ -7234,7 +7303,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -7245,7 +7314,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D44" t="s">
         <v>133</v>
@@ -7259,7 +7328,7 @@
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -7270,7 +7339,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -7281,7 +7350,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -7292,7 +7361,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -7303,7 +7372,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated eml sheet wrt updated solr schema generation rules to provide items previously not present in solr schema that had xPath definitions defined here (investigator,origin,project,etc).  Task #2254
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="24700" windowHeight="19460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -848,27 +848,15 @@
     <t>systemMetadata/identifier/text()</t>
   </si>
   <si>
-    <t>RULE NOT PRESENT IN INDEX PROCESSING - //eml:eml/dataset/creator/individualName/surName/text()</t>
-  </si>
-  <si>
     <t>systemMetadata/replicationPolicy/@numberReplicas</t>
   </si>
   <si>
     <t>systemMetadata/formatId/text()</t>
   </si>
   <si>
-    <t>RULE NOT PRESENT IN INDEX PROCESSING - concat (//eml:eml/ dataset/ creator/ individualName/ givenName /text(),' ',//eml:eml/ dataset/ creator/ individualName/ surName /text())</t>
-  </si>
-  <si>
     <t>systemMetadata/replicationPolicy/preferredMemberNode/text()</t>
   </si>
   <si>
-    <t>RULE NOT PRESENT IN INDEX PROCESSING - //eml:eml/ dataset/ project/ title/text()</t>
-  </si>
-  <si>
-    <t>RULE NOT PRESENT IN INDEX PROCESSING - //dataset/pubDate/text()</t>
-  </si>
-  <si>
     <t>systemMetadata/replicationPolicy/@replicationAllowed</t>
   </si>
   <si>
@@ -1230,6 +1218,18 @@
   </si>
   <si>
     <t>Contains the :func:`CNRead.resolve` URL for the object ONLY if the object is a science metadata object.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //eml:eml/dataset/creator/individualName/surName/text()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //eml:eml/ dataset/ project/ title/text()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //dataset/pubDate/text()</t>
+  </si>
+  <si>
+    <t>(//eml:eml/ dataset/ creator/ individualName/ givenName /text(),' ',//eml:eml/ dataset/ creator/ individualName/ surName /text())</t>
   </si>
 </sst>
 </file>
@@ -2800,7 +2800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -2832,7 +2832,7 @@
         <v>148</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F1" t="s">
         <v>208</v>
@@ -2858,7 +2858,7 @@
         <v>115</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -2878,7 +2878,7 @@
         <v>115</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G3" t="s">
         <v>184</v>
@@ -2901,7 +2901,7 @@
         <v>115</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -2921,7 +2921,7 @@
         <v>115</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -2944,10 +2944,10 @@
         <v>113</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F6" t="s">
         <v>279</v>
-      </c>
-      <c r="F6" t="s">
-        <v>283</v>
       </c>
       <c r="G6" t="s">
         <v>175</v>
@@ -2970,10 +2970,10 @@
         <v>113</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
@@ -2993,10 +2993,10 @@
         <v>113</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H8" t="s">
         <v>5</v>
@@ -3016,7 +3016,7 @@
         <v>115</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G9" t="s">
         <v>215</v>
@@ -3039,7 +3039,7 @@
         <v>115</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
@@ -3059,7 +3059,7 @@
         <v>206</v>
       </c>
       <c r="E11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="H11" t="s">
         <v>5</v>
@@ -3079,7 +3079,7 @@
         <v>113</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F12" t="s">
         <v>209</v>
@@ -3105,10 +3105,10 @@
         <v>113</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F13" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="G13" t="s">
         <v>197</v>
@@ -3131,10 +3131,10 @@
         <v>113</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F14" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30">
@@ -3151,10 +3151,10 @@
         <v>113</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F15" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G15" t="s">
         <v>177</v>
@@ -3177,7 +3177,7 @@
         <v>115</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G16" t="s">
         <v>205</v>
@@ -3246,7 +3246,7 @@
         <v>115</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G19" t="s">
         <v>23</v>
@@ -3269,7 +3269,7 @@
         <v>115</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -3289,7 +3289,7 @@
         <v>115</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G21" t="s">
         <v>27</v>
@@ -3312,7 +3312,7 @@
         <v>115</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G22" t="s">
         <v>215</v>
@@ -3335,7 +3335,7 @@
         <v>115</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3355,7 +3355,7 @@
         <v>115</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H24" t="s">
         <v>5</v>
@@ -3375,7 +3375,7 @@
         <v>115</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -3395,7 +3395,7 @@
         <v>115</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G26" t="s">
         <v>215</v>
@@ -3418,7 +3418,7 @@
         <v>115</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G27" t="s">
         <v>122</v>
@@ -3441,10 +3441,10 @@
         <v>113</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F28" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G28" t="s">
         <v>196</v>
@@ -3467,7 +3467,7 @@
         <v>206</v>
       </c>
       <c r="E29" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G29" t="s">
         <v>180</v>
@@ -3490,7 +3490,7 @@
         <v>115</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G30" t="s">
         <v>165</v>
@@ -3513,7 +3513,7 @@
         <v>206</v>
       </c>
       <c r="E31" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="H31" t="s">
         <v>5</v>
@@ -3533,7 +3533,7 @@
         <v>115</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G32" t="s">
         <v>200</v>
@@ -3556,7 +3556,7 @@
         <v>115</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G33" t="s">
         <v>114</v>
@@ -3579,7 +3579,7 @@
         <v>206</v>
       </c>
       <c r="E34" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="H34" t="s">
         <v>5</v>
@@ -3599,7 +3599,7 @@
         <v>115</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G35" t="s">
         <v>215</v>
@@ -3622,7 +3622,7 @@
         <v>115</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3642,7 +3642,7 @@
         <v>115</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G37" t="s">
         <v>200</v>
@@ -3665,7 +3665,7 @@
         <v>115</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G38" t="s">
         <v>126</v>
@@ -3688,10 +3688,10 @@
         <v>113</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F39" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G39" t="s">
         <v>181</v>
@@ -3714,10 +3714,10 @@
         <v>113</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F40" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="H40" t="s">
         <v>5</v>
@@ -3737,10 +3737,10 @@
         <v>113</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F41" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H41" t="s">
         <v>5</v>
@@ -3760,10 +3760,10 @@
         <v>113</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F42" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="H42" t="s">
         <v>5</v>
@@ -3783,7 +3783,7 @@
         <v>115</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3803,7 +3803,7 @@
         <v>115</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G44" t="s">
         <v>215</v>
@@ -3826,7 +3826,7 @@
         <v>115</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G45" t="s">
         <v>166</v>
@@ -3849,7 +3849,7 @@
         <v>115</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3869,7 +3869,7 @@
         <v>206</v>
       </c>
       <c r="E47" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G47" t="s">
         <v>183</v>
@@ -3892,7 +3892,7 @@
         <v>206</v>
       </c>
       <c r="E48" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G48" t="s">
         <v>182</v>
@@ -3915,7 +3915,7 @@
         <v>115</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -3935,7 +3935,7 @@
         <v>206</v>
       </c>
       <c r="E50" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3955,7 +3955,7 @@
         <v>115</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G51" t="s">
         <v>215</v>
@@ -3978,7 +3978,7 @@
         <v>115</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G52" t="s">
         <v>111</v>
@@ -4001,10 +4001,10 @@
         <v>113</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F53" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G53" t="s">
         <v>185</v>
@@ -4027,7 +4027,7 @@
         <v>115</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -4047,7 +4047,7 @@
         <v>115</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G55" t="s">
         <v>167</v>
@@ -4070,7 +4070,7 @@
         <v>206</v>
       </c>
       <c r="E56" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G56" t="s">
         <v>186</v>
@@ -4093,7 +4093,7 @@
         <v>115</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H57" t="s">
         <v>5</v>
@@ -4113,7 +4113,7 @@
         <v>115</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4133,10 +4133,10 @@
         <v>113</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F59" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G59" t="s">
         <v>187</v>
@@ -4159,7 +4159,7 @@
         <v>113</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F60" t="s">
         <v>210</v>
@@ -4182,7 +4182,7 @@
         <v>115</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -4202,7 +4202,7 @@
         <v>206</v>
       </c>
       <c r="E62" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G62" t="s">
         <v>188</v>
@@ -4225,7 +4225,7 @@
         <v>115</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -4245,7 +4245,7 @@
         <v>206</v>
       </c>
       <c r="E64" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -4265,10 +4265,10 @@
         <v>113</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F65" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="H65" t="s">
         <v>5</v>
@@ -4288,7 +4288,7 @@
         <v>206</v>
       </c>
       <c r="E66" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G66" t="s">
         <v>176</v>
@@ -4311,7 +4311,7 @@
         <v>115</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -4331,7 +4331,7 @@
         <v>206</v>
       </c>
       <c r="E68" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G68" t="s">
         <v>189</v>
@@ -4354,7 +4354,7 @@
         <v>115</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G69" t="s">
         <v>79</v>
@@ -4377,7 +4377,7 @@
         <v>115</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="G70" t="s">
         <v>215</v>
@@ -4400,10 +4400,10 @@
         <v>113</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F71" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="H71" t="s">
         <v>5</v>
@@ -4423,7 +4423,7 @@
         <v>115</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4443,7 +4443,7 @@
         <v>206</v>
       </c>
       <c r="E73" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G73" t="s">
         <v>190</v>
@@ -4489,7 +4489,7 @@
         <v>115</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H75" t="s">
         <v>5</v>
@@ -4509,7 +4509,7 @@
         <v>206</v>
       </c>
       <c r="E76" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G76" t="s">
         <v>192</v>
@@ -4532,7 +4532,7 @@
         <v>206</v>
       </c>
       <c r="E77" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G77" t="s">
         <v>192</v>
@@ -4555,7 +4555,7 @@
         <v>115</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -4575,7 +4575,7 @@
         <v>206</v>
       </c>
       <c r="E79" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G79" t="s">
         <v>193</v>
@@ -4598,7 +4598,7 @@
         <v>206</v>
       </c>
       <c r="E80" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G80" t="s">
         <v>195</v>
@@ -4621,7 +4621,7 @@
         <v>115</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G81" t="s">
         <v>201</v>
@@ -4644,7 +4644,7 @@
         <v>115</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G82" t="s">
         <v>94</v>
@@ -4667,10 +4667,10 @@
         <v>113</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F83" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G83" t="s">
         <v>173</v>
@@ -4690,10 +4690,10 @@
         <v>113</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F84" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="G84" t="s">
         <v>172</v>
@@ -4753,10 +4753,10 @@
         <v>113</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G87" t="s">
         <v>168</v>
@@ -4776,10 +4776,10 @@
         <v>113</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4811,10 +4811,10 @@
         <v>113</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="30">
@@ -4852,7 +4852,7 @@
         <v>115</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G92" t="s">
         <v>170</v>
@@ -4872,7 +4872,7 @@
         <v>115</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G93" t="s">
         <v>171</v>
@@ -4892,7 +4892,7 @@
         <v>115</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="30">
@@ -4909,7 +4909,7 @@
         <v>115</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -4922,7 +4922,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4958,7 +4957,7 @@
         <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -4978,7 +4977,7 @@
         <v>222</v>
       </c>
       <c r="E2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4995,7 +4994,7 @@
         <v>223</v>
       </c>
       <c r="E3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5012,7 +5011,7 @@
         <v>224</v>
       </c>
       <c r="E4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5046,7 +5045,7 @@
         <v>227</v>
       </c>
       <c r="E6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5063,7 +5062,7 @@
         <v>228</v>
       </c>
       <c r="E7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5080,7 +5079,7 @@
         <v>229</v>
       </c>
       <c r="E8" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5097,7 +5096,7 @@
         <v>231</v>
       </c>
       <c r="E9" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5111,10 +5110,10 @@
         <v>213</v>
       </c>
       <c r="D10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E10" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5128,10 +5127,10 @@
         <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5145,10 +5144,10 @@
         <v>213</v>
       </c>
       <c r="D12" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E12" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -5162,10 +5161,10 @@
         <v>213</v>
       </c>
       <c r="D13" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E13" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5179,10 +5178,10 @@
         <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E14" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -5196,10 +5195,10 @@
         <v>213</v>
       </c>
       <c r="D15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E15" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -5213,7 +5212,7 @@
         <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E16" t="s">
         <v>210</v>
@@ -5230,10 +5229,10 @@
         <v>213</v>
       </c>
       <c r="D17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E17" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5247,10 +5246,10 @@
         <v>213</v>
       </c>
       <c r="D18" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E18" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5264,10 +5263,10 @@
         <v>213</v>
       </c>
       <c r="D19" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E19" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5281,10 +5280,10 @@
         <v>212</v>
       </c>
       <c r="D20" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E20" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5298,10 +5297,10 @@
         <v>212</v>
       </c>
       <c r="D21" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5315,10 +5314,10 @@
         <v>212</v>
       </c>
       <c r="D22" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
@@ -5332,10 +5331,10 @@
         <v>212</v>
       </c>
       <c r="D23" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5349,10 +5348,10 @@
         <v>213</v>
       </c>
       <c r="D24" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -5394,7 +5393,7 @@
         <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -5472,11 +5471,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:C49"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5500,7 +5499,7 @@
         <v>207</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>146</v>
@@ -5744,7 +5743,7 @@
         <v>212</v>
       </c>
       <c r="D18" t="s">
-        <v>232</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5855,7 +5854,7 @@
         <v>212</v>
       </c>
       <c r="D27" t="s">
-        <v>235</v>
+        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5924,7 +5923,7 @@
         <v>213</v>
       </c>
       <c r="D33" t="s">
-        <v>237</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -5938,7 +5937,7 @@
         <v>213</v>
       </c>
       <c r="D34" t="s">
-        <v>238</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6060,7 +6059,7 @@
         <v>212</v>
       </c>
       <c r="D44" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6123,7 +6122,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6159,7 +6157,7 @@
         <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -6432,7 +6430,7 @@
         <v>213</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -6549,7 +6547,7 @@
         <v>212</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -6788,7 +6786,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6823,7 +6820,7 @@
         <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
Corrected signature MNReplication.getReplica; Switched CNIdentity.listSubject and getSubjectInfo to return SubjectInfo structures. Closes #2273
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="24700" windowHeight="19460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="34680" windowHeight="23720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="362">
   <si>
     <t>Notes</t>
   </si>
@@ -848,15 +848,27 @@
     <t>systemMetadata/identifier/text()</t>
   </si>
   <si>
+    <t>RULE NOT PRESENT IN INDEX PROCESSING - //eml:eml/dataset/creator/individualName/surName/text()</t>
+  </si>
+  <si>
     <t>systemMetadata/replicationPolicy/@numberReplicas</t>
   </si>
   <si>
     <t>systemMetadata/formatId/text()</t>
   </si>
   <si>
+    <t>RULE NOT PRESENT IN INDEX PROCESSING - concat (//eml:eml/ dataset/ creator/ individualName/ givenName /text(),' ',//eml:eml/ dataset/ creator/ individualName/ surName /text())</t>
+  </si>
+  <si>
     <t>systemMetadata/replicationPolicy/preferredMemberNode/text()</t>
   </si>
   <si>
+    <t>RULE NOT PRESENT IN INDEX PROCESSING - //eml:eml/ dataset/ project/ title/text()</t>
+  </si>
+  <si>
+    <t>RULE NOT PRESENT IN INDEX PROCESSING - //dataset/pubDate/text()</t>
+  </si>
+  <si>
     <t>systemMetadata/replicationPolicy/@replicationAllowed</t>
   </si>
   <si>
@@ -905,9 +917,6 @@
     <t>The starting date of the temporal range of the content described by the metadata document.</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Taxonomic class name(s)</t>
   </si>
   <si>
@@ -1220,16 +1229,13 @@
     <t>Contains the :func:`CNRead.resolve` URL for the object ONLY if the object is a science metadata object.</t>
   </si>
   <si>
-    <t xml:space="preserve"> //eml:eml/dataset/creator/individualName/surName/text()</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> //eml:eml/ dataset/ project/ title/text()</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> //dataset/pubDate/text()</t>
-  </si>
-  <si>
-    <t>(//eml:eml/ dataset/ creator/ individualName/ givenName /text(),' ',//eml:eml/ dataset/ creator/ individualName/ surName /text())</t>
+    <t>Terms drawn from a controlled vocabulary of concepts that are applicable to the content described by the metadata document.</t>
+  </si>
+  <si>
+    <t>The name of the location(s) relevant to the content described by the metadata document.</t>
+  </si>
+  <si>
+    <t>Organizations that played an indirect role in the development of the data set and metadata that should be cited or mentioned as contributing to the development of the data or metadata.</t>
   </si>
 </sst>
 </file>
@@ -2800,11 +2806,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2832,7 +2838,7 @@
         <v>148</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F1" t="s">
         <v>208</v>
@@ -2858,7 +2864,7 @@
         <v>115</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -2878,7 +2884,7 @@
         <v>115</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
         <v>184</v>
@@ -2901,7 +2907,7 @@
         <v>115</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -2921,7 +2927,7 @@
         <v>115</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -2944,10 +2950,10 @@
         <v>113</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F6" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="G6" t="s">
         <v>175</v>
@@ -2970,10 +2976,10 @@
         <v>113</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F7" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
@@ -2993,10 +2999,10 @@
         <v>113</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="F8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="H8" t="s">
         <v>5</v>
@@ -3016,7 +3022,7 @@
         <v>115</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G9" t="s">
         <v>215</v>
@@ -3039,7 +3045,7 @@
         <v>115</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
@@ -3059,7 +3065,7 @@
         <v>206</v>
       </c>
       <c r="E11" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H11" t="s">
         <v>5</v>
@@ -3079,7 +3085,7 @@
         <v>113</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F12" t="s">
         <v>209</v>
@@ -3105,10 +3111,10 @@
         <v>113</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F13" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G13" t="s">
         <v>197</v>
@@ -3131,10 +3137,10 @@
         <v>113</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F14" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30">
@@ -3151,10 +3157,10 @@
         <v>113</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F15" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G15" t="s">
         <v>177</v>
@@ -3177,7 +3183,7 @@
         <v>115</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G16" t="s">
         <v>205</v>
@@ -3246,7 +3252,7 @@
         <v>115</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="G19" t="s">
         <v>23</v>
@@ -3269,7 +3275,7 @@
         <v>115</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -3289,7 +3295,7 @@
         <v>115</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="G21" t="s">
         <v>27</v>
@@ -3312,7 +3318,7 @@
         <v>115</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="G22" t="s">
         <v>215</v>
@@ -3335,7 +3341,7 @@
         <v>115</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3355,7 +3361,7 @@
         <v>115</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="H24" t="s">
         <v>5</v>
@@ -3375,7 +3381,7 @@
         <v>115</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -3395,7 +3401,7 @@
         <v>115</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="G26" t="s">
         <v>215</v>
@@ -3418,7 +3424,7 @@
         <v>115</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="G27" t="s">
         <v>122</v>
@@ -3441,10 +3447,10 @@
         <v>113</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="F28" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="G28" t="s">
         <v>196</v>
@@ -3467,7 +3473,7 @@
         <v>206</v>
       </c>
       <c r="E29" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G29" t="s">
         <v>180</v>
@@ -3490,7 +3496,7 @@
         <v>115</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="G30" t="s">
         <v>165</v>
@@ -3513,7 +3519,7 @@
         <v>206</v>
       </c>
       <c r="E31" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="H31" t="s">
         <v>5</v>
@@ -3533,7 +3539,7 @@
         <v>115</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G32" t="s">
         <v>200</v>
@@ -3556,7 +3562,7 @@
         <v>115</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G33" t="s">
         <v>114</v>
@@ -3579,7 +3585,7 @@
         <v>206</v>
       </c>
       <c r="E34" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="H34" t="s">
         <v>5</v>
@@ -3599,7 +3605,7 @@
         <v>115</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G35" t="s">
         <v>215</v>
@@ -3622,7 +3628,7 @@
         <v>115</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3642,7 +3648,7 @@
         <v>115</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="G37" t="s">
         <v>200</v>
@@ -3665,7 +3671,7 @@
         <v>115</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="G38" t="s">
         <v>126</v>
@@ -3688,10 +3694,10 @@
         <v>113</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="F39" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="G39" t="s">
         <v>181</v>
@@ -3714,10 +3720,10 @@
         <v>113</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="F40" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="H40" t="s">
         <v>5</v>
@@ -3737,10 +3743,10 @@
         <v>113</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F41" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="H41" t="s">
         <v>5</v>
@@ -3760,10 +3766,10 @@
         <v>113</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F42" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="H42" t="s">
         <v>5</v>
@@ -3783,7 +3789,7 @@
         <v>115</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3803,7 +3809,7 @@
         <v>115</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G44" t="s">
         <v>215</v>
@@ -3826,7 +3832,7 @@
         <v>115</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="G45" t="s">
         <v>166</v>
@@ -3849,7 +3855,7 @@
         <v>115</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3869,7 +3875,7 @@
         <v>206</v>
       </c>
       <c r="E47" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="G47" t="s">
         <v>183</v>
@@ -3892,7 +3898,7 @@
         <v>206</v>
       </c>
       <c r="E48" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="G48" t="s">
         <v>182</v>
@@ -3915,7 +3921,7 @@
         <v>115</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -3935,7 +3941,7 @@
         <v>206</v>
       </c>
       <c r="E50" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3955,7 +3961,7 @@
         <v>115</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="G51" t="s">
         <v>215</v>
@@ -3978,7 +3984,7 @@
         <v>115</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G52" t="s">
         <v>111</v>
@@ -4001,10 +4007,10 @@
         <v>113</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F53" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="G53" t="s">
         <v>185</v>
@@ -4027,7 +4033,7 @@
         <v>115</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -4047,7 +4053,7 @@
         <v>115</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G55" t="s">
         <v>167</v>
@@ -4070,7 +4076,7 @@
         <v>206</v>
       </c>
       <c r="E56" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G56" t="s">
         <v>186</v>
@@ -4093,7 +4099,7 @@
         <v>115</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="H57" t="s">
         <v>5</v>
@@ -4113,7 +4119,7 @@
         <v>115</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4133,10 +4139,10 @@
         <v>113</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F59" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G59" t="s">
         <v>187</v>
@@ -4159,7 +4165,7 @@
         <v>113</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="F60" t="s">
         <v>210</v>
@@ -4182,7 +4188,7 @@
         <v>115</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -4202,7 +4208,7 @@
         <v>206</v>
       </c>
       <c r="E62" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="G62" t="s">
         <v>188</v>
@@ -4225,7 +4231,7 @@
         <v>115</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -4245,7 +4251,7 @@
         <v>206</v>
       </c>
       <c r="E64" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -4265,10 +4271,10 @@
         <v>113</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="F65" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="H65" t="s">
         <v>5</v>
@@ -4288,7 +4294,7 @@
         <v>206</v>
       </c>
       <c r="E66" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G66" t="s">
         <v>176</v>
@@ -4311,7 +4317,7 @@
         <v>115</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -4331,7 +4337,7 @@
         <v>206</v>
       </c>
       <c r="E68" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="G68" t="s">
         <v>189</v>
@@ -4354,7 +4360,7 @@
         <v>115</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="G69" t="s">
         <v>79</v>
@@ -4377,7 +4383,7 @@
         <v>115</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="G70" t="s">
         <v>215</v>
@@ -4400,10 +4406,10 @@
         <v>113</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="F71" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="H71" t="s">
         <v>5</v>
@@ -4423,7 +4429,7 @@
         <v>115</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4443,7 +4449,7 @@
         <v>206</v>
       </c>
       <c r="E73" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G73" t="s">
         <v>190</v>
@@ -4489,7 +4495,7 @@
         <v>115</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="H75" t="s">
         <v>5</v>
@@ -4509,7 +4515,7 @@
         <v>206</v>
       </c>
       <c r="E76" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="G76" t="s">
         <v>192</v>
@@ -4532,7 +4538,7 @@
         <v>206</v>
       </c>
       <c r="E77" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="G77" t="s">
         <v>192</v>
@@ -4555,7 +4561,7 @@
         <v>115</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -4575,7 +4581,7 @@
         <v>206</v>
       </c>
       <c r="E79" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="G79" t="s">
         <v>193</v>
@@ -4598,7 +4604,7 @@
         <v>206</v>
       </c>
       <c r="E80" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="G80" t="s">
         <v>195</v>
@@ -4621,7 +4627,7 @@
         <v>115</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="G81" t="s">
         <v>201</v>
@@ -4644,7 +4650,7 @@
         <v>115</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G82" t="s">
         <v>94</v>
@@ -4667,10 +4673,10 @@
         <v>113</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F83" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="G83" t="s">
         <v>173</v>
@@ -4690,10 +4696,10 @@
         <v>113</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F84" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="G84" t="s">
         <v>172</v>
@@ -4753,10 +4759,10 @@
         <v>113</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="G87" t="s">
         <v>168</v>
@@ -4776,10 +4782,10 @@
         <v>113</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4811,10 +4817,10 @@
         <v>113</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="30">
@@ -4838,7 +4844,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" ht="30">
       <c r="A92" t="s">
         <v>161</v>
       </c>
@@ -4852,13 +4858,13 @@
         <v>115</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>251</v>
+        <v>359</v>
       </c>
       <c r="G92" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" ht="30">
       <c r="A93" t="s">
         <v>162</v>
       </c>
@@ -4872,13 +4878,13 @@
         <v>115</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>251</v>
+        <v>360</v>
       </c>
       <c r="G93" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" ht="45">
       <c r="A94" t="s">
         <v>164</v>
       </c>
@@ -4892,7 +4898,7 @@
         <v>115</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>251</v>
+        <v>361</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="30">
@@ -4909,7 +4915,7 @@
         <v>115</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4922,6 +4928,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4957,7 +4964,7 @@
         <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -4977,7 +4984,7 @@
         <v>222</v>
       </c>
       <c r="E2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4994,7 +5001,7 @@
         <v>223</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5011,7 +5018,7 @@
         <v>224</v>
       </c>
       <c r="E4" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5045,7 +5052,7 @@
         <v>227</v>
       </c>
       <c r="E6" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5062,7 +5069,7 @@
         <v>228</v>
       </c>
       <c r="E7" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5079,7 +5086,7 @@
         <v>229</v>
       </c>
       <c r="E8" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5096,7 +5103,7 @@
         <v>231</v>
       </c>
       <c r="E9" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5110,10 +5117,10 @@
         <v>213</v>
       </c>
       <c r="D10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E10" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5127,10 +5134,10 @@
         <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E11" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5144,10 +5151,10 @@
         <v>213</v>
       </c>
       <c r="D12" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="E12" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -5161,10 +5168,10 @@
         <v>213</v>
       </c>
       <c r="D13" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="E13" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5178,10 +5185,10 @@
         <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E14" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -5195,10 +5202,10 @@
         <v>213</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E15" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -5212,7 +5219,7 @@
         <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E16" t="s">
         <v>210</v>
@@ -5229,10 +5236,10 @@
         <v>213</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E17" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5246,10 +5253,10 @@
         <v>213</v>
       </c>
       <c r="D18" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E18" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5263,10 +5270,10 @@
         <v>213</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="E19" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5280,10 +5287,10 @@
         <v>212</v>
       </c>
       <c r="D20" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E20" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5297,10 +5304,10 @@
         <v>212</v>
       </c>
       <c r="D21" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5314,10 +5321,10 @@
         <v>212</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
@@ -5331,10 +5338,10 @@
         <v>212</v>
       </c>
       <c r="D23" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5348,10 +5355,10 @@
         <v>213</v>
       </c>
       <c r="D24" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -5393,7 +5400,7 @@
         <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -5471,11 +5478,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5499,7 +5506,7 @@
         <v>207</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>146</v>
@@ -5743,7 +5750,7 @@
         <v>212</v>
       </c>
       <c r="D18" t="s">
-        <v>356</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5854,7 +5861,7 @@
         <v>212</v>
       </c>
       <c r="D27" t="s">
-        <v>359</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5923,7 +5930,7 @@
         <v>213</v>
       </c>
       <c r="D33" t="s">
-        <v>357</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -5937,7 +5944,7 @@
         <v>213</v>
       </c>
       <c r="D34" t="s">
-        <v>358</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6059,7 +6066,7 @@
         <v>212</v>
       </c>
       <c r="D44" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6122,6 +6129,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6157,7 +6165,7 @@
         <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>
@@ -6430,7 +6438,7 @@
         <v>213</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -6547,7 +6555,7 @@
         <v>212</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -6786,6 +6794,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6820,7 +6829,7 @@
         <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E1" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
Updated search description using path element for queryType and remainder of URL being passed to the query engine.
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="34680" windowHeight="23720" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="15320" yWindow="3900" windowWidth="34680" windowHeight="23720" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -2806,11 +2806,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5478,11 +5478,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:C49"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated some more FGDC field descriptions for metadata parsing
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="372">
   <si>
     <t>Notes</t>
   </si>
@@ -410,18 +410,12 @@
     <t>//metadata/mercury/Principal_Investigator/Name/text()</t>
   </si>
   <si>
-    <t>//metadata/mercury/Project/text()</t>
-  </si>
-  <si>
     <t>//metadata/mercury/Parameter_Description/Sensor/text()</t>
   </si>
   <si>
     <t>//metadata/mercury/Parameter_Description/Source/text()</t>
   </si>
   <si>
-    <t>//metadata/mercury/Site_Information/Site/text()</t>
-  </si>
-  <si>
     <t>//metadata/mercury/Parameter_Description/Term/text()</t>
   </si>
   <si>
@@ -1248,6 +1242,34 @@
   </si>
   <si>
     <t>//taxoncl/taxonrv[../taxonrn='Order']</t>
+  </si>
+  <si>
+    <t>//metadata/citation/citeinfo/origin</t>
+  </si>
+  <si>
+    <t>8.1 Originator -- the name of an organization or individual that developed the data set.  If the name of editors or compilers are provided, the name must be followed by "(ed.)" or "(comp.)" respectively.</t>
+  </si>
+  <si>
+    <t>This could be //idinfo/citation/citeinfo/origin or perhaps //ptcontact/cntinfo/cntperp/cntper</t>
+  </si>
+  <si>
+    <t>//metadata/idinfo/spdom/descgeog</t>
+  </si>
+  <si>
+    <t>1: if //keywords/theme/themekt == "GCMD Science Keywords", then take
+the first "themekey" and split by "&gt;". The first value in the
+resulting list would be the "topic"
+2. If //keywords/theme/themekt == "none" or blank, then "topic" is the
+first "themekey" entry.</t>
+  </si>
+  <si>
+    <t>//idinfo/descript/purpose</t>
+  </si>
+  <si>
+    <t>//digform/digtinfo/formname</t>
+  </si>
+  <si>
+    <t>May also be //idinfo/citation/citeinfo/geoform</t>
   </si>
 </sst>
 </file>
@@ -2922,28 +2944,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30">
@@ -2954,13 +2976,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -2974,16 +2996,16 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2997,13 +3019,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -3017,13 +3039,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -3034,25 +3056,25 @@
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3066,16 +3088,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
@@ -3089,16 +3111,16 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
@@ -3112,16 +3134,16 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -3135,13 +3157,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>
@@ -3155,13 +3177,13 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
@@ -3175,19 +3197,19 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -3201,19 +3223,19 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
@@ -3221,45 +3243,45 @@
     </row>
     <row r="14" spans="1:8" ht="30">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H15" t="s">
         <v>4</v>
@@ -3273,16 +3295,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
@@ -3290,22 +3312,22 @@
     </row>
     <row r="17" spans="1:8" ht="30">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -3313,22 +3335,22 @@
     </row>
     <row r="18" spans="1:8" ht="45">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H18" t="s">
         <v>4</v>
@@ -3342,13 +3364,13 @@
         <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G19" t="s">
         <v>20</v>
@@ -3365,13 +3387,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -3385,13 +3407,13 @@
         <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G21" t="s">
         <v>23</v>
@@ -3408,16 +3430,16 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -3431,13 +3453,13 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3451,13 +3473,13 @@
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
@@ -3471,13 +3493,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -3491,16 +3513,16 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -3514,16 +3536,16 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -3537,19 +3559,19 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F28" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H28" t="s">
         <v>4</v>
@@ -3563,16 +3585,16 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
@@ -3586,16 +3608,16 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
@@ -3609,13 +3631,13 @@
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E31" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
@@ -3629,16 +3651,16 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G32" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H32" t="s">
         <v>4</v>
@@ -3652,16 +3674,16 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H33" t="s">
         <v>4</v>
@@ -3675,13 +3697,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E34" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
@@ -3695,16 +3717,16 @@
         <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -3718,13 +3740,13 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3738,16 +3760,16 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G37" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H37" t="s">
         <v>4</v>
@@ -3761,16 +3783,16 @@
         <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H38" t="s">
         <v>4</v>
@@ -3778,25 +3800,25 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F39" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -3810,16 +3832,16 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F40" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H40" t="s">
         <v>4</v>
@@ -3827,22 +3849,22 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F41" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H41" t="s">
         <v>4</v>
@@ -3856,16 +3878,16 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F42" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H42" t="s">
         <v>4</v>
@@ -3879,13 +3901,13 @@
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3899,16 +3921,16 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G44" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3922,16 +3944,16 @@
         <v>3</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G45" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H45" t="s">
         <v>4</v>
@@ -3945,13 +3967,13 @@
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3965,16 +3987,16 @@
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D47" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E47" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G47" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3988,16 +4010,16 @@
         <v>2</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D48" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E48" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G48" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H48" t="s">
         <v>4</v>
@@ -4011,13 +4033,13 @@
         <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -4031,13 +4053,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D50" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E50" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -4051,16 +4073,16 @@
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D51" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -4074,16 +4096,16 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H52" t="s">
         <v>4</v>
@@ -4091,25 +4113,25 @@
     </row>
     <row r="53" spans="1:8" ht="30">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F53" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G53" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -4123,13 +4145,13 @@
         <v>3</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D54" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -4143,16 +4165,16 @@
         <v>3</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D55" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G55" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H55" t="s">
         <v>4</v>
@@ -4166,16 +4188,16 @@
         <v>2</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E56" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G56" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H56" t="s">
         <v>4</v>
@@ -4189,13 +4211,13 @@
         <v>8</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D57" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H57" t="s">
         <v>4</v>
@@ -4209,13 +4231,13 @@
         <v>2</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D58" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4223,25 +4245,25 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D59" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F59" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G59" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -4255,16 +4277,16 @@
         <v>3</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F60" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -4278,13 +4300,13 @@
         <v>3</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D61" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -4298,16 +4320,16 @@
         <v>2</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D62" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E62" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G62" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -4321,13 +4343,13 @@
         <v>3</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D63" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -4341,13 +4363,13 @@
         <v>2</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D64" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E64" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -4361,16 +4383,16 @@
         <v>65</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D65" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F65" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H65" t="s">
         <v>4</v>
@@ -4384,16 +4406,16 @@
         <v>67</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D66" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E66" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G66" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H66" t="s">
         <v>4</v>
@@ -4407,13 +4429,13 @@
         <v>3</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D67" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -4427,16 +4449,16 @@
         <v>2</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D68" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E68" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G68" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -4450,13 +4472,13 @@
         <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G69" t="s">
         <v>71</v>
@@ -4473,16 +4495,16 @@
         <v>3</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D70" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G70" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -4496,16 +4518,16 @@
         <v>3</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D71" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F71" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H71" t="s">
         <v>4</v>
@@ -4519,13 +4541,13 @@
         <v>3</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4539,16 +4561,16 @@
         <v>2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D73" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E73" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G73" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -4562,16 +4584,16 @@
         <v>2</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D74" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E74" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G74" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H74" t="s">
         <v>4</v>
@@ -4585,13 +4607,13 @@
         <v>3</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D75" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H75" t="s">
         <v>4</v>
@@ -4605,16 +4627,16 @@
         <v>3</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D76" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E76" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G76" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H76" t="s">
         <v>4</v>
@@ -4628,16 +4650,16 @@
         <v>3</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D77" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E77" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G77" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H77" t="s">
         <v>4</v>
@@ -4651,13 +4673,13 @@
         <v>3</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D78" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -4671,16 +4693,16 @@
         <v>2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D79" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E79" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G79" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -4694,16 +4716,16 @@
         <v>8</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D80" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E80" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G80" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H80" t="s">
         <v>4</v>
@@ -4717,16 +4739,16 @@
         <v>3</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D81" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G81" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H81" t="s">
         <v>4</v>
@@ -4740,13 +4762,13 @@
         <v>19</v>
       </c>
       <c r="C82" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G82" t="s">
         <v>84</v>
@@ -4757,261 +4779,261 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B83" t="s">
         <v>3</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D83" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F83" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G83" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D84" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F84" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G84" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B85" t="s">
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D85" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G85" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="30">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B86" t="s">
         <v>3</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D86" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G86" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="30">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B87" t="s">
         <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D87" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G87" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="30">
       <c r="A88" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B88" t="s">
         <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D88" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B89" t="s">
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D89" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F89" s="3"/>
     </row>
     <row r="90" spans="1:8" ht="30">
       <c r="A90" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B90" t="s">
         <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D90" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="30">
       <c r="A91" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B91" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C91" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D91" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="30">
       <c r="A92" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B92" t="s">
         <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D92" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G92" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="30">
       <c r="A93" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B93" t="s">
         <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D93" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G93" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="45">
       <c r="A94" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B94" t="s">
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D94" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="30">
       <c r="A95" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B95" t="s">
         <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D95" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -5051,36 +5073,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5091,13 +5113,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5108,13 +5130,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5125,13 +5147,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5142,47 +5164,47 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5193,30 +5215,30 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5227,30 +5249,30 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -5261,47 +5283,47 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E15" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -5312,13 +5334,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5329,13 +5351,13 @@
         <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E17" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5346,115 +5368,115 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -5487,67 +5509,67 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5593,22 +5615,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5619,13 +5641,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5636,16 +5658,16 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5656,13 +5678,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
         <v>120</v>
-      </c>
-      <c r="E4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5673,13 +5695,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5690,7 +5712,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5701,13 +5723,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5718,10 +5740,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5732,13 +5754,13 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5749,7 +5771,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5760,13 +5782,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5777,7 +5799,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5788,7 +5810,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5799,7 +5821,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5810,7 +5832,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -5821,7 +5843,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5832,7 +5854,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5843,10 +5865,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5857,7 +5879,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5868,10 +5890,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5882,7 +5904,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5893,7 +5915,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5904,7 +5926,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5915,13 +5937,13 @@
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -5932,7 +5954,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5943,7 +5965,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -5954,10 +5976,10 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5968,7 +5990,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -5979,7 +6001,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5990,7 +6012,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6001,7 +6023,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6012,7 +6034,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -6023,10 +6045,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D33" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -6037,10 +6059,10 @@
         <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D34" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6051,7 +6073,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -6062,7 +6084,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -6073,7 +6095,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -6084,7 +6106,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -6095,10 +6117,10 @@
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -6109,7 +6131,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -6120,7 +6142,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -6131,13 +6153,13 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -6148,7 +6170,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -6159,10 +6181,10 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D44" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6173,54 +6195,54 @@
         <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -6238,8 +6260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6254,22 +6276,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6280,10 +6302,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6294,7 +6316,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E3" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6305,7 +6333,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6316,10 +6344,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6330,10 +6358,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6344,10 +6372,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6358,7 +6386,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6369,10 +6397,10 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6383,10 +6411,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6397,10 +6425,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6411,10 +6439,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -6425,7 +6453,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -6436,7 +6464,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -6447,10 +6475,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -6461,13 +6489,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -6475,13 +6503,13 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D17" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -6489,13 +6517,16 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -6503,10 +6534,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -6514,13 +6545,13 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -6528,13 +6559,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -6542,13 +6573,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -6556,10 +6587,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -6567,13 +6598,13 @@
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -6581,10 +6612,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -6592,13 +6623,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -6606,13 +6637,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D27" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -6620,13 +6651,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D28" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -6634,10 +6665,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -6645,13 +6676,13 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -6659,13 +6690,13 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -6673,10 +6704,16 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>191</v>
+      </c>
+      <c r="D32" t="s">
+        <v>370</v>
+      </c>
+      <c r="E32" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -6684,13 +6721,13 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -6698,13 +6735,13 @@
         <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D34" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -6712,13 +6749,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D35" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -6726,13 +6763,13 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -6740,13 +6777,13 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -6754,13 +6791,13 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -6768,13 +6805,13 @@
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D39" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -6782,13 +6819,13 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -6796,13 +6833,13 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -6810,13 +6847,13 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D42" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="90">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -6824,13 +6861,16 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>89</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -6838,13 +6878,13 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D44" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -6852,54 +6892,54 @@
         <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D45" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -6930,22 +6970,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6956,7 +6996,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6967,7 +7007,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6978,7 +7018,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6989,7 +7029,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -7000,7 +7040,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7011,7 +7051,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -7022,7 +7062,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -7033,7 +7073,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -7044,7 +7084,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -7055,7 +7095,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7066,7 +7106,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -7077,7 +7117,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -7088,7 +7128,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -7099,7 +7139,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -7110,7 +7150,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -7121,7 +7161,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -7132,10 +7172,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -7146,7 +7186,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -7157,10 +7197,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -7171,7 +7211,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -7182,7 +7222,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -7193,7 +7233,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -7204,7 +7244,7 @@
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -7215,7 +7255,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -7226,7 +7266,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -7237,10 +7277,10 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -7251,7 +7291,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -7262,7 +7302,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -7273,7 +7313,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -7284,7 +7324,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -7295,7 +7335,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -7306,7 +7346,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -7317,7 +7357,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -7328,7 +7368,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -7339,7 +7379,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -7350,7 +7390,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -7361,7 +7401,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -7372,7 +7412,7 @@
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -7383,7 +7423,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -7394,7 +7434,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -7405,10 +7445,10 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D42" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -7419,7 +7459,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -7430,10 +7470,10 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -7444,51 +7484,51 @@
         <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated search fields derived from system metadata wrt camel case names for objectformat and rightsholder
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="25600" windowHeight="14840" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="10280" yWindow="540" windowWidth="25600" windowHeight="14840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="374">
   <si>
     <t>Notes</t>
   </si>
@@ -1270,6 +1270,12 @@
   </si>
   <si>
     <t>May also be //idinfo/citation/citeinfo/geoform</t>
+  </si>
+  <si>
+    <t>objectformat</t>
+  </si>
+  <si>
+    <t>rightsholder</t>
   </si>
 </sst>
 </file>
@@ -5046,7 +5052,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5060,8 +5065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5243,7 +5248,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>372</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -5328,7 +5333,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>373</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -6247,7 +6252,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6260,7 +6264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -6944,7 +6948,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated field documentation for search data derived from science metadata.  field updated 'fullText' to 'text'
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10280" yWindow="540" windowWidth="25600" windowHeight="14840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="13560" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -779,9 +779,6 @@
     <t>systemMetadata/identifier/text()</t>
   </si>
   <si>
-    <t>RULE NOT PRESENT IN INDEX PROCESSING - //eml:eml/dataset/creator/individualName/surName/text()</t>
-  </si>
-  <si>
     <t>systemMetadata/replicationPolicy/@numberReplicas</t>
   </si>
   <si>
@@ -792,12 +789,6 @@
   </si>
   <si>
     <t>systemMetadata/replicationPolicy/preferredMemberNode/text()</t>
-  </si>
-  <si>
-    <t>RULE NOT PRESENT IN INDEX PROCESSING - //eml:eml/ dataset/ project/ title/text()</t>
-  </si>
-  <si>
-    <t>RULE NOT PRESENT IN INDEX PROCESSING - //dataset/pubDate/text()</t>
   </si>
   <si>
     <t>systemMetadata/replicationPolicy/@replicationAllowed</t>
@@ -1276,6 +1267,15 @@
   </si>
   <si>
     <t>rightsholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //eml:eml/ dataset/ project/ title/text()</t>
+  </si>
+  <si>
+    <t>//dataset/pubDate/text()</t>
+  </si>
+  <si>
+    <t>//eml:eml/dataset/creator/individualName/surName/text()</t>
   </si>
 </sst>
 </file>
@@ -2962,7 +2962,7 @@
         <v>126</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F1" t="s">
         <v>186</v>
@@ -2988,7 +2988,7 @@
         <v>93</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -3008,7 +3008,7 @@
         <v>93</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G3" t="s">
         <v>162</v>
@@ -3031,7 +3031,7 @@
         <v>93</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -3051,7 +3051,7 @@
         <v>93</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -3074,10 +3074,10 @@
         <v>91</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F6" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G6" t="s">
         <v>153</v>
@@ -3100,10 +3100,10 @@
         <v>91</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F7" t="s">
         <v>257</v>
-      </c>
-      <c r="F7" t="s">
-        <v>260</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
@@ -3123,10 +3123,10 @@
         <v>91</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
@@ -3146,7 +3146,7 @@
         <v>93</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G9" t="s">
         <v>193</v>
@@ -3169,7 +3169,7 @@
         <v>93</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>
@@ -3189,7 +3189,7 @@
         <v>184</v>
       </c>
       <c r="E11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
@@ -3209,7 +3209,7 @@
         <v>91</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F12" t="s">
         <v>187</v>
@@ -3235,10 +3235,10 @@
         <v>91</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G13" t="s">
         <v>175</v>
@@ -3261,10 +3261,10 @@
         <v>91</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F14" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30">
@@ -3281,10 +3281,10 @@
         <v>91</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G15" t="s">
         <v>155</v>
@@ -3307,7 +3307,7 @@
         <v>93</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G16" t="s">
         <v>183</v>
@@ -3376,7 +3376,7 @@
         <v>93</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G19" t="s">
         <v>20</v>
@@ -3399,7 +3399,7 @@
         <v>93</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -3419,7 +3419,7 @@
         <v>93</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G21" t="s">
         <v>23</v>
@@ -3442,7 +3442,7 @@
         <v>93</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G22" t="s">
         <v>193</v>
@@ -3465,7 +3465,7 @@
         <v>93</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3485,7 +3485,7 @@
         <v>93</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
@@ -3505,7 +3505,7 @@
         <v>93</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -3525,7 +3525,7 @@
         <v>93</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G26" t="s">
         <v>193</v>
@@ -3548,7 +3548,7 @@
         <v>93</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G27" t="s">
         <v>100</v>
@@ -3571,10 +3571,10 @@
         <v>91</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F28" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G28" t="s">
         <v>174</v>
@@ -3597,7 +3597,7 @@
         <v>184</v>
       </c>
       <c r="E29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G29" t="s">
         <v>158</v>
@@ -3620,7 +3620,7 @@
         <v>93</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G30" t="s">
         <v>143</v>
@@ -3643,7 +3643,7 @@
         <v>184</v>
       </c>
       <c r="E31" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
@@ -3663,7 +3663,7 @@
         <v>93</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G32" t="s">
         <v>178</v>
@@ -3686,7 +3686,7 @@
         <v>93</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G33" t="s">
         <v>92</v>
@@ -3709,7 +3709,7 @@
         <v>184</v>
       </c>
       <c r="E34" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
@@ -3729,7 +3729,7 @@
         <v>93</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G35" t="s">
         <v>193</v>
@@ -3752,7 +3752,7 @@
         <v>93</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3772,7 +3772,7 @@
         <v>93</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G37" t="s">
         <v>178</v>
@@ -3795,7 +3795,7 @@
         <v>93</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G38" t="s">
         <v>104</v>
@@ -3818,10 +3818,10 @@
         <v>91</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F39" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G39" t="s">
         <v>159</v>
@@ -3844,10 +3844,10 @@
         <v>91</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F40" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H40" t="s">
         <v>4</v>
@@ -3867,10 +3867,10 @@
         <v>91</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F41" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H41" t="s">
         <v>4</v>
@@ -3890,10 +3890,10 @@
         <v>91</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F42" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H42" t="s">
         <v>4</v>
@@ -3913,7 +3913,7 @@
         <v>93</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3933,7 +3933,7 @@
         <v>93</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G44" t="s">
         <v>193</v>
@@ -3956,7 +3956,7 @@
         <v>93</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G45" t="s">
         <v>144</v>
@@ -3979,7 +3979,7 @@
         <v>93</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3999,7 +3999,7 @@
         <v>184</v>
       </c>
       <c r="E47" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G47" t="s">
         <v>161</v>
@@ -4022,7 +4022,7 @@
         <v>184</v>
       </c>
       <c r="E48" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G48" t="s">
         <v>160</v>
@@ -4045,7 +4045,7 @@
         <v>93</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -4065,7 +4065,7 @@
         <v>184</v>
       </c>
       <c r="E50" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G51" t="s">
         <v>193</v>
@@ -4108,7 +4108,7 @@
         <v>93</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G52" t="s">
         <v>90</v>
@@ -4131,10 +4131,10 @@
         <v>91</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F53" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G53" t="s">
         <v>163</v>
@@ -4157,7 +4157,7 @@
         <v>93</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -4177,7 +4177,7 @@
         <v>93</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G55" t="s">
         <v>145</v>
@@ -4200,7 +4200,7 @@
         <v>184</v>
       </c>
       <c r="E56" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G56" t="s">
         <v>164</v>
@@ -4223,7 +4223,7 @@
         <v>93</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H57" t="s">
         <v>4</v>
@@ -4243,7 +4243,7 @@
         <v>93</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4263,10 +4263,10 @@
         <v>91</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F59" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G59" t="s">
         <v>165</v>
@@ -4289,7 +4289,7 @@
         <v>91</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F60" t="s">
         <v>188</v>
@@ -4312,7 +4312,7 @@
         <v>93</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -4332,7 +4332,7 @@
         <v>184</v>
       </c>
       <c r="E62" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G62" t="s">
         <v>166</v>
@@ -4355,7 +4355,7 @@
         <v>93</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -4375,7 +4375,7 @@
         <v>184</v>
       </c>
       <c r="E64" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -4395,10 +4395,10 @@
         <v>91</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F65" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H65" t="s">
         <v>4</v>
@@ -4418,7 +4418,7 @@
         <v>184</v>
       </c>
       <c r="E66" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G66" t="s">
         <v>154</v>
@@ -4441,7 +4441,7 @@
         <v>93</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -4461,7 +4461,7 @@
         <v>184</v>
       </c>
       <c r="E68" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G68" t="s">
         <v>167</v>
@@ -4484,7 +4484,7 @@
         <v>93</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G69" t="s">
         <v>71</v>
@@ -4507,7 +4507,7 @@
         <v>93</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G70" t="s">
         <v>193</v>
@@ -4530,10 +4530,10 @@
         <v>91</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F71" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H71" t="s">
         <v>4</v>
@@ -4553,7 +4553,7 @@
         <v>93</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4573,7 +4573,7 @@
         <v>184</v>
       </c>
       <c r="E73" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G73" t="s">
         <v>168</v>
@@ -4619,7 +4619,7 @@
         <v>93</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H75" t="s">
         <v>4</v>
@@ -4639,7 +4639,7 @@
         <v>184</v>
       </c>
       <c r="E76" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G76" t="s">
         <v>170</v>
@@ -4662,7 +4662,7 @@
         <v>184</v>
       </c>
       <c r="E77" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G77" t="s">
         <v>170</v>
@@ -4685,7 +4685,7 @@
         <v>93</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -4705,7 +4705,7 @@
         <v>184</v>
       </c>
       <c r="E79" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G79" t="s">
         <v>171</v>
@@ -4728,7 +4728,7 @@
         <v>184</v>
       </c>
       <c r="E80" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G80" t="s">
         <v>173</v>
@@ -4751,7 +4751,7 @@
         <v>93</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G81" t="s">
         <v>179</v>
@@ -4774,7 +4774,7 @@
         <v>93</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G82" t="s">
         <v>84</v>
@@ -4797,10 +4797,10 @@
         <v>91</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F83" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G83" t="s">
         <v>151</v>
@@ -4820,10 +4820,10 @@
         <v>91</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F84" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G84" t="s">
         <v>150</v>
@@ -4883,10 +4883,10 @@
         <v>91</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G87" t="s">
         <v>146</v>
@@ -4906,10 +4906,10 @@
         <v>91</v>
       </c>
       <c r="E88" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="F88" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4941,10 +4941,10 @@
         <v>91</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="30">
@@ -4982,7 +4982,7 @@
         <v>93</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G92" t="s">
         <v>148</v>
@@ -5002,7 +5002,7 @@
         <v>93</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G93" t="s">
         <v>149</v>
@@ -5022,7 +5022,7 @@
         <v>93</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="30">
@@ -5039,7 +5039,7 @@
         <v>93</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -5065,7 +5065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -5087,7 +5087,7 @@
         <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E1" t="s">
         <v>124</v>
@@ -5107,7 +5107,7 @@
         <v>199</v>
       </c>
       <c r="E2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5124,7 +5124,7 @@
         <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5141,7 +5141,7 @@
         <v>201</v>
       </c>
       <c r="E4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5175,7 +5175,7 @@
         <v>204</v>
       </c>
       <c r="E6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5192,7 +5192,7 @@
         <v>205</v>
       </c>
       <c r="E7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5209,7 +5209,7 @@
         <v>206</v>
       </c>
       <c r="E8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5226,7 +5226,7 @@
         <v>208</v>
       </c>
       <c r="E9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5240,15 +5240,15 @@
         <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -5257,10 +5257,10 @@
         <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E11" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5274,10 +5274,10 @@
         <v>191</v>
       </c>
       <c r="D12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -5291,10 +5291,10 @@
         <v>191</v>
       </c>
       <c r="D13" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E13" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5308,10 +5308,10 @@
         <v>190</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E14" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -5325,15 +5325,15 @@
         <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E15" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -5342,7 +5342,7 @@
         <v>191</v>
       </c>
       <c r="D16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E16" t="s">
         <v>188</v>
@@ -5359,10 +5359,10 @@
         <v>191</v>
       </c>
       <c r="D17" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E17" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5376,10 +5376,10 @@
         <v>191</v>
       </c>
       <c r="D18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E18" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5393,10 +5393,10 @@
         <v>191</v>
       </c>
       <c r="D19" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5410,10 +5410,10 @@
         <v>190</v>
       </c>
       <c r="D20" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5427,10 +5427,10 @@
         <v>190</v>
       </c>
       <c r="D21" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5444,10 +5444,10 @@
         <v>190</v>
       </c>
       <c r="D22" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
@@ -5461,10 +5461,10 @@
         <v>190</v>
       </c>
       <c r="D23" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5478,10 +5478,10 @@
         <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -5523,7 +5523,7 @@
         <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E1" t="s">
         <v>124</v>
@@ -5601,11 +5601,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5629,7 +5629,7 @@
         <v>185</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>124</v>
@@ -5649,7 +5649,7 @@
         <v>191</v>
       </c>
       <c r="D2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E2" t="s">
         <v>115</v>
@@ -5820,7 +5820,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -5873,7 +5873,7 @@
         <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5984,7 +5984,7 @@
         <v>190</v>
       </c>
       <c r="D27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -6053,7 +6053,7 @@
         <v>191</v>
       </c>
       <c r="D33" t="s">
-        <v>214</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -6067,7 +6067,7 @@
         <v>191</v>
       </c>
       <c r="D34" t="s">
-        <v>215</v>
+        <v>372</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6189,7 +6189,7 @@
         <v>190</v>
       </c>
       <c r="D44" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6265,7 +6265,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6289,7 +6289,7 @@
         <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E1" t="s">
         <v>124</v>
@@ -6309,7 +6309,7 @@
         <v>191</v>
       </c>
       <c r="D2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6323,10 +6323,10 @@
         <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E3" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6351,7 +6351,7 @@
         <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6365,7 +6365,7 @@
         <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6379,7 +6379,7 @@
         <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6404,7 +6404,7 @@
         <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6418,7 +6418,7 @@
         <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6432,7 +6432,7 @@
         <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6446,7 +6446,7 @@
         <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -6462,7 +6462,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -6482,7 +6482,7 @@
         <v>190</v>
       </c>
       <c r="D15" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -6496,7 +6496,7 @@
         <v>190</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6510,7 +6510,7 @@
         <v>191</v>
       </c>
       <c r="D17" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6527,7 +6527,7 @@
         <v>85</v>
       </c>
       <c r="E18" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6566,7 +6566,7 @@
         <v>190</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -6580,7 +6580,7 @@
         <v>191</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -6605,7 +6605,7 @@
         <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -6630,7 +6630,7 @@
         <v>190</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -6644,7 +6644,7 @@
         <v>190</v>
       </c>
       <c r="D27" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -6658,7 +6658,7 @@
         <v>190</v>
       </c>
       <c r="D28" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6683,7 +6683,7 @@
         <v>190</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6697,7 +6697,7 @@
         <v>190</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6711,10 +6711,10 @@
         <v>191</v>
       </c>
       <c r="D32" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E32" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -6728,7 +6728,7 @@
         <v>191</v>
       </c>
       <c r="D33" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -6742,7 +6742,7 @@
         <v>191</v>
       </c>
       <c r="D34" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6756,7 +6756,7 @@
         <v>191</v>
       </c>
       <c r="D35" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -6784,7 +6784,7 @@
         <v>190</v>
       </c>
       <c r="D37" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -6812,7 +6812,7 @@
         <v>191</v>
       </c>
       <c r="D39" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -6826,7 +6826,7 @@
         <v>190</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -6854,7 +6854,7 @@
         <v>191</v>
       </c>
       <c r="D42" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="90">
@@ -6871,7 +6871,7 @@
         <v>89</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -6885,7 +6885,7 @@
         <v>190</v>
       </c>
       <c r="D44" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6899,7 +6899,7 @@
         <v>191</v>
       </c>
       <c r="D45" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -6982,7 +6982,7 @@
         <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E1" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
missed a reference to old field name:'objectformat'.  replaced with 'formatId'
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="367">
   <si>
     <t>Notes</t>
   </si>
@@ -1201,9 +1201,6 @@
   </si>
   <si>
     <t>May also be //idinfo/citation/citeinfo/geoform</t>
-  </si>
-  <si>
-    <t>objectformat</t>
   </si>
   <si>
     <t xml:space="preserve"> //eml:eml/ dataset/ project/ title/text()</t>
@@ -3001,7 +2998,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -3044,7 +3041,7 @@
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="A6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -3179,7 +3176,7 @@
     </row>
     <row r="12" spans="1:8" ht="30">
       <c r="A12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -3231,7 +3228,7 @@
     </row>
     <row r="14" spans="1:8" ht="30">
       <c r="A14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -3251,7 +3248,7 @@
     </row>
     <row r="15" spans="1:8" ht="30">
       <c r="A15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -3788,7 +3785,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
@@ -3814,7 +3811,7 @@
     </row>
     <row r="40" spans="1:8" ht="30">
       <c r="A40" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
@@ -3860,7 +3857,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B42" t="s">
         <v>2</v>
@@ -4078,7 +4075,7 @@
     </row>
     <row r="52" spans="1:8" ht="30">
       <c r="A52" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -4210,7 +4207,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B58" t="s">
         <v>176</v>
@@ -4675,7 +4672,7 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -4698,7 +4695,7 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B80" t="s">
         <v>3</v>
@@ -4744,7 +4741,7 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B82" t="s">
         <v>3</v>
@@ -4767,7 +4764,7 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B83" t="s">
         <v>3</v>
@@ -4790,7 +4787,7 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
@@ -4989,8 +4986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5019,7 +5016,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -5070,7 +5067,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -5104,7 +5101,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -5121,7 +5118,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -5155,7 +5152,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -5172,7 +5169,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -5206,7 +5203,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -5223,7 +5220,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B14" t="s">
         <v>176</v>
@@ -5291,7 +5288,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -5308,7 +5305,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -5464,7 +5461,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -5571,7 +5568,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -5767,7 +5764,7 @@
         <v>174</v>
       </c>
       <c r="D18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5847,7 +5844,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -5947,7 +5944,7 @@
         <v>175</v>
       </c>
       <c r="D33" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -5961,7 +5958,7 @@
         <v>175</v>
       </c>
       <c r="D34" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6074,7 +6071,7 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -6158,7 +6155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -6225,7 +6222,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -6504,7 +6501,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -6770,7 +6767,7 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added initial revision of Dryad metadata terms
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="16780" yWindow="7820" windowWidth="32940" windowHeight="19800" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="372">
   <si>
     <t>Notes</t>
   </si>
@@ -434,12 +434,6 @@
     <t>PropertLookup_props_writer.java</t>
   </si>
   <si>
-    <t>//mets:METS/ mets:dmdSec/ mets:mdWrap/ mets:xmlData/ dim:dim/ dim:field[@qualifier='author']/text()</t>
-  </si>
-  <si>
-    <t>//mets:METS/ mets:dmdSec/ mets:mdWrap/ mets:xmlData/ dim:dim/ dim:field[@element='subject']/text()</t>
-  </si>
-  <si>
     <t>//dataset/keywordSet/keyword/text()</t>
   </si>
   <si>
@@ -459,12 +453,6 @@
   </si>
   <si>
     <t>//dataset/title/text()</t>
-  </si>
-  <si>
-    <t>//mets:METS/ mets:dmdSec/ mets:mdWrap/ mets:xmlData/ dim:dim/ dim:field[@element='title']/text()</t>
-  </si>
-  <si>
-    <t>//mets:METS/ mets:dmdSec/ mets:mdWrap/ mets:xmlData/ dim:dim/ dim:field[@qualifier='uri']/text()</t>
   </si>
   <si>
     <t>SOLR</t>
@@ -1256,12 +1244,39 @@
   <si>
     <t>resourceMap</t>
   </si>
+  <si>
+    <t>Multiple entries in Dryad - will need to concatenate</t>
+  </si>
+  <si>
+    <t>dcterms:dateSubmitted</t>
+  </si>
+  <si>
+    <t>dwc:scientificName</t>
+  </si>
+  <si>
+    <t>dcterms:subject</t>
+  </si>
+  <si>
+    <t>dcterms:creator</t>
+  </si>
+  <si>
+    <t>dcterms:spatial</t>
+  </si>
+  <si>
+    <t>dcterms:description</t>
+  </si>
+  <si>
+    <t>dcterms:title</t>
+  </si>
+  <si>
+    <t>http://dryad.googlecode.com/svn/trunk/dryad/dspace/modules/xmlui/src/main/webapp/themes/Dryad/meta/schema/v3/dryad.xsd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1319,6 +1334,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1931,7 +1951,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1944,6 +1964,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="592">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2929,28 +2950,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30">
@@ -2961,13 +2982,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
         <v>90</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -2981,16 +3002,16 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
         <v>90</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2998,19 +3019,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D4" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -3024,13 +3045,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
         <v>90</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -3041,25 +3062,25 @@
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="A6" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
         <v>88</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F6" t="s">
         <v>235</v>
       </c>
-      <c r="F6" t="s">
-        <v>239</v>
-      </c>
       <c r="G6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3073,16 +3094,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
         <v>88</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
@@ -3096,16 +3117,16 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
         <v>88</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
@@ -3119,16 +3140,16 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
         <v>90</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -3142,13 +3163,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
         <v>90</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>
@@ -3162,13 +3183,13 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
@@ -3176,22 +3197,22 @@
     </row>
     <row r="12" spans="1:8" ht="30">
       <c r="A12" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D12" t="s">
         <v>88</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F12" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G12" t="s">
         <v>91</v>
@@ -3208,19 +3229,19 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
@@ -3228,45 +3249,45 @@
     </row>
     <row r="14" spans="1:8" ht="30">
       <c r="A14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
         <v>88</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F14" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30">
       <c r="A15" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
         <v>88</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H15" t="s">
         <v>4</v>
@@ -3280,16 +3301,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
         <v>90</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G16" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
@@ -3297,22 +3318,22 @@
     </row>
     <row r="17" spans="1:8" ht="30">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -3326,16 +3347,16 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H18" t="s">
         <v>4</v>
@@ -3349,13 +3370,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D19" t="s">
         <v>90</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
@@ -3372,13 +3393,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
         <v>90</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -3392,13 +3413,13 @@
         <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
         <v>90</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
@@ -3415,16 +3436,16 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D22" t="s">
         <v>90</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G22" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -3438,13 +3459,13 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D23" t="s">
         <v>90</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3458,13 +3479,13 @@
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D24" t="s">
         <v>90</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
@@ -3478,13 +3499,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D25" t="s">
         <v>90</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -3498,16 +3519,16 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D26" t="s">
         <v>90</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G26" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -3521,13 +3542,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D27" t="s">
         <v>90</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G27" t="s">
         <v>93</v>
@@ -3544,19 +3565,19 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D28" t="s">
         <v>88</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F28" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G28" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H28" t="s">
         <v>4</v>
@@ -3570,16 +3591,16 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D29" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G29" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
@@ -3593,16 +3614,16 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D30" t="s">
         <v>90</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G30" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
@@ -3616,13 +3637,13 @@
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D31" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E31" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
@@ -3636,16 +3657,16 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D32" t="s">
         <v>90</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G32" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H32" t="s">
         <v>4</v>
@@ -3659,13 +3680,13 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D33" t="s">
         <v>90</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G33" t="s">
         <v>89</v>
@@ -3682,13 +3703,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D34" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E34" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
@@ -3702,16 +3723,16 @@
         <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D35" t="s">
         <v>90</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G35" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -3725,13 +3746,13 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D36" t="s">
         <v>90</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3745,16 +3766,16 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D37" t="s">
         <v>90</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G37" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H37" t="s">
         <v>4</v>
@@ -3768,16 +3789,16 @@
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D38" t="s">
         <v>90</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H38" t="s">
         <v>4</v>
@@ -3785,25 +3806,25 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D39" t="s">
         <v>88</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F39" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G39" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -3811,22 +3832,22 @@
     </row>
     <row r="40" spans="1:8" ht="30">
       <c r="A40" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D40" t="s">
         <v>88</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F40" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H40" t="s">
         <v>4</v>
@@ -3840,16 +3861,16 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D41" t="s">
         <v>88</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F41" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H41" t="s">
         <v>4</v>
@@ -3857,19 +3878,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B42" t="s">
         <v>2</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D42" t="s">
         <v>90</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -3883,16 +3904,16 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D43" t="s">
         <v>90</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G43" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3906,16 +3927,16 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D44" t="s">
         <v>90</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G44" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H44" t="s">
         <v>4</v>
@@ -3929,13 +3950,13 @@
         <v>3</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D45" t="s">
         <v>90</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3949,16 +3970,16 @@
         <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E46" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G46" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3972,16 +3993,16 @@
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D47" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E47" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G47" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H47" t="s">
         <v>4</v>
@@ -3995,13 +4016,13 @@
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D48" t="s">
         <v>90</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -4015,13 +4036,13 @@
         <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D49" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E49" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -4035,16 +4056,16 @@
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D50" t="s">
         <v>90</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G50" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -4058,13 +4079,13 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D51" t="s">
         <v>90</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G51" t="s">
         <v>87</v>
@@ -4075,25 +4096,25 @@
     </row>
     <row r="52" spans="1:8" ht="30">
       <c r="A52" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D52" t="s">
         <v>88</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F52" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -4107,13 +4128,13 @@
         <v>3</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
         <v>90</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -4127,16 +4148,16 @@
         <v>3</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D54" t="s">
         <v>90</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="G54" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H54" t="s">
         <v>4</v>
@@ -4150,16 +4171,16 @@
         <v>2</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E55" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G55" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H55" t="s">
         <v>4</v>
@@ -4173,13 +4194,13 @@
         <v>8</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D56" t="s">
         <v>90</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="H56" t="s">
         <v>4</v>
@@ -4193,13 +4214,13 @@
         <v>2</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
         <v>90</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -4207,25 +4228,25 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B58" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D58" t="s">
         <v>88</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F58" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G58" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4239,16 +4260,16 @@
         <v>3</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D59" t="s">
         <v>88</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F59" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -4262,13 +4283,13 @@
         <v>3</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D60" t="s">
         <v>90</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -4282,16 +4303,16 @@
         <v>2</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D61" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E61" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G61" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -4305,13 +4326,13 @@
         <v>3</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D62" t="s">
         <v>90</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -4325,13 +4346,13 @@
         <v>2</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D63" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E63" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -4345,16 +4366,16 @@
         <v>63</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D64" t="s">
         <v>88</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F64" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H64" t="s">
         <v>4</v>
@@ -4368,16 +4389,16 @@
         <v>65</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E65" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G65" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H65" t="s">
         <v>4</v>
@@ -4391,13 +4412,13 @@
         <v>3</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D66" t="s">
         <v>90</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -4411,16 +4432,16 @@
         <v>2</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D67" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E67" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="G67" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -4434,13 +4455,13 @@
         <v>18</v>
       </c>
       <c r="C68" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D68" t="s">
         <v>90</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G68" t="s">
         <v>69</v>
@@ -4457,16 +4478,16 @@
         <v>3</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D69" t="s">
         <v>90</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G69" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -4480,16 +4501,16 @@
         <v>3</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D70" t="s">
         <v>88</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F70" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="H70" t="s">
         <v>4</v>
@@ -4503,13 +4524,13 @@
         <v>3</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D71" t="s">
         <v>90</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -4523,16 +4544,16 @@
         <v>2</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D72" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E72" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G72" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4546,16 +4567,16 @@
         <v>2</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D73" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" t="s">
         <v>174</v>
       </c>
-      <c r="D73" t="s">
-        <v>168</v>
-      </c>
-      <c r="E73" t="s">
-        <v>178</v>
-      </c>
       <c r="G73" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H73" t="s">
         <v>4</v>
@@ -4569,13 +4590,13 @@
         <v>3</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D74" t="s">
         <v>90</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H74" t="s">
         <v>4</v>
@@ -4589,16 +4610,16 @@
         <v>3</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D75" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E75" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G75" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H75" t="s">
         <v>4</v>
@@ -4612,16 +4633,16 @@
         <v>3</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D76" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E76" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G76" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H76" t="s">
         <v>4</v>
@@ -4635,13 +4656,13 @@
         <v>3</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D77" t="s">
         <v>90</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -4655,16 +4676,16 @@
         <v>2</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D78" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E78" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="G78" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -4672,22 +4693,22 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D79" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E79" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G79" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H79" t="s">
         <v>4</v>
@@ -4695,22 +4716,22 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B80" t="s">
         <v>3</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D80" t="s">
         <v>90</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G80" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H80" t="s">
         <v>4</v>
@@ -4724,13 +4745,13 @@
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D81" t="s">
         <v>90</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G81" t="s">
         <v>81</v>
@@ -4741,226 +4762,226 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B82" t="s">
         <v>3</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D82" t="s">
         <v>88</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F82" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G82" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B83" t="s">
         <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D83" t="s">
         <v>88</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F83" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G83" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D84" t="s">
+        <v>152</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G84" t="s">
         <v>156</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G84" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="30">
       <c r="A85" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B85" t="s">
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D85" t="s">
         <v>88</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G85" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="30">
       <c r="A86" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B86" t="s">
         <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="30">
       <c r="A87" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B87" t="s">
         <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D87" t="s">
         <v>88</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="30">
       <c r="A88" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B88" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C88" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D88" t="s">
         <v>88</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F88" s="3"/>
       <c r="G88" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="30">
       <c r="A89" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B89" t="s">
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D89" t="s">
         <v>90</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G89" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="30">
       <c r="A90" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B90" t="s">
         <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D90" t="s">
         <v>90</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G90" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="45">
       <c r="A91" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
         <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D91" t="s">
         <v>90</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="30">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B92" t="s">
         <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D92" t="s">
         <v>90</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -4986,7 +5007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -4999,36 +5020,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5039,13 +5060,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5056,30 +5077,30 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5090,47 +5111,47 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5141,47 +5162,47 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E10" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E11" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5192,47 +5213,47 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D12" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E12" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B14" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E14" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -5243,13 +5264,13 @@
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -5260,13 +5281,13 @@
         <v>63</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E16" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5277,115 +5298,115 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E17" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E18" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E19" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D20" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D21" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D22" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C23" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D23" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -5418,30 +5439,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -5454,20 +5475,20 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -5511,22 +5532,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5537,13 +5558,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5554,33 +5575,33 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5591,13 +5612,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5608,7 +5629,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5619,13 +5640,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5636,10 +5657,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5650,13 +5671,13 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5667,7 +5688,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5678,13 +5699,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5695,7 +5716,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5706,7 +5727,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5717,7 +5738,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5728,7 +5749,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -5739,7 +5760,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5750,7 +5771,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5761,10 +5782,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D18" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5775,7 +5796,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5786,10 +5807,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5800,7 +5821,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5811,7 +5832,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5822,7 +5843,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5833,24 +5854,24 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5861,7 +5882,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -5872,10 +5893,10 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5886,7 +5907,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -5897,7 +5918,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5908,7 +5929,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5919,7 +5940,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -5930,7 +5951,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -5941,10 +5962,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D33" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -5955,10 +5976,10 @@
         <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D34" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -5969,7 +5990,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -5980,7 +6001,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -5991,7 +6012,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -6002,7 +6023,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -6013,10 +6034,10 @@
         <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -6027,7 +6048,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -6038,7 +6059,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -6049,13 +6070,13 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E42" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -6066,21 +6087,21 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D44" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6091,54 +6112,54 @@
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D45" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -6171,22 +6192,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6197,10 +6218,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6211,24 +6232,24 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6239,10 +6260,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6253,10 +6274,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6267,10 +6288,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6281,7 +6302,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6292,10 +6313,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6306,10 +6327,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6320,10 +6341,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D11" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6334,10 +6355,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D12" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -6348,7 +6369,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -6359,7 +6380,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -6370,10 +6391,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D15" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -6384,10 +6405,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6398,10 +6419,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6412,13 +6433,13 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D18" t="s">
         <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6429,7 +6450,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -6440,7 +6461,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D20" t="s">
         <v>35</v>
@@ -6454,10 +6475,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -6468,10 +6489,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -6482,7 +6503,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -6493,21 +6514,21 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D24" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -6518,10 +6539,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -6532,10 +6553,10 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D27" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -6546,10 +6567,10 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D28" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6560,7 +6581,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -6571,10 +6592,10 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6585,10 +6606,10 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6599,13 +6620,13 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D32" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E32" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -6616,10 +6637,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D33" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -6630,10 +6651,10 @@
         <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D34" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6644,10 +6665,10 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D35" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -6658,7 +6679,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D36" t="s">
         <v>83</v>
@@ -6672,10 +6693,10 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D37" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -6686,7 +6707,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D38" t="s">
         <v>84</v>
@@ -6700,10 +6721,10 @@
         <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D39" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -6714,10 +6735,10 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -6728,7 +6749,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D41" t="s">
         <v>85</v>
@@ -6742,10 +6763,10 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D42" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="90">
@@ -6756,27 +6777,27 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D43" t="s">
         <v>86</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D44" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6787,54 +6808,54 @@
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D45" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -6851,8 +6872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6864,22 +6885,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6890,7 +6911,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>171</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="E2" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6901,7 +6928,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>171</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="F3" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6912,7 +6945,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6923,7 +6956,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6934,7 +6967,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6945,7 +6978,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6956,7 +6989,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6967,7 +7000,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6978,7 +7011,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6989,7 +7022,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7000,7 +7033,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -7011,7 +7044,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -7022,7 +7055,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -7033,7 +7066,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -7044,7 +7077,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -7055,7 +7088,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -7066,10 +7099,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D18" t="s">
-        <v>94</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -7080,7 +7110,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -7091,10 +7121,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" t="s">
-        <v>95</v>
+        <v>170</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -7105,7 +7135,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -7116,7 +7146,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -7127,7 +7157,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -7138,7 +7168,7 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -7149,7 +7179,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -7160,7 +7190,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -7171,10 +7201,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D27" t="s">
-        <v>94</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -7185,7 +7212,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -7196,7 +7223,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -7207,7 +7234,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -7218,7 +7245,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -7229,7 +7256,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -7240,7 +7267,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -7251,7 +7278,10 @@
         <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -7262,7 +7292,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -7273,7 +7303,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -7284,7 +7314,10 @@
         <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -7295,7 +7328,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -7306,7 +7339,7 @@
         <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -7317,7 +7350,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -7328,7 +7361,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -7339,10 +7372,10 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D42" t="s">
-        <v>103</v>
+        <v>171</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -7353,7 +7386,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -7364,10 +7397,7 @@
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -7378,51 +7408,54 @@
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>174</v>
+        <v>170</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redmine 4180 - documenting 'attibute' fields from eml
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16780" yWindow="7820" windowWidth="32940" windowHeight="19800" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="383">
   <si>
     <t>Notes</t>
   </si>
@@ -1270,6 +1270,39 @@
   </si>
   <si>
     <t>http://dryad.googlecode.com/svn/trunk/dryad/dspace/modules/xmlui/src/main/webapp/themes/Dryad/meta/schema/v3/dryad.xsd</t>
+  </si>
+  <si>
+    <t>attributeName</t>
+  </si>
+  <si>
+    <t>//dataTable/attributeList/attribute/attributeName/text()</t>
+  </si>
+  <si>
+    <t>attributeLabel</t>
+  </si>
+  <si>
+    <t>//dataTable/attributeList/attribute/attributeLabel/text()</t>
+  </si>
+  <si>
+    <t>attributeDescription</t>
+  </si>
+  <si>
+    <t>//dataTable/attributeList/attribute/attributeDefinition/text()</t>
+  </si>
+  <si>
+    <t>attributeUnit</t>
+  </si>
+  <si>
+    <t>//dataTable//standardUnit/text() | //dataTable//customUnit/text()</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string </t>
+  </si>
+  <si>
+    <t>//dataTable/attributeList/attribute</t>
   </si>
 </sst>
 </file>
@@ -5511,13 +5544,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A45" sqref="A45"/>
+      <selection pane="bottomRight" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6151,7 +6184,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>122</v>
       </c>
@@ -6160,6 +6193,76 @@
       </c>
       <c r="C49" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>372</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>374</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>376</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>378</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>170</v>
+      </c>
+      <c r="D53" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>380</v>
+      </c>
+      <c r="B54" t="s">
+        <v>381</v>
+      </c>
+      <c r="C54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -6872,7 +6975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added geohash fields to SearchMetadata documentation.
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Dryad" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$H$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$H$101</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="394">
   <si>
     <t>Notes</t>
   </si>
@@ -1303,6 +1303,39 @@
   </si>
   <si>
     <t>//dataTable/attributeList/attribute</t>
+  </si>
+  <si>
+    <t>geohash_1</t>
+  </si>
+  <si>
+    <t>An encoded string that represents the geographic coordinates of the centroid of a spatial extent. This can be used for searching and plotting.</t>
+  </si>
+  <si>
+    <t>geohash_2</t>
+  </si>
+  <si>
+    <t>geohash_3</t>
+  </si>
+  <si>
+    <t>geohash_4</t>
+  </si>
+  <si>
+    <t>geohash_5</t>
+  </si>
+  <si>
+    <t>geohash_6</t>
+  </si>
+  <si>
+    <t>geohash_7</t>
+  </si>
+  <si>
+    <t>geohash_8</t>
+  </si>
+  <si>
+    <t>geohash_9</t>
+  </si>
+  <si>
+    <t>Encoded from centroid of northBoundCoord, sourthBoundCoord, eastBoundCoord, westBoundCoord</t>
   </si>
 </sst>
 </file>
@@ -2961,13 +2994,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A87" sqref="A87:XFD87"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3590,58 +3623,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="45">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>383</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>291</v>
+        <v>384</v>
       </c>
       <c r="F28" t="s">
-        <v>241</v>
-      </c>
-      <c r="G28" t="s">
-        <v>154</v>
-      </c>
-      <c r="H28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="45">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>385</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
-      </c>
-      <c r="E29" t="s">
-        <v>292</v>
-      </c>
-      <c r="G29" t="s">
-        <v>138</v>
-      </c>
-      <c r="H29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="30">
+        <v>90</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F29" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>386</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -3653,61 +3677,55 @@
         <v>90</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G30" t="s">
-        <v>124</v>
-      </c>
-      <c r="H30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>384</v>
+      </c>
+      <c r="F30" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>387</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" t="s">
-        <v>293</v>
-      </c>
-      <c r="H31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>90</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F31" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="45">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>388</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D32" t="s">
         <v>90</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="G32" t="s">
-        <v>158</v>
-      </c>
-      <c r="H32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="60">
+        <v>384</v>
+      </c>
+      <c r="F32" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="45">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>389</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -3719,38 +3737,35 @@
         <v>90</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="G33" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>384</v>
+      </c>
+      <c r="F33" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="45">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>390</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E34" t="s">
-        <v>295</v>
-      </c>
-      <c r="H34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>90</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F34" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="45">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>391</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
@@ -3762,38 +3777,35 @@
         <v>90</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G35" t="s">
-        <v>173</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="30">
+        <v>384</v>
+      </c>
+      <c r="F35" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="45">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>392</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D36" t="s">
         <v>90</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="30">
+        <v>384</v>
+      </c>
+      <c r="F36" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
@@ -3802,85 +3814,82 @@
         <v>171</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>228</v>
+        <v>291</v>
+      </c>
+      <c r="F37" t="s">
+        <v>241</v>
       </c>
       <c r="G37" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>218</v>
+        <v>164</v>
+      </c>
+      <c r="E38" t="s">
+        <v>292</v>
       </c>
       <c r="G38" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="H38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="30">
       <c r="A39" t="s">
-        <v>355</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="F39" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="G39" t="s">
-        <v>139</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="30">
+        <v>124</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>356</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F40" t="s">
-        <v>244</v>
+        <v>164</v>
+      </c>
+      <c r="E40" t="s">
+        <v>293</v>
       </c>
       <c r="H40" t="s">
         <v>4</v>
@@ -3888,7 +3897,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
@@ -3897,64 +3906,64 @@
         <v>171</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="F41" t="s">
-        <v>247</v>
+        <v>226</v>
+      </c>
+      <c r="G41" t="s">
+        <v>158</v>
       </c>
       <c r="H41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="60">
       <c r="A42" t="s">
-        <v>349</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D42" t="s">
         <v>90</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
+        <v>227</v>
+      </c>
+      <c r="G42" t="s">
+        <v>89</v>
+      </c>
+      <c r="H42" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D43" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G43" t="s">
-        <v>173</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
+        <v>164</v>
+      </c>
+      <c r="E43" t="s">
+        <v>295</v>
+      </c>
+      <c r="H43" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -3966,188 +3975,191 @@
         <v>90</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>272</v>
+        <v>211</v>
       </c>
       <c r="G44" t="s">
-        <v>125</v>
-      </c>
-      <c r="H44" t="s">
-        <v>4</v>
+        <v>173</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="30">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D45" t="s">
         <v>90</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" ht="30">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D46" t="s">
-        <v>164</v>
-      </c>
-      <c r="E46" t="s">
-        <v>296</v>
+        <v>90</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="G46" t="s">
-        <v>141</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>158</v>
+      </c>
+      <c r="H46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>170</v>
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>164</v>
-      </c>
-      <c r="E47" t="s">
-        <v>297</v>
+        <v>90</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="G47" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="H47" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="27">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>355</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>274</v>
+        <v>88</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F48" t="s">
+        <v>242</v>
+      </c>
+      <c r="G48" t="s">
+        <v>139</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" ht="30">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>356</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D49" t="s">
-        <v>164</v>
-      </c>
-      <c r="E49" t="s">
-        <v>298</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
+        <v>88</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F49" t="s">
+        <v>244</v>
+      </c>
+      <c r="H49" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G50" t="s">
-        <v>173</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="30">
+        <v>246</v>
+      </c>
+      <c r="F50" t="s">
+        <v>247</v>
+      </c>
+      <c r="H50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>349</v>
       </c>
       <c r="B51" t="s">
         <v>2</v>
       </c>
-      <c r="C51" t="s">
-        <v>170</v>
+      <c r="C51" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D51" t="s">
         <v>90</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="G51" t="s">
-        <v>87</v>
-      </c>
-      <c r="H51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="30">
+        <v>229</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>357</v>
+        <v>43</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D52" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="F52" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="G52" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -4155,105 +4167,108 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D53" t="s">
         <v>90</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="53">
+        <v>272</v>
+      </c>
+      <c r="G53" t="s">
+        <v>125</v>
+      </c>
+      <c r="H53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="30">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D54" t="s">
         <v>90</v>
       </c>
-      <c r="E54" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G54" t="s">
-        <v>126</v>
-      </c>
-      <c r="H54" t="s">
-        <v>4</v>
+      <c r="E54" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B55" t="s">
         <v>2</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D55" t="s">
         <v>164</v>
       </c>
       <c r="E55" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G55" t="s">
-        <v>144</v>
-      </c>
-      <c r="H55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="30">
+        <v>141</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D56" t="s">
-        <v>90</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>288</v>
+        <v>164</v>
+      </c>
+      <c r="E56" t="s">
+        <v>297</v>
+      </c>
+      <c r="G56" t="s">
+        <v>140</v>
       </c>
       <c r="H56" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="30">
+    <row r="57" spans="1:8" ht="27">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D57" t="s">
         <v>90</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>278</v>
+      <c r="E57" s="5" t="s">
+        <v>274</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -4261,25 +4276,19 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>358</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>172</v>
+        <v>2</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D58" t="s">
-        <v>88</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="F58" t="s">
-        <v>251</v>
-      </c>
-      <c r="G58" t="s">
-        <v>145</v>
+        <v>164</v>
+      </c>
+      <c r="E58" t="s">
+        <v>298</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4287,22 +4296,22 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D59" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="F59" t="s">
-        <v>168</v>
+        <v>213</v>
+      </c>
+      <c r="G59" t="s">
+        <v>173</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -4310,148 +4319,154 @@
     </row>
     <row r="60" spans="1:8" ht="30">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
         <v>170</v>
       </c>
       <c r="D60" t="s">
         <v>90</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>275</v>
+      </c>
+      <c r="G60" t="s">
+        <v>87</v>
+      </c>
+      <c r="H60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="30">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>357</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
-      </c>
-      <c r="C61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
         <v>170</v>
       </c>
       <c r="D61" t="s">
-        <v>164</v>
-      </c>
-      <c r="E61" t="s">
-        <v>300</v>
+        <v>88</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F61" t="s">
+        <v>248</v>
       </c>
       <c r="G61" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="27">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D62" t="s">
         <v>90</v>
       </c>
-      <c r="E62" s="5" t="s">
-        <v>280</v>
+      <c r="E62" s="3" t="s">
+        <v>276</v>
       </c>
       <c r="H62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" ht="53">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B63" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D63" t="s">
-        <v>164</v>
-      </c>
-      <c r="E63" t="s">
-        <v>301</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="G63" t="s">
+        <v>126</v>
+      </c>
+      <c r="H63" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>88</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F64" t="s">
-        <v>253</v>
+        <v>164</v>
+      </c>
+      <c r="E64" t="s">
+        <v>299</v>
+      </c>
+      <c r="G64" t="s">
+        <v>144</v>
       </c>
       <c r="H64" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" ht="30">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>164</v>
-      </c>
-      <c r="E65" t="s">
-        <v>292</v>
-      </c>
-      <c r="G65" t="s">
-        <v>134</v>
+        <v>90</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="H65" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="27">
+    <row r="66" spans="1:8" ht="30">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D66" t="s">
         <v>90</v>
       </c>
-      <c r="E66" s="5" t="s">
-        <v>281</v>
+      <c r="E66" s="3" t="s">
+        <v>278</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -4459,53 +4474,56 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>358</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>172</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>164</v>
-      </c>
-      <c r="E67" t="s">
-        <v>302</v>
+        <v>88</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F67" t="s">
+        <v>251</v>
       </c>
       <c r="G67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
-      </c>
-      <c r="C68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D68" t="s">
-        <v>90</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="G68" t="s">
-        <v>69</v>
-      </c>
-      <c r="H68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F68" t="s">
+        <v>168</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="30">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
@@ -4517,41 +4535,38 @@
         <v>90</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="G69" t="s">
-        <v>173</v>
+        <v>279</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D70" t="s">
-        <v>88</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F70" t="s">
-        <v>256</v>
-      </c>
-      <c r="H70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="66">
+        <v>164</v>
+      </c>
+      <c r="E70" t="s">
+        <v>300</v>
+      </c>
+      <c r="G70" t="s">
+        <v>146</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="27">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B71" t="s">
         <v>3</v>
@@ -4563,7 +4578,7 @@
         <v>90</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -4571,7 +4586,7 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B72" t="s">
         <v>2</v>
@@ -4583,10 +4598,7 @@
         <v>164</v>
       </c>
       <c r="E72" t="s">
-        <v>303</v>
-      </c>
-      <c r="G72" t="s">
-        <v>148</v>
+        <v>301</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4594,22 +4606,22 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D73" t="s">
-        <v>164</v>
-      </c>
-      <c r="E73" t="s">
-        <v>174</v>
-      </c>
-      <c r="G73" t="s">
-        <v>149</v>
+        <v>88</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F73" t="s">
+        <v>253</v>
       </c>
       <c r="H73" t="s">
         <v>4</v>
@@ -4617,139 +4629,142 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B74" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D74" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>230</v>
+        <v>164</v>
+      </c>
+      <c r="E74" t="s">
+        <v>292</v>
+      </c>
+      <c r="G74" t="s">
+        <v>134</v>
       </c>
       <c r="H74" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" ht="27">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B75" t="s">
         <v>3</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D75" t="s">
-        <v>164</v>
-      </c>
-      <c r="E75" t="s">
-        <v>304</v>
-      </c>
-      <c r="G75" t="s">
-        <v>150</v>
-      </c>
-      <c r="H75" t="s">
-        <v>4</v>
+        <v>90</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D76" t="s">
         <v>164</v>
       </c>
       <c r="E76" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G76" t="s">
-        <v>150</v>
-      </c>
-      <c r="H76" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="40">
+        <v>147</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="30">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>170</v>
+        <v>18</v>
+      </c>
+      <c r="C77" t="s">
+        <v>171</v>
       </c>
       <c r="D77" t="s">
         <v>90</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
+      <c r="E77" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G77" t="s">
+        <v>69</v>
+      </c>
+      <c r="H77" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B78" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D78" t="s">
-        <v>164</v>
-      </c>
-      <c r="E78" t="s">
-        <v>305</v>
+        <v>90</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="G78" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="H78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" ht="30">
       <c r="A79" t="s">
-        <v>359</v>
+        <v>71</v>
       </c>
       <c r="B79" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D79" t="s">
-        <v>164</v>
-      </c>
-      <c r="E79" t="s">
-        <v>306</v>
-      </c>
-      <c r="G79" t="s">
-        <v>153</v>
+        <v>88</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F79" t="s">
+        <v>256</v>
       </c>
       <c r="H79" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" ht="66">
       <c r="A80" t="s">
-        <v>350</v>
+        <v>72</v>
       </c>
       <c r="B80" t="s">
         <v>3</v>
@@ -4760,265 +4775,463 @@
       <c r="D80" t="s">
         <v>90</v>
       </c>
-      <c r="E80" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="G80" t="s">
-        <v>159</v>
-      </c>
-      <c r="H80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="30">
+      <c r="E80" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
-      </c>
-      <c r="C81" t="s">
-        <v>171</v>
+        <v>2</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="D81" t="s">
-        <v>90</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>220</v>
+        <v>164</v>
+      </c>
+      <c r="E81" t="s">
+        <v>303</v>
       </c>
       <c r="G81" t="s">
-        <v>81</v>
-      </c>
-      <c r="H81" t="s">
-        <v>4</v>
+        <v>148</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>360</v>
+        <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D82" t="s">
-        <v>88</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="F82" t="s">
-        <v>257</v>
+        <v>164</v>
+      </c>
+      <c r="E82" t="s">
+        <v>174</v>
       </c>
       <c r="G82" t="s">
-        <v>132</v>
+        <v>149</v>
+      </c>
+      <c r="H82" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>361</v>
+        <v>74</v>
       </c>
       <c r="B83" t="s">
         <v>3</v>
       </c>
-      <c r="C83" t="s">
-        <v>170</v>
+      <c r="C83" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D83" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="F83" t="s">
-        <v>259</v>
-      </c>
-      <c r="G83" t="s">
-        <v>131</v>
+        <v>230</v>
+      </c>
+      <c r="H83" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>362</v>
+        <v>75</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
       </c>
-      <c r="C84" t="s">
-        <v>170</v>
+      <c r="C84" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D84" t="s">
-        <v>152</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
+      </c>
+      <c r="E84" t="s">
+        <v>304</v>
       </c>
       <c r="G84" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="30">
+        <v>150</v>
+      </c>
+      <c r="H84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="B85" t="s">
         <v>3</v>
       </c>
-      <c r="C85" t="s">
-        <v>170</v>
+      <c r="C85" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D85" t="s">
-        <v>88</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>262</v>
+        <v>164</v>
+      </c>
+      <c r="E85" t="s">
+        <v>304</v>
       </c>
       <c r="G85" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="30">
+        <v>150</v>
+      </c>
+      <c r="H85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="40">
       <c r="A86" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="B86" t="s">
         <v>3</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D86" t="s">
-        <v>88</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="30">
+        <v>90</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D87" t="s">
-        <v>88</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="30">
+        <v>164</v>
+      </c>
+      <c r="E87" t="s">
+        <v>305</v>
+      </c>
+      <c r="G87" t="s">
+        <v>151</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>119</v>
+        <v>359</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
-      </c>
-      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D88" t="s">
-        <v>88</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F88" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="E88" t="s">
+        <v>306</v>
+      </c>
       <c r="G88" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="30">
+        <v>153</v>
+      </c>
+      <c r="H88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>120</v>
+        <v>350</v>
       </c>
       <c r="B89" t="s">
         <v>3</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D89" t="s">
         <v>90</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="G89" t="s">
-        <v>129</v>
+        <v>159</v>
+      </c>
+      <c r="H89" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="30">
       <c r="A90" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D90" t="s">
         <v>90</v>
       </c>
       <c r="E90" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G90" t="s">
+        <v>81</v>
+      </c>
+      <c r="H90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>360</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D91" t="s">
+        <v>88</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F91" t="s">
+        <v>257</v>
+      </c>
+      <c r="G91" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>361</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" t="s">
+        <v>170</v>
+      </c>
+      <c r="D92" t="s">
+        <v>88</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F92" t="s">
+        <v>259</v>
+      </c>
+      <c r="G92" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>362</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" t="s">
+        <v>170</v>
+      </c>
+      <c r="D93" t="s">
+        <v>152</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G93" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="30">
+      <c r="A94" t="s">
+        <v>116</v>
+      </c>
+      <c r="B94" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" t="s">
+        <v>170</v>
+      </c>
+      <c r="D94" t="s">
+        <v>88</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G94" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="30">
+      <c r="A95" t="s">
+        <v>117</v>
+      </c>
+      <c r="B95" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" t="s">
+        <v>170</v>
+      </c>
+      <c r="D95" t="s">
+        <v>88</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="30">
+      <c r="A96" t="s">
+        <v>118</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" t="s">
+        <v>170</v>
+      </c>
+      <c r="D96" t="s">
+        <v>88</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="30">
+      <c r="A97" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" t="s">
+        <v>172</v>
+      </c>
+      <c r="C97" t="s">
+        <v>171</v>
+      </c>
+      <c r="D97" t="s">
+        <v>88</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F97" s="3"/>
+      <c r="G97" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="30">
+      <c r="A98" t="s">
+        <v>120</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" t="s">
+        <v>170</v>
+      </c>
+      <c r="D98" t="s">
+        <v>90</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G98" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="30">
+      <c r="A99" t="s">
+        <v>121</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" t="s">
+        <v>170</v>
+      </c>
+      <c r="D99" t="s">
+        <v>90</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G99" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="45">
-      <c r="A91" t="s">
+    <row r="100" spans="1:7" ht="45">
+      <c r="A100" t="s">
         <v>123</v>
       </c>
-      <c r="B91" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91" t="s">
-        <v>170</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>170</v>
+      </c>
+      <c r="D100" t="s">
         <v>90</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="30">
-      <c r="A92" t="s">
+    <row r="101" spans="1:7" ht="30">
+      <c r="A101" t="s">
         <v>122</v>
       </c>
-      <c r="B92" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92" t="s">
-        <v>170</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="B101" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" t="s">
+        <v>170</v>
+      </c>
+      <c r="D101" t="s">
         <v>90</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="E101" s="4" t="s">
         <v>215</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A93">
+  <conditionalFormatting sqref="A2:A102">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>IF($D2="Y",1,0)</formula>
     </cfRule>
@@ -5546,8 +5759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A55" sqref="A55"/>
@@ -6267,6 +6480,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add details of schema.org 'Dataset' indexing
Issue #14
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="EML" sheetId="3" r:id="rId4"/>
     <sheet name="FGDC" sheetId="4" r:id="rId5"/>
     <sheet name="Dryad" sheetId="5" r:id="rId6"/>
+    <sheet name="schema_org" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$H$101</definedName>
@@ -150,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="429">
   <si>
     <t>Notes</t>
   </si>
@@ -1337,12 +1338,285 @@
   <si>
     <t>Encoded from centroid of northBoundCoord, sourthBoundCoord, eastBoundCoord, westBoundCoord</t>
   </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#common-properties</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#roles-of-people</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#temporal-coverage</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#spatial-coverage</t>
+  </si>
+  <si>
+    <t>serviceEndpoint</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>authorGivenName</t>
+  </si>
+  <si>
+    <t>hasPart</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#advanced-publishing-techniques</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#funding</t>
+  </si>
+  <si>
+    <t>SELECT ( ?name as ?title )
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        ?datasetId SO:name ?name .
+        FILTER NOT EXISTS { ?id SO:hasPart ?datasetId . }
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT ?label
+    WHERE {
+      ?datasetId rdf:type SO:Dataset .
+      ?datasetId SO:alternateName ?label .
+      FILTER NOT EXISTS { ?id SO:hasPart ?datasetId . }
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT (?name as ?author)
+    WHERE {
+        ?dsId rdf:type SO:Dataset .
+        ?dsId SO:creator ?list .
+        ?list list:index (?pos ?member) .
+        ?member SO:name ?name .
+    }
+    order by (?pos)
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT (?identifier as ?funderIdentifier)
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        ?datasetId SO:funder ?funderId .
+        ?funderId SO:identifier ?identifier.
+    }</t>
+  </si>
+  <si>
+    <t>SELECT (?name as ?funderName)
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        ?datasetId SO:funder ?funderId .
+        ?funderId SO:name ?name .
+    }</t>
+  </si>
+  <si>
+    <t>SELECT (?name as ?origin)
+    WHERE {
+        ?dsId rdf:type SO:Dataset .
+        ?dsId SO:creator ?list .
+        ?list list:index (?pos ?member) .
+        ?member SO:name ?name .
+    }
+    order by (?pos)</t>
+  </si>
+  <si>
+    <t>SELECT ?hasPart
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        {
+        ?datasetId SO:hasPart ?node .
+        ?node      rdf:type   SO:Dataset .
+        ?node      SO:name    ?hasPart .
+        }
+        UNION
+        {
+        ?datasetId SO:hasPart ?hasPart .
+        FILTER NOT EXISTS { ?hasPart rdf:type SO:Dataset . }
+        }
+    }</t>
+  </si>
+  <si>
+    <t>PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX list: &lt;http://jena.hpl.hp.com/ARQ/list#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX SO:   &lt;https://schema.org/&gt;
+SELECT ( ?description as ?abstract )
+    WHERE {
+        ?datasetId rdf:type       SO:Dataset .
+        ?datasetId SO:description ?description   .
+        FILTER NOT EXISTS { ?id SO:hasPart ?datasetId . }
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT ?keywords
+    WHERE {
+        ?datasetId rdf:type    SO:Dataset .
+        ?datasetId SO:keywords ?keywords .
+    }</t>
+  </si>
+  <si>
+    <t>SELECT ?southBoundCoord
+    WHERE {
+        ?datasetId rdf:type           SO:Dataset .
+        ?datasetId SO:spatialCoverage ?spatial .
+        ?spatial   rdf:type           SO:Place .
+        ?spatial   SO:geo             ?geo .
+        ?geo       rdf:type           SO:GeoShape .
+        ?geo       SO:box             ?box .
+        bind(strbefore(replace(str(?box), "\\s*,\\s*|\\s{2,}", " "), " ") as ?southBoundCoord)
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT ?westBoundCoord
+    WHERE {
+        ?datasetId rdf:type           SO:Dataset .
+        ?datasetId SO:spatialCoverage ?spatial .
+        ?spatial   rdf:type           SO:Place .
+        ?spatial   SO:geo             ?geo .
+        ?geo       rdf:type           SO:GeoShape .
+        ?geo       SO:box             ?box .
+        bind(strbefore(replace(str(?box), "\\s*,\\s*|\\s{2,}", " "), " ") as ?southBoundCoord)
+        bind(strafter(replace(str(?box), "\\s*,\\s*|\\s{2,}", " "), " ") as ?rest)
+        bind(strbefore(str(?rest), " ") as ?westBoundCoord)
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT ?northBoundCoord
+    WHERE {
+        ?datasetId rdf:type           SO:Dataset .
+        ?datasetId SO:spatialCoverage ?spatial .
+        ?spatial   rdf:type           SO:Place .
+        ?spatial   SO:geo             ?geo .
+        ?geo       rdf:type           SO:GeoShape .
+        ?geo       SO:box             ?box .
+        bind(strbefore(replace(str(?box), "\\s*,\\s*|\\s{2,}", " "), " ") as ?southBoundCoord)
+        bind(strafter(replace(str(?box), "\\s*,\\s*|\\s{2,}", " "), " ") as ?rest)
+        bind(strbefore(str(?rest), " ") as ?westBoundCoord)
+        bind(strafter(str(?rest), " ") as ?rest2)
+        bind(strbefore(str(?rest2), " ") as ?northBoundCoord)
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT ?eastBoundCoord
+    WHERE {
+        ?datasetId rdf:type           SO:Dataset .
+        ?datasetId SO:spatialCoverage ?spatial .
+        ?spatial   rdf:type           SO:Place .
+        ?spatial   SO:geo             ?geo .
+        ?geo       rdf:type           SO:GeoShape .
+        ?geo       SO:box             ?box .
+        bind(strbefore(replace(str(?box), "\\s*,\\s*|\\s{2,}", " "), " ") as ?southBoundCoord)
+        bind(strafter(replace(str(?box), "\\s*,\\s*|\\s{2,}", " "), " ") as ?rest)
+        bind(strbefore(str(?rest), " ") as ?westBoundCoord)
+        bind(strafter(str(?rest), " ") as ?rest2)
+        bind(strbefore(str(?rest2), " ") as ?northBoundCoord)
+        bind(strafter(str(?rest2), " ") as ?eastBoundCoord)
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT ?namedLocation
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        ?datasetId SO:spatialCoverage ?namedLocation .
+        FILTER NOT EXISTS { ?namedLocation rdf:type SO:Place . }
+    }</t>
+  </si>
+  <si>
+    <t>SELECT (if(contains(?dates, "/"), strafter(?dates, "/"), "") as ?endDate)
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        ?datasetId SO:temporalCoverage ?dates .
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT (?variableMeasured as ?parameter)
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        {
+            ?datasetId SO:variableMeasured ?variable .
+            ?variable  rdf:type            SO:PropertyValue .
+            ?variable  SO:name             ?variableMeasured .
+        }
+        UNION
+        {
+            ?datasetId SO:variableMeasured ?variableMeasured .
+            FILTER NOT EXISTS { ?parameter rdf:type SO:PropertyValue . }
+        }
+    }</t>
+  </si>
+  <si>
+    <t>SELECT ( str(?version) as ?edition )
+    WHERE {
+        ?datasetId rdf:type schema:Dataset .
+        ?datasetId schema:version ?version .
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT ( str(?url) as ?serviceEndpoint )
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        ?datasetId SO:url ?url .
+        FILTER NOT EXISTS { ?id SO:hasPart ?datasetId . }
+    }</t>
+  </si>
+  <si>
+    <t>funderIdentifier</t>
+  </si>
+  <si>
+    <t>funderName</t>
+  </si>
+  <si>
+    <t>tfloat</t>
+  </si>
+  <si>
+    <t>SELECT (?givenName as ?authorGivenName)
+    WHERE {
+        ?dsId rdf:type SO:Dataset .
+        ?dsId SO:creator ?list .
+        ?list list:index (?pos ?member) .
+        ?member SO:givenName ?givenName .
+    }
+    order by (?pos)
+    limit 1</t>
+  </si>
+  <si>
+    <t>SELECT (?familyName as ?authorLastName)
+    WHERE {
+        ?dsId rdf:type SO:Dataset .
+        ?dsId SO:creator ?list .
+        ?list list:index (?pos ?member) .
+        ?member SO:familyName ?familyName .
+    }
+    order by (?pos)</t>
+  </si>
+  <si>
+    <t>SELECT (if(contains(?dates, "/"), strbefore(?dates, "/"), ?dates) as ?beginDate)
+    WHERE {
+        ?datasetId rdf:type SO:Dataset .
+        ?datasetId SO:temporalCoverage ?dates .
+    }
+    limit 1</t>
+  </si>
+  <si>
+    <t>SPARQL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1405,6 +1679,12 @@
       <color rgb="FF000000"/>
       <name val="Courier"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1423,7 +1703,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="592">
+  <cellStyleXfs count="614">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2016,8 +2296,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2031,8 +2333,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="592">
+  <cellStyles count="614">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2336,6 +2660,17 @@
     <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2624,6 +2959,17 @@
     <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -2996,8 +3342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
@@ -5671,7 +6017,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5760,10 +6106,10 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A55" sqref="A55"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6493,8 +6839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A33" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7189,7 +7535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -7783,4 +8129,844 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="114.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.83203125" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="A1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="180">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="135">
+      <c r="A3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="135">
+      <c r="A4" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="120">
+      <c r="A5" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90">
+      <c r="A6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="240">
+      <c r="A7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="90">
+      <c r="A8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90">
+      <c r="A9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="90">
+      <c r="A10" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="90">
+      <c r="A11" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="210">
+      <c r="A12" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="75">
+      <c r="A13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="105">
+      <c r="A14" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90">
+      <c r="A15" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="225">
+      <c r="A16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="120">
+      <c r="A17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="210">
+      <c r="A18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90">
+      <c r="A19" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="165">
+      <c r="A20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="105">
+      <c r="A21" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="195">
+      <c r="A22" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>349</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>350</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added add'l Solr fields for schema.org
Issue #14

Added Solr fields `awardNumber`, `awardTitle`, `investigator`, `pubDate` to `SearchFields.xslx` for schema.org tab ("Search Metadata Elements Extracted from schema.org:Dataset")
</commit_message>
<xml_diff>
--- a/source/design/data/SearchFields.xlsx
+++ b/source/design/data/SearchFields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="4180" yWindow="2960" windowWidth="25920" windowHeight="14900" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="439">
   <si>
     <t>Notes</t>
   </si>
@@ -1610,6 +1610,80 @@
   </si>
   <si>
     <t>SPARQL</t>
+  </si>
+  <si>
+    <t>awardNumber</t>
+  </si>
+  <si>
+    <t>awardTitle</t>
+  </si>
+  <si>
+    <t>SELECT
+    ( str(?datePublished) as ?pubDate)
+WHERE {
+    ?datasetId rdf:type SO:Dataset .
+    ?datasetId SO:datePublished ?datePublished
+    # Don't include referenced sub-Datasets (i.e. a Dataset in a 'hasPart' property)
+    FILTER NOT EXISTS { ?id SO:hasPart ?datasetId . }
+}</t>
+  </si>
+  <si>
+    <t>https://schema.org/datePublished</t>
+  </si>
+  <si>
+    <t>SELECT
+    ( str(?identifier) as ?awardNumber)
+WHERE {
+    ?datasetId rdf:type SO:Dataset .
+    {
+        ?awardId rdf:type SO:MonetaryGrant .
+        ?awardId SO:fundedItem ?datasetId .
+        ?awardId SO:identifier ?identifier .
+    }
+    UNION
+    {
+        ?datasetId SO:about ?awardId .
+        ?awardId rdf:type SO:MonetaryGrant .
+        ?awardId SO:sameAs ?identifier .
+    }
+}</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/1.2.0/guides/Dataset.md#funding</t>
+  </si>
+  <si>
+    <t>SELECT
+    ( str(?name) as ?awardTitle)
+WHERE {
+    ?datasetId rdf:type SO:Dataset .
+    {
+        ?awardId rdf:type SO:MonetaryGrant .
+        ?awardId SO:fundedItem ?datasetId .
+        ?awardId SO:name ?name .
+    }
+    UNION
+    {
+        ?datasetId SO:about ?awardId .
+        ?awardId rdf:type SO:MonetaryGrant .
+        ?awardId SO:name ?name .
+    }
+}</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>SELECT (?familyName as ?investigator)
+WHERE {
+    ?dsId rdf:type SO:Dataset .
+    ?dsId SO:creator ?list .
+    ?list list:index (?pos ?member) .
+    ?member SO:familyName ?familyName .
+}
+order by (?pos)</t>
+  </si>
+  <si>
+    <t>https://schema.org/alternateName</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +1777,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="614">
+  <cellStyleXfs count="616">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2113,6 +2187,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2356,7 +2432,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="614">
+  <cellStyles count="616">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2671,6 +2747,7 @@
     <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2970,6 +3047,7 @@
     <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -8133,10 +8211,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8238,354 +8316,369 @@
         <v>395</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="90">
+    <row r="6" spans="1:6" ht="240">
       <c r="A6" s="12" t="s">
-        <v>7</v>
+        <v>429</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>396</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="240">
       <c r="A7" s="12" t="s">
-        <v>17</v>
+        <v>430</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>424</v>
+        <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>416</v>
+        <v>435</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>397</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90">
       <c r="A8" s="12" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>171</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="90">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="240">
       <c r="A9" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>8</v>
+        <v>424</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>171</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90">
       <c r="A10" s="12" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="90">
       <c r="A11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90">
+      <c r="A12" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90">
+      <c r="A13" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="B13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="210">
-      <c r="A12" s="12" t="s">
+    <row r="14" spans="1:6" ht="210">
+      <c r="A14" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="B14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E14" s="12" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="75">
-      <c r="A13" s="12" t="s">
+    <row r="15" spans="1:6" ht="120">
+      <c r="A15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="75">
+      <c r="A16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B16" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="105">
-      <c r="A14" s="12" t="s">
+    <row r="17" spans="1:6" ht="105">
+      <c r="A17" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="B17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="90">
-      <c r="A15" s="12" t="s">
+      <c r="E17" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="90">
+      <c r="A18" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="B18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E18" s="12" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="225">
-      <c r="A16" s="12" t="s">
+    <row r="19" spans="1:6" ht="225">
+      <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B19" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="C19" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="120">
-      <c r="A17" s="12" t="s">
+    <row r="20" spans="1:6" ht="120">
+      <c r="A20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="B20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="210">
-      <c r="A18" s="12" t="s">
+    <row r="21" spans="1:6" ht="210">
+      <c r="A21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="B21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>419</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="90">
-      <c r="A19" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="165">
-      <c r="A20" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>413</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="105">
-      <c r="A21" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>404</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="195">
+    <row r="22" spans="1:6" ht="120">
       <c r="A22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="90">
+      <c r="A23" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="165">
+      <c r="A24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="105">
+      <c r="A25" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="195">
+      <c r="A26" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B26" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="C26" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E26" s="12" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>381</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>170</v>
@@ -8595,256 +8688,268 @@
       <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>170</v>
-      </c>
-      <c r="D28" s="11"/>
+      <c r="A28" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>171</v>
-      </c>
-      <c r="D29" s="11"/>
+      <c r="A29" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="A30" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D30" s="11"/>
+        <v>170</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3</v>
+      <c r="A31" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>381</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>170</v>
       </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="C37" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>26</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B38" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="C38" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>27</v>
       </c>
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>28</v>
       </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>33</v>
       </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
         <v>349</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+      <c r="C45" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
         <v>50</v>
       </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>53</v>
-      </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>171</v>
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>171</v>
@@ -8852,29 +8957,29 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
@@ -8885,7 +8990,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
@@ -8896,7 +9001,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
@@ -8907,7 +9012,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
@@ -8918,7 +9023,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>350</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
@@ -8929,34 +9034,56 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>350</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
         <v>120</v>
       </c>
-      <c r="B58" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="2" t="s">
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="2" t="s">
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>